<commit_message>
Teamreport updated with project backlog
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\Documents\GitHub\gedcom-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95AA235C-B92F-4ABF-81DE-F6707E25487E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DA4766-E1A1-423F-A895-1A84DAB63048}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8280" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8280" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="196">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -656,6 +656,9 @@
   </si>
   <si>
     <t>Birth Before Death</t>
+  </si>
+  <si>
+    <t>KS</t>
   </si>
 </sst>
 </file>
@@ -1839,7 +1842,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -1903,7 +1906,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
       <c r="A5" s="16" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>183</v>
@@ -1963,17 +1966,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.1875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.76171875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1996,15 +1999,313 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="C2" s="1"/>
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="C3" s="1"/>
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B16" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B20" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B21" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B23" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B24" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B25" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B26" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>138</v>
+      </c>
+      <c r="C27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B28" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B29" t="s">
+        <v>140</v>
+      </c>
+      <c r="C29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B30" t="s">
+        <v>141</v>
+      </c>
+      <c r="C30" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B31" t="s">
+        <v>142</v>
+      </c>
+      <c r="C31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B32" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B33" t="s">
+        <v>148</v>
+      </c>
+      <c r="C33" t="s">
+        <v>103</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2251,8 +2552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -2395,7 +2696,7 @@
         <v>69</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="20">
@@ -2413,7 +2714,7 @@
         <v>70</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="20">
@@ -2627,8 +2928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A36" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
cleaned up Sprint 1 tab
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10909"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\Documents\GitHub\gedcom-parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rozanitis/Documents/Stevens/Semesters/Fall2018/SSW-555/gedcom-parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A478E38-66F3-4394-B6FD-6FDAE51370FE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675F1F6C-10FC-7248-9F89-040BF250856C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8280" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19880" windowHeight="15240" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -28,11 +28,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -41,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="200">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -659,6 +654,18 @@
   </si>
   <si>
     <t>KS</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Assigned</t>
+  </si>
+  <si>
+    <t>in Progress</t>
   </si>
 </sst>
 </file>
@@ -805,7 +812,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -817,13 +824,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -838,11 +841,23 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="66">
@@ -913,7 +928,88 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -953,7 +1049,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1024,7 +1120,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1845,15 +1941,15 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.80859375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.47265625" customWidth="1"/>
-    <col min="3" max="3" width="8.47265625" customWidth="1"/>
-    <col min="4" max="5" width="20.47265625" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -1870,83 +1966,83 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="14" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="14" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="16" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
-      <c r="A6" s="16" t="s">
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="14" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="D9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
   </sheetData>
   <sortState ref="A3:D5">
@@ -1972,16 +2068,15 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.76171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -1998,7 +2093,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2008,11 +2103,11 @@
       <c r="C2" t="s">
         <v>153</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="17" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2022,11 +2117,11 @@
       <c r="C3" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="17" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2036,11 +2131,11 @@
       <c r="C4" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="17" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2050,11 +2145,11 @@
       <c r="C5" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="17" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2064,11 +2159,11 @@
       <c r="C6" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="17" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2078,11 +2173,11 @@
       <c r="C7" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="17" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2092,11 +2187,11 @@
       <c r="C8" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="17" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
         <v>118</v>
       </c>
@@ -2104,7 +2199,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>119</v>
       </c>
@@ -2112,7 +2207,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
         <v>120</v>
       </c>
@@ -2120,7 +2215,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>121</v>
       </c>
@@ -2128,7 +2223,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
         <v>122</v>
       </c>
@@ -2136,7 +2231,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>124</v>
       </c>
@@ -2144,7 +2239,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
         <v>125</v>
       </c>
@@ -2152,7 +2247,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>126</v>
       </c>
@@ -2160,7 +2255,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
         <v>127</v>
       </c>
@@ -2168,7 +2263,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>128</v>
       </c>
@@ -2176,7 +2271,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
         <v>129</v>
       </c>
@@ -2184,7 +2279,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>130</v>
       </c>
@@ -2192,7 +2287,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
         <v>131</v>
       </c>
@@ -2200,7 +2295,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B22" t="s">
         <v>132</v>
       </c>
@@ -2208,7 +2303,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B23" t="s">
         <v>133</v>
       </c>
@@ -2216,7 +2311,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B24" t="s">
         <v>134</v>
       </c>
@@ -2224,7 +2319,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B25" t="s">
         <v>135</v>
       </c>
@@ -2232,7 +2327,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B26" t="s">
         <v>137</v>
       </c>
@@ -2240,7 +2335,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>1</v>
       </c>
@@ -2254,7 +2349,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
         <v>139</v>
       </c>
@@ -2262,7 +2357,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B29" t="s">
         <v>140</v>
       </c>
@@ -2270,7 +2365,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B30" t="s">
         <v>141</v>
       </c>
@@ -2278,7 +2373,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B31" t="s">
         <v>142</v>
       </c>
@@ -2286,7 +2381,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
         <v>143</v>
       </c>
@@ -2294,7 +2389,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B33" t="s">
         <v>148</v>
       </c>
@@ -2317,47 +2412,47 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.80859375" style="7"/>
-    <col min="2" max="2" width="9.47265625" customWidth="1"/>
-    <col min="3" max="3" width="15.80859375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="6"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.80859375" customWidth="1"/>
-    <col min="6" max="6" width="12.47265625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A1" s="6" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="6" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="6" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="6" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="6" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="6" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>158</v>
       </c>
@@ -2376,122 +2471,122 @@
       <c r="F14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>159</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="11">
         <v>41065</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="12">
         <v>24</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="12">
         <v>0</v>
       </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="9"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="F15" s="12"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>160</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="11">
         <v>41078</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="12">
         <v>18</v>
       </c>
       <c r="D16">
         <f>C15-C16</f>
         <v>6</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="12">
         <v>250</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="12">
         <v>120</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="8">
         <f>(E16-E15)/F16*60</f>
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A17" s="7" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="11">
         <v>41092</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="12">
         <v>12</v>
       </c>
       <c r="D17">
         <f t="shared" ref="D17:D19" si="0">C16-C17</f>
         <v>6</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="12">
         <v>480</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="13">
         <v>135</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="8">
         <f t="shared" ref="G17:G19" si="1">(E17-E16)/F17*60</f>
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A18" s="7" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A18" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18" s="11">
         <v>41106</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="12">
         <v>6</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="12">
         <v>740</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="13">
         <v>160</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="8">
         <f t="shared" si="1"/>
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A19" s="7" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A19" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="B19" s="13">
+      <c r="B19" s="11">
         <v>41120</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="12">
         <v>0</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="12">
         <v>1100</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="13">
         <v>145</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="8">
         <f t="shared" si="1"/>
         <v>148.9655172413793</v>
       </c>
@@ -2511,17 +2606,17 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.1875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2537,7 +2632,7 @@
       <c r="E1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2550,212 +2645,265 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.1875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.80859375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" style="1" customWidth="1"/>
+    <col min="3" max="8" width="11.83203125" style="22" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="20">
+      <c r="D2" s="21"/>
+      <c r="E2" s="21">
         <v>30</v>
       </c>
-      <c r="F2" s="20">
+      <c r="F2" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A3" s="19" t="s">
+      <c r="I2" s="23" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21">
         <v>20</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="21">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="19" t="s">
+      <c r="I3" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="20">
+      <c r="D4" s="21"/>
+      <c r="E4" s="21">
         <v>15</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="21">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="19" t="s">
+      <c r="I4" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="20">
+      <c r="D5" s="21"/>
+      <c r="E5" s="21">
         <v>20</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="19" t="s">
+      <c r="G5" s="22">
+        <v>14</v>
+      </c>
+      <c r="H5" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="20">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21">
         <v>15</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="19" t="s">
+      <c r="G6" s="22">
+        <v>22</v>
+      </c>
+      <c r="H6" s="22">
+        <v>2</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20">
+      <c r="D7" s="21"/>
+      <c r="E7" s="21">
         <v>20</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A8" s="19" t="s">
+      <c r="I7" s="23" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="20">
+      <c r="D8" s="21"/>
+      <c r="E8" s="21">
         <v>30</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="19" t="s">
+      <c r="I8" s="23" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="17" t="s">
         <v>139</v>
       </c>
       <c r="B9" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="21">
         <v>30</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I9" s="23" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="5"/>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="16" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="5"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:2" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>$Z$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>$Z$4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>$Z$5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{CD5E5333-BB02-5640-AC97-520BF8D0F172}">
+      <formula1>$Z$2:$Z$5</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
@@ -2767,20 +2915,19 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.1875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.80859375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2793,19 +2940,19 @@
       <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2822,20 +2969,19 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.1875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.80859375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2848,19 +2994,19 @@
       <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2876,20 +3022,19 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.1875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.80859375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2902,19 +3047,19 @@
       <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2928,18 +3073,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.76171875" customWidth="1"/>
-    <col min="3" max="3" width="69.09375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" customWidth="1"/>
+    <col min="3" max="3" width="69.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>110</v>
       </c>
@@ -2950,465 +3095,465 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>111</v>
       </c>
       <c r="B2" t="s">
         <v>153</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>112</v>
       </c>
       <c r="B3" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>113</v>
       </c>
       <c r="B4" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>114</v>
       </c>
       <c r="B5" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>115</v>
       </c>
       <c r="B6" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>116</v>
       </c>
       <c r="B7" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>117</v>
       </c>
       <c r="B8" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>118</v>
       </c>
       <c r="B9" t="s">
         <v>154</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="10" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>119</v>
       </c>
       <c r="B10" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="10" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>120</v>
       </c>
       <c r="B11" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="10" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>121</v>
       </c>
       <c r="B12" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>122</v>
       </c>
       <c r="B13" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="10" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>123</v>
       </c>
       <c r="B14" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="10" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>124</v>
       </c>
       <c r="B15" t="s">
         <v>167</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>125</v>
       </c>
       <c r="B16" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>126</v>
       </c>
       <c r="B17" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>127</v>
       </c>
       <c r="B18" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>128</v>
       </c>
       <c r="B19" t="s">
         <v>82</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>129</v>
       </c>
       <c r="B20" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>130</v>
       </c>
       <c r="B21" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>131</v>
       </c>
       <c r="B22" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="10" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>132</v>
       </c>
       <c r="B23" t="s">
         <v>88</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="10" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>133</v>
       </c>
       <c r="B24" t="s">
         <v>89</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>134</v>
       </c>
       <c r="B25" t="s">
         <v>90</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>135</v>
       </c>
       <c r="B26" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" ht="85" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>136</v>
       </c>
       <c r="B27" t="s">
         <v>92</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="10" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>137</v>
       </c>
       <c r="B28" t="s">
         <v>93</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>138</v>
       </c>
       <c r="B29" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="10" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>139</v>
       </c>
       <c r="B30" t="s">
         <v>95</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>140</v>
       </c>
       <c r="B31" t="s">
         <v>96</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>141</v>
       </c>
       <c r="B32" t="s">
         <v>97</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>142</v>
       </c>
       <c r="B33" t="s">
         <v>98</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>143</v>
       </c>
       <c r="B34" t="s">
         <v>99</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>144</v>
       </c>
       <c r="B35" t="s">
         <v>109</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>145</v>
       </c>
       <c r="B36" t="s">
         <v>100</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>146</v>
       </c>
       <c r="B37" t="s">
         <v>101</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>147</v>
       </c>
       <c r="B38" t="s">
         <v>102</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>148</v>
       </c>
       <c r="B39" t="s">
         <v>103</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>149</v>
       </c>
       <c r="B40" t="s">
         <v>104</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>150</v>
       </c>
       <c r="B41" t="s">
         <v>105</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="10" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>151</v>
       </c>
       <c r="B42" t="s">
         <v>107</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C42" s="10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>152</v>
       </c>
       <c r="B43" t="s">
         <v>108</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="C43" s="10" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding birth_before_marriage function, this Checks for birth before marriages if marriage happens before birth, individual will be removed from family
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rozanitis/Documents/Stevens/Semesters/Fall2018/SSW-555/gedcom-parser/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/latinocodes/PycharmProjects/gedcom-parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675F1F6C-10FC-7248-9F89-040BF250856C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34741FAE-C90B-CD4B-8ADC-BF12CC3DE66C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="19880" windowHeight="15240" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -841,9 +841,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -858,6 +855,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="66">
@@ -928,7 +928,17 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -946,66 +956,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2038,11 +1988,11 @@
       <c r="D9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
     </row>
   </sheetData>
   <sortState ref="A3:D5">
@@ -2647,14 +2597,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" style="1" customWidth="1"/>
-    <col min="3" max="8" width="11.83203125" style="22" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" style="23" customWidth="1"/>
+    <col min="3" max="8" width="11.83203125" style="21" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.15">
@@ -2664,25 +2616,25 @@
       <c r="B1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="19" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2693,17 +2645,17 @@
       <c r="B2" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21">
+      <c r="D2" s="20"/>
+      <c r="E2" s="20">
         <v>30</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="20">
         <v>2</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="22" t="s">
         <v>197</v>
       </c>
     </row>
@@ -2714,17 +2666,17 @@
       <c r="B3" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20">
         <v>20</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="20">
         <v>1</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="22" t="s">
         <v>199</v>
       </c>
       <c r="Z3" t="s">
@@ -2738,17 +2690,17 @@
       <c r="B4" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21">
+      <c r="D4" s="20"/>
+      <c r="E4" s="20">
         <v>15</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="20">
         <v>1.5</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="22" t="s">
         <v>199</v>
       </c>
       <c r="Z4" t="s">
@@ -2762,23 +2714,23 @@
       <c r="B5" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21">
+      <c r="D5" s="20"/>
+      <c r="E5" s="20">
         <v>20</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="20">
         <v>2</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="21">
         <v>14</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="21">
         <v>1.5</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="22" t="s">
         <v>196</v>
       </c>
       <c r="Z5" t="s">
@@ -2792,23 +2744,23 @@
       <c r="B6" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21">
+      <c r="D6" s="20"/>
+      <c r="E6" s="20">
         <v>15</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="20">
         <v>2</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="21">
         <v>22</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="21">
         <v>2</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="22" t="s">
         <v>196</v>
       </c>
     </row>
@@ -2819,17 +2771,17 @@
       <c r="B7" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21">
+      <c r="D7" s="20"/>
+      <c r="E7" s="20">
         <v>20</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="20">
         <v>2</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="I7" s="22" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2840,17 +2792,17 @@
       <c r="B8" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21">
+      <c r="D8" s="20"/>
+      <c r="E8" s="20">
         <v>30</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="20">
         <v>2</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="22" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2861,17 +2813,23 @@
       <c r="B9" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="20">
         <v>30</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="20">
         <v>2</v>
       </c>
-      <c r="I9" s="23" t="s">
-        <v>199</v>
+      <c r="G9" s="21">
+        <v>20</v>
+      </c>
+      <c r="H9" s="21">
+        <v>1</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -2889,13 +2847,13 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>$Z$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>$Z$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>$Z$5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
updating teamReport.xlsx file and adding doc strings to functions
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/latinocodes/PycharmProjects/gedcom-parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34741FAE-C90B-CD4B-8ADC-BF12CC3DE66C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0B4463-9F9E-2E47-8CCB-63CFE1DDF219}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19880" windowHeight="15240" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19880" windowHeight="15240" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="203">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -666,6 +666,15 @@
   </si>
   <si>
     <t>in Progress</t>
+  </si>
+  <si>
+    <t>Pair Programming Story</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -676,7 +685,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -719,6 +728,17 @@
       <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -812,7 +832,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -858,6 +878,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="66">
@@ -928,14 +956,14 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -951,11 +979,41 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2014,8 +2072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A15" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2278,33 +2336,39 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>0</v>
+      </c>
       <c r="B26" t="s">
         <v>137</v>
       </c>
       <c r="C26" t="s">
         <v>93</v>
       </c>
+      <c r="D26" s="25" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27">
-        <v>1</v>
-      </c>
       <c r="B27" t="s">
         <v>138</v>
       </c>
       <c r="C27" t="s">
         <v>94</v>
       </c>
-      <c r="D27" t="s">
-        <v>173</v>
-      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>1</v>
+      </c>
       <c r="B28" t="s">
         <v>139</v>
       </c>
       <c r="C28" t="s">
         <v>95</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
@@ -2358,7 +2422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A102" zoomScale="150" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -2598,7 +2662,7 @@
   <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2676,8 +2740,14 @@
       <c r="F3" s="20">
         <v>1</v>
       </c>
+      <c r="G3" s="21">
+        <v>20</v>
+      </c>
+      <c r="H3" s="21">
+        <v>1</v>
+      </c>
       <c r="I3" s="22" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="Z3" t="s">
         <v>198</v>
@@ -2836,29 +2906,85 @@
       <c r="B14" s="5"/>
     </row>
     <row r="15" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="5"/>
+      <c r="A15" s="24" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="5"/>
-    </row>
-    <row r="20" spans="2:2" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>147</v>
+      </c>
+      <c r="B17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="E17" s="21">
+        <v>20</v>
+      </c>
+      <c r="F17" s="21">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+  <conditionalFormatting sqref="I1:I10 I14:I15 I17:I1048576">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>$Z$5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>$Z$4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>$Z$3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>$Z$5</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>$Z$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>$Z$5</formula>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>$Z$3</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{CD5E5333-BB02-5640-AC97-520BF8D0F172}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I10 I17:I1048576 I14:I15" xr:uid="{CD5E5333-BB02-5640-AC97-520BF8D0F172}">
       <formula1>$Z$2:$Z$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -3029,10 +3155,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3042,7 +3168,7 @@
     <col min="3" max="3" width="69.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>110</v>
       </c>
@@ -3052,19 +3178,25 @@
       <c r="C1" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D1" s="24" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>111</v>
       </c>
       <c r="B2" t="s">
         <v>153</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="26" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="D2" s="25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -3074,8 +3206,11 @@
       <c r="C3" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="D3" s="25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -3085,8 +3220,11 @@
       <c r="C4" s="10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D4" s="25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -3096,8 +3234,11 @@
       <c r="C5" s="10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="D5" s="25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>115</v>
       </c>
@@ -3107,8 +3248,11 @@
       <c r="C6" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="D6" s="25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>116</v>
       </c>
@@ -3118,8 +3262,11 @@
       <c r="C7" s="10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D7" s="25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>117</v>
       </c>
@@ -3129,8 +3276,11 @@
       <c r="C8" s="10" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="D8" s="25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>118</v>
       </c>
@@ -3141,7 +3291,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>119</v>
       </c>
@@ -3152,7 +3302,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>120</v>
       </c>
@@ -3163,7 +3313,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>121</v>
       </c>
@@ -3174,7 +3324,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>122</v>
       </c>
@@ -3185,7 +3335,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>123</v>
       </c>
@@ -3196,7 +3346,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>124</v>
       </c>
@@ -3207,7 +3357,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>125</v>
       </c>
@@ -3218,7 +3368,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>126</v>
       </c>
@@ -3229,7 +3379,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>127</v>
       </c>
@@ -3240,7 +3390,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>128</v>
       </c>
@@ -3251,7 +3401,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>129</v>
       </c>
@@ -3262,7 +3412,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>130</v>
       </c>
@@ -3273,7 +3423,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>131</v>
       </c>
@@ -3284,7 +3434,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>132</v>
       </c>
@@ -3295,7 +3445,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>133</v>
       </c>
@@ -3306,7 +3456,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>134</v>
       </c>
@@ -3317,7 +3467,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>135</v>
       </c>
@@ -3328,7 +3478,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="85" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="85" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>136</v>
       </c>
@@ -3339,7 +3489,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>137</v>
       </c>
@@ -3350,7 +3500,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>138</v>
       </c>
@@ -3361,7 +3511,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>139</v>
       </c>
@@ -3371,8 +3521,11 @@
       <c r="C30" s="10" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="D30" s="25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>140</v>
       </c>
@@ -3383,7 +3536,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>141</v>
       </c>

</xml_diff>

<commit_message>
pair programming story added
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20919"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\Documents\GitHub\gedcom-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="13_ncr:1_{0B041C8F-1391-4066-8283-CF9C72F04E23}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{C28E91ED-5EC8-4502-88CB-3F738715170B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A5AA30-480B-4B89-AF14-BDE799241DC1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="462" windowWidth="19878" windowHeight="15240" tabRatio="500" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="462" windowWidth="19878" windowHeight="15240" tabRatio="500" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,15 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="179020" concurrentCalc="0"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="195">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -651,7 +656,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -854,14 +859,14 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
@@ -2792,19 +2797,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.4"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.76171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.47265625" customWidth="1"/>
+    <col min="3" max="3" width="8.47265625" customWidth="1"/>
+    <col min="4" max="5" width="20.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2821,7 +2826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.95">
+    <row r="3" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
       <c r="A3" s="13" t="s">
         <v>5</v>
       </c>
@@ -2838,7 +2843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.95">
+    <row r="4" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
       <c r="A4" s="13" t="s">
         <v>10</v>
       </c>
@@ -2855,7 +2860,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.95">
+    <row r="5" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
       <c r="A5" s="13" t="s">
         <v>15</v>
       </c>
@@ -2872,7 +2877,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.95">
+    <row r="6" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
@@ -2889,15 +2894,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
     </row>
   </sheetData>
   <sortState ref="A3:D5">
@@ -2919,19 +2924,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.4"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.76171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="6.47265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>27</v>
       </c>
@@ -2948,7 +2953,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2962,7 +2967,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2976,7 +2981,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2990,7 +2995,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3004,7 +3009,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3018,7 +3023,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3032,7 +3037,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3046,7 +3051,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
         <v>46</v>
       </c>
@@ -3054,7 +3059,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
         <v>48</v>
       </c>
@@ -3062,7 +3067,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
         <v>50</v>
       </c>
@@ -3070,7 +3075,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>52</v>
       </c>
@@ -3078,7 +3083,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
         <v>54</v>
       </c>
@@ -3086,7 +3091,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
         <v>56</v>
       </c>
@@ -3094,7 +3099,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>58</v>
       </c>
@@ -3102,7 +3107,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
         <v>60</v>
       </c>
@@ -3110,7 +3115,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
         <v>62</v>
       </c>
@@ -3118,7 +3123,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B18" t="s">
         <v>64</v>
       </c>
@@ -3126,7 +3131,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
         <v>66</v>
       </c>
@@ -3134,7 +3139,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
         <v>68</v>
       </c>
@@ -3142,7 +3147,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
         <v>70</v>
       </c>
@@ -3150,7 +3155,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
         <v>72</v>
       </c>
@@ -3158,7 +3163,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
         <v>74</v>
       </c>
@@ -3166,7 +3171,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
         <v>76</v>
       </c>
@@ -3174,7 +3179,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
         <v>78</v>
       </c>
@@ -3182,7 +3187,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>0</v>
       </c>
@@ -3196,7 +3201,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
         <v>82</v>
       </c>
@@ -3204,7 +3209,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>1</v>
       </c>
@@ -3218,7 +3223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>86</v>
       </c>
@@ -3226,7 +3231,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
         <v>88</v>
       </c>
@@ -3234,7 +3239,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
         <v>90</v>
       </c>
@@ -3242,7 +3247,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
         <v>92</v>
       </c>
@@ -3250,7 +3255,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
         <v>94</v>
       </c>
@@ -3269,51 +3274,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="150" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
+    <sheetView topLeftCell="A4" zoomScale="150" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.4"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.75" style="2"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.75" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.76171875" style="2"/>
+    <col min="2" max="2" width="9.47265625" customWidth="1"/>
+    <col min="3" max="3" width="15.76171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.37890625" customWidth="1"/>
+    <col min="5" max="5" width="6.76171875" customWidth="1"/>
+    <col min="6" max="6" width="12.47265625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>102</v>
       </c>
@@ -3336,7 +3341,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>109</v>
       </c>
@@ -3352,7 +3357,7 @@
       <c r="F15" s="11"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>110</v>
       </c>
@@ -3377,7 +3382,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>111</v>
       </c>
@@ -3402,7 +3407,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>112</v>
       </c>
@@ -3427,7 +3432,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>113</v>
       </c>
@@ -3461,25 +3466,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A3:G8"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.4"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="9.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.37890625" style="2" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6171875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="12.75"/>
-    <row r="2" spans="1:7" ht="12.75"/>
-    <row r="3" spans="1:7" s="4" customFormat="1">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>102</v>
       </c>
@@ -3502,22 +3505,22 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="12.75">
-      <c r="A4" s="28" t="s">
+    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4" s="28">
         <v>41900</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="27">
         <v>32</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="27">
         <v>0</v>
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -3541,7 +3544,7 @@
         <v>14.592592592592593</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -3549,7 +3552,7 @@
         <v>41927</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -3557,7 +3560,7 @@
         <v>41941</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -3575,21 +3578,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:Z25"/>
+  <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="14.1" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" style="1" customWidth="1"/>
-    <col min="3" max="8" width="11.75" style="20" customWidth="1"/>
-    <col min="9" max="9" width="11.75" style="21" customWidth="1"/>
+    <col min="3" max="8" width="11.76171875" style="20" customWidth="1"/>
+    <col min="9" max="9" width="11.76171875" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.4">
+    <row r="1" spans="1:26" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -3618,7 +3621,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="14.1" customHeight="1">
+    <row r="2" spans="1:26" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="16" t="s">
         <v>32</v>
       </c>
@@ -3641,11 +3644,11 @@
       <c r="H2" s="20">
         <v>3</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="26" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.1" customHeight="1">
+    <row r="3" spans="1:26" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="16" t="s">
         <v>34</v>
       </c>
@@ -3675,7 +3678,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.1" customHeight="1">
+    <row r="4" spans="1:26" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="16" t="s">
         <v>36</v>
       </c>
@@ -3705,7 +3708,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.1" customHeight="1">
+    <row r="5" spans="1:26" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="16" t="s">
         <v>38</v>
       </c>
@@ -3735,7 +3738,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.1" customHeight="1">
+    <row r="6" spans="1:26" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="16" t="s">
         <v>40</v>
       </c>
@@ -3762,7 +3765,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.1" customHeight="1">
+    <row r="7" spans="1:26" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="16" t="s">
         <v>42</v>
       </c>
@@ -3789,7 +3792,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.1" customHeight="1">
+    <row r="8" spans="1:26" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="16" t="s">
         <v>44</v>
       </c>
@@ -3816,7 +3819,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.1" customHeight="1">
+    <row r="9" spans="1:26" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="16" t="s">
         <v>84</v>
       </c>
@@ -3842,36 +3845,36 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.1" customHeight="1">
+    <row r="11" spans="1:26" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.1" customHeight="1">
+    <row r="12" spans="1:26" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:26" ht="14.1" customHeight="1">
+    <row r="13" spans="1:26" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.1" customHeight="1">
+    <row r="15" spans="1:26" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:26" ht="14.1" customHeight="1">
+    <row r="16" spans="1:26" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="5" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="14.1" customHeight="1">
+    <row r="21" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B21" s="5"/>
     </row>
-    <row r="23" spans="1:9" ht="14.1" customHeight="1">
+    <row r="23" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="22" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="14.1" customHeight="1">
+    <row r="24" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
         <v>28</v>
       </c>
@@ -3900,7 +3903,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="14.1" customHeight="1">
+    <row r="25" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>128</v>
       </c>
@@ -3915,6 +3918,23 @@
       </c>
       <c r="F25" s="20">
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>174</v>
+      </c>
+      <c r="B26" t="s">
+        <v>175</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="20">
+        <v>20</v>
+      </c>
+      <c r="F26" s="20">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3955,21 +3975,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0" xr3:uid="{78B4E459-6924-5F8B-B7BA-2DD04133E49E}"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.4"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.47265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.37890625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.76171875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.47265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -4009,21 +4029,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0" xr3:uid="{9B253EF2-77E0-53E3-AE26-4D66ECD923F3}"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.4"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.47265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.37890625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.76171875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.47265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -4062,21 +4082,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0" xr3:uid="{85D5C41F-068E-5C55-9968-509E7C2A5619}"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.4"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.47265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.37890625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.76171875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.47265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -4115,18 +4135,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0" xr3:uid="{44B22561-5205-5C8A-B808-2C70100D228F}">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.4"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.75" customWidth="1"/>
-    <col min="3" max="3" width="69.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.76171875" customWidth="1"/>
+    <col min="3" max="3" width="69.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>129</v>
       </c>
@@ -4140,7 +4160,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -4154,7 +4174,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -4168,7 +4188,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4182,7 +4202,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -4196,7 +4216,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -4210,7 +4230,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -4224,7 +4244,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -4238,7 +4258,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -4249,7 +4269,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -4260,7 +4280,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -4271,7 +4291,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -4282,7 +4302,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -4293,7 +4313,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="45">
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>146</v>
       </c>
@@ -4304,7 +4324,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -4315,7 +4335,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -4326,7 +4346,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15">
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -4337,7 +4357,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -4348,7 +4368,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -4359,7 +4379,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -4370,7 +4390,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -4381,7 +4401,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15">
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -4392,7 +4412,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15">
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -4403,7 +4423,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -4414,7 +4434,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30">
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -4425,7 +4445,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>78</v>
       </c>
@@ -4436,7 +4456,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="75">
+    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>161</v>
       </c>
@@ -4447,7 +4467,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>80</v>
       </c>
@@ -4458,7 +4478,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15">
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -4469,7 +4489,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -4483,7 +4503,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -4494,7 +4514,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15">
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -4505,7 +4525,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -4516,7 +4536,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>92</v>
       </c>
@@ -4527,7 +4547,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>171</v>
       </c>
@@ -4538,7 +4558,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15">
+    <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>174</v>
       </c>
@@ -4549,7 +4569,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>177</v>
       </c>
@@ -4560,7 +4580,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>128</v>
       </c>
@@ -4571,7 +4591,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15">
+    <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>94</v>
       </c>
@@ -4582,7 +4602,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>183</v>
       </c>
@@ -4593,7 +4613,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15">
+    <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>186</v>
       </c>
@@ -4604,7 +4624,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15">
+    <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>189</v>
       </c>
@@ -4615,7 +4635,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>192</v>
       </c>

</xml_diff>

<commit_message>
Team Report Updated for sprint 1
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/latinocodes/PycharmProjects/gedcom-parser/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\Documents\GitHub\gedcom-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B187B54E-7271-5444-B7D4-6B1FAF6A20A8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49843B71-7F36-4F59-AC2A-0CDB7F4239F5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19880" windowHeight="15240" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="462" windowWidth="19878" windowHeight="15240" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -28,15 +28,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="205">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -644,6 +646,33 @@
   </si>
   <si>
     <t>List recent Death</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2) Quick meeting on Wednesday to discuss any issues anyone is facing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4) TravisCI - continuous integration has been extremely beneficial </t>
+  </si>
+  <si>
+    <t>5) Making improvements to other developer's code when you see an opportunity to improve it</t>
+  </si>
+  <si>
+    <t>1) Using WhatsApp to stay in contact with one another - it has been very beneficial to know when people are working on or have completed their user stories and also to reachout to teammates when in doubts about something</t>
+  </si>
+  <si>
+    <t>3) Hangouts meeting on weekend (when necessary) to plan next sprint</t>
+  </si>
+  <si>
+    <t>1) Waiting until Tuesday to start our user stories (our team is good about not doing this but still important)</t>
+  </si>
+  <si>
+    <t>2) Becoming complacent with our process - although we have only done one sprint, we should continue to review our process and make changes if necessary</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -654,7 +683,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -663,30 +692,36 @@
       <b/>
       <sz val="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="11"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="13"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="13"/>
@@ -713,6 +748,20 @@
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -738,7 +787,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="66">
+  <cellStyleXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -805,8 +854,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -862,11 +913,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="66"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="66">
+  <cellStyles count="68">
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
@@ -932,9 +996,351 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="67" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="66" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="40">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1035,7 +1441,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1106,7 +1512,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2799,15 +3205,15 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.80859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.47265625" customWidth="1"/>
+    <col min="3" max="3" width="8.47265625" customWidth="1"/>
+    <col min="4" max="5" width="20.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2824,7 +3230,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
       <c r="A3" s="13" t="s">
         <v>5</v>
       </c>
@@ -2841,7 +3247,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
       <c r="A4" s="13" t="s">
         <v>10</v>
       </c>
@@ -2858,7 +3264,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
       <c r="A5" s="13" t="s">
         <v>15</v>
       </c>
@@ -2875,7 +3281,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
@@ -2892,15 +3298,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
     </row>
   </sheetData>
   <sortState ref="A3:D5">
@@ -2920,21 +3326,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:Y33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:C12"/>
+    <sheetView topLeftCell="A15" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.80859375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.47265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>27</v>
       </c>
@@ -2951,318 +3358,556 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+        <v>20</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+        <v>5</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+        <v>20</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+      <c r="E6" s="26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+        <v>10</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E8" s="26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>1</v>
+      </c>
       <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" t="s">
+        <v>175</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>177</v>
+      </c>
+      <c r="C14" t="s">
+        <v>178</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
         <v>46</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C15" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B10" t="s">
+      <c r="D15" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
         <v>48</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C16" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B11" t="s">
+      <c r="D16" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
         <v>50</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C17" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B12" t="s">
-        <v>177</v>
-      </c>
-      <c r="C12" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B13" t="s">
+      <c r="D17" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
         <v>54</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C18" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B14" t="s">
+      <c r="D18" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
         <v>56</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C19" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B16" t="s">
+      <c r="D19" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" t="s">
+        <v>180</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B23" t="s">
         <v>60</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B18" t="s">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B24" t="s">
         <v>64</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C24" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B19" t="s">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B25" t="s">
         <v>66</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C25" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B20" t="s">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B26" t="s">
         <v>68</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C26" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B21" t="s">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B27" t="s">
         <v>70</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C27" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B22" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B23" t="s">
-        <v>174</v>
-      </c>
-      <c r="C23" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B24" t="s">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B28" t="s">
         <v>76</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C28" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B25" t="s">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B29" t="s">
         <v>78</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C29" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26">
-        <v>0</v>
-      </c>
-      <c r="B26" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" t="s">
-        <v>81</v>
-      </c>
-      <c r="D26" s="23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B27" t="s">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B30" t="s">
         <v>82</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C30" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" s="23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B29" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B30" t="s">
+      <c r="D30" s="23"/>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B31" t="s">
         <v>88</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B31" t="s">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B32" t="s">
         <v>90</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B32" t="s">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B33" t="s">
         <v>92</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B33" t="s">
-        <v>94</v>
-      </c>
-      <c r="C33" t="s">
-        <v>95</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState ref="A2:E33">
+    <sortCondition ref="A2"/>
+  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="E2:E14">
+    <cfRule type="cellIs" dxfId="39" priority="25" operator="equal">
+      <formula>$Y$18</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="26" operator="equal">
+      <formula>$Y$17</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="27" operator="equal">
+      <formula>$Y$16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25:E26">
+    <cfRule type="cellIs" dxfId="36" priority="22" operator="equal">
+      <formula>"Complete"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="23" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="24" operator="equal">
+      <formula>"Assigned"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="cellIs" dxfId="33" priority="19" operator="equal">
+      <formula>"Complete"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="20" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="21" operator="equal">
+      <formula>"Assigned"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E32">
+    <cfRule type="cellIs" dxfId="30" priority="16" operator="equal">
+      <formula>"Complete"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="17" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="18" operator="equal">
+      <formula>"Assigned"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E33">
+    <cfRule type="cellIs" dxfId="27" priority="13" operator="equal">
+      <formula>"Complete"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="14" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="15" operator="equal">
+      <formula>"Assigned"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29">
+    <cfRule type="cellIs" dxfId="24" priority="10" operator="equal">
+      <formula>"Complete"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+      <formula>"Assigned"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23">
+    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
+      <formula>"Complete"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+      <formula>"Assigned"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15:E22">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
+      <formula>$Y$18</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
+      <formula>$Y$17</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+      <formula>$Y$16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E8" xr:uid="{43AF2B61-28F2-4BE8-AA5E-BD171B39E9D3}">
+      <formula1>$Z$2:$Z$5</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
@@ -3276,47 +3921,47 @@
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.80859375" style="2"/>
+    <col min="2" max="2" width="9.47265625" customWidth="1"/>
+    <col min="3" max="3" width="15.80859375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
+    <col min="5" max="5" width="6.80859375" customWidth="1"/>
+    <col min="6" max="6" width="12.47265625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>102</v>
       </c>
@@ -3339,7 +3984,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>109</v>
       </c>
@@ -3355,7 +4000,7 @@
       <c r="F15" s="11"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>110</v>
       </c>
@@ -3380,7 +4025,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>111</v>
       </c>
@@ -3405,7 +4050,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>112</v>
       </c>
@@ -3430,7 +4075,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>113</v>
       </c>
@@ -3467,20 +4112,20 @@
   <dimension ref="A3:G8"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="9.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>102</v>
       </c>
@@ -3503,7 +4148,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="27" t="s">
         <v>109</v>
       </c>
@@ -3518,7 +4163,7 @@
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -3532,9 +4177,11 @@
         <v>8</v>
       </c>
       <c r="E5">
+        <f>Sprint1!G10</f>
         <v>197</v>
       </c>
       <c r="F5">
+        <f>(Sprint1!H10*60)</f>
         <v>810</v>
       </c>
       <c r="G5" s="7">
@@ -3542,7 +4189,7 @@
         <v>14.592592592592593</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -3550,7 +4197,7 @@
         <v>41927</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -3558,7 +4205,7 @@
         <v>41941</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -3569,28 +4216,28 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:Z26"/>
+  <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.05" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" style="1" customWidth="1"/>
-    <col min="3" max="8" width="11.83203125" style="20" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" style="21" customWidth="1"/>
+    <col min="3" max="8" width="11.80859375" style="20" customWidth="1"/>
+    <col min="9" max="9" width="11.80859375" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:26" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -3619,7 +4266,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:26" ht="14.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="16" t="s">
         <v>32</v>
       </c>
@@ -3629,7 +4276,9 @@
       <c r="C2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="19"/>
+      <c r="D2" s="26" t="s">
+        <v>119</v>
+      </c>
       <c r="E2" s="19">
         <v>30</v>
       </c>
@@ -3642,11 +4291,11 @@
       <c r="H2" s="20">
         <v>3</v>
       </c>
-      <c r="I2" s="26" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I2" s="30" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="16" t="s">
         <v>34</v>
       </c>
@@ -3656,7 +4305,9 @@
       <c r="C3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="19"/>
+      <c r="D3" s="21" t="s">
+        <v>119</v>
+      </c>
       <c r="E3" s="19">
         <v>20</v>
       </c>
@@ -3669,14 +4320,14 @@
       <c r="H3" s="20">
         <v>1</v>
       </c>
-      <c r="I3" s="21" t="s">
-        <v>119</v>
+      <c r="I3" s="30" t="s">
+        <v>203</v>
       </c>
       <c r="Z3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:26" ht="14.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="16" t="s">
         <v>36</v>
       </c>
@@ -3686,7 +4337,9 @@
       <c r="C4" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="19"/>
+      <c r="D4" s="30" t="s">
+        <v>119</v>
+      </c>
       <c r="E4" s="19">
         <v>15</v>
       </c>
@@ -3699,14 +4352,14 @@
       <c r="H4" s="20">
         <v>1</v>
       </c>
-      <c r="I4" s="21" t="s">
-        <v>119</v>
+      <c r="I4" s="30" t="s">
+        <v>203</v>
       </c>
       <c r="Z4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:26" ht="14.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="16" t="s">
         <v>38</v>
       </c>
@@ -3716,7 +4369,9 @@
       <c r="C5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="19"/>
+      <c r="D5" s="21" t="s">
+        <v>119</v>
+      </c>
       <c r="E5" s="19">
         <v>20</v>
       </c>
@@ -3729,14 +4384,14 @@
       <c r="H5" s="20">
         <v>1.5</v>
       </c>
-      <c r="I5" s="21" t="s">
-        <v>119</v>
+      <c r="I5" s="30" t="s">
+        <v>203</v>
       </c>
       <c r="Z5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:26" ht="14.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="16" t="s">
         <v>40</v>
       </c>
@@ -3746,7 +4401,9 @@
       <c r="C6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="19"/>
+      <c r="D6" s="21" t="s">
+        <v>119</v>
+      </c>
       <c r="E6" s="19">
         <v>15</v>
       </c>
@@ -3759,11 +4416,11 @@
       <c r="H6" s="20">
         <v>2</v>
       </c>
-      <c r="I6" s="21" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I6" s="30" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="16" t="s">
         <v>42</v>
       </c>
@@ -3773,7 +4430,9 @@
       <c r="C7" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="19"/>
+      <c r="D7" s="21" t="s">
+        <v>119</v>
+      </c>
       <c r="E7" s="19">
         <v>20</v>
       </c>
@@ -3786,11 +4445,11 @@
       <c r="H7" s="20">
         <v>2.5</v>
       </c>
-      <c r="I7" s="21" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I7" s="30" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="16" t="s">
         <v>44</v>
       </c>
@@ -3800,7 +4459,9 @@
       <c r="C8" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="19"/>
+      <c r="D8" s="21" t="s">
+        <v>119</v>
+      </c>
       <c r="E8" s="19">
         <v>30</v>
       </c>
@@ -3813,11 +4474,11 @@
       <c r="H8" s="20">
         <v>1.5</v>
       </c>
-      <c r="I8" s="21" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I8" s="30" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="16" t="s">
         <v>84</v>
       </c>
@@ -3827,6 +4488,9 @@
       <c r="C9" s="19" t="s">
         <v>5</v>
       </c>
+      <c r="D9" s="21" t="s">
+        <v>119</v>
+      </c>
       <c r="E9" s="19">
         <v>30</v>
       </c>
@@ -3839,146 +4503,256 @@
       <c r="H9" s="20">
         <v>1</v>
       </c>
-      <c r="I9" s="21" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I9" s="30" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G10" s="20">
+        <f>SUM(G2:G9)</f>
+        <v>197</v>
+      </c>
+      <c r="H10" s="20">
+        <f>SUM(H2:H9)</f>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:26" ht="14.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:26" ht="14.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="5" t="s">
+    <row r="14" spans="1:26" ht="87.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="32" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="32" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="32" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="26.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="32" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="14.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="5" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="5"/>
-    </row>
-    <row r="23" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="22" t="s">
+    <row r="20" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="32" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="63.3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="32" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="14.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="5"/>
+    </row>
+    <row r="25" spans="1:9" ht="14.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="22" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="4" t="s">
+    <row r="26" spans="1:9" ht="14.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B26" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C26" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D26" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E26" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F26" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="G24" s="17" t="s">
+      <c r="G26" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="H24" s="17" t="s">
+      <c r="H26" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="I24" s="18" t="s">
+      <c r="I26" s="18" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
+    <row r="27" spans="1:9" ht="14.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
         <v>177</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" t="s">
         <v>195</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C27" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="20">
+      <c r="D27" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E27" s="20">
         <v>20</v>
       </c>
-      <c r="F25" s="20">
+      <c r="F27" s="20">
         <v>1.5</v>
       </c>
-      <c r="G25" s="20">
+      <c r="G27" s="20">
         <v>20</v>
       </c>
-      <c r="H25" s="20">
+      <c r="H27" s="20">
         <v>2</v>
       </c>
-      <c r="I25" s="21" t="s">
+      <c r="I27" s="30" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="14.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>174</v>
+      </c>
+      <c r="B28" t="s">
+        <v>175</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="21" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" t="s">
-        <v>174</v>
-      </c>
-      <c r="B26" t="s">
-        <v>175</v>
-      </c>
-      <c r="C26" s="20" t="s">
+      <c r="E28" s="20">
+        <v>20</v>
+      </c>
+      <c r="F28" s="20">
+        <v>2</v>
+      </c>
+      <c r="G28" s="20">
+        <v>20</v>
+      </c>
+      <c r="H28" s="20">
+        <v>2</v>
+      </c>
+      <c r="I28" s="30" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="14.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E29" s="20">
         <v>15</v>
       </c>
-      <c r="E26" s="20">
+      <c r="F29" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="I29" s="30" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="14.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="F26" s="20">
-        <v>2</v>
-      </c>
-      <c r="G26" s="20">
-        <v>20</v>
-      </c>
-      <c r="H26" s="20">
-        <v>2</v>
-      </c>
-      <c r="I26" s="21" t="s">
-        <v>119</v>
+      <c r="D30" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="E30" s="20">
+        <v>15</v>
+      </c>
+      <c r="F30" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="I30" s="30" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="I1:I10 I15 I19:I23 I25:I1048576">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+  <conditionalFormatting sqref="I15 I19:I25 I1 I10 D2:D9 I31:I1048576 D27:D30">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
       <formula>$Z$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
       <formula>$Z$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
       <formula>$Z$3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I24">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <conditionalFormatting sqref="I26">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>$Z$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>$Z$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>$Z$3</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I9">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",I2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",I2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27:I30">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",I27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",I27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I10 I15 I19:I23 I25:I1048576" xr:uid="{CD5E5333-BB02-5640-AC97-520BF8D0F172}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I15 I19:I25 D2:D9 I10 D27:D30 I31:I1048576" xr:uid="{CD5E5333-BB02-5640-AC97-520BF8D0F172}">
       <formula1>$Z$2:$Z$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -3989,23 +4763,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="28.1875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.76171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5234375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.80859375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6171875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -4034,10 +4811,229 @@
         <v>118</v>
       </c>
     </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A2" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="29">
+        <v>25</v>
+      </c>
+      <c r="F2" s="29">
+        <v>2</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A3" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3" s="29">
+        <v>25</v>
+      </c>
+      <c r="F3" s="29">
+        <v>2</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A4" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" s="29">
+        <v>30</v>
+      </c>
+      <c r="F4" s="29">
+        <v>2</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A5" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="29">
+        <v>20</v>
+      </c>
+      <c r="F5" s="29">
+        <v>2</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A6" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" s="29">
+        <v>15</v>
+      </c>
+      <c r="F6" s="29">
+        <v>1.5</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="29">
+        <v>30</v>
+      </c>
+      <c r="F7" s="29">
+        <v>2</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A8" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" s="29">
+        <v>20</v>
+      </c>
+      <c r="F8" s="29">
+        <v>1.5</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="X8" s="33" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A9" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" s="29">
+        <v>25</v>
+      </c>
+      <c r="F9" s="29">
+        <v>1.5</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="X9" s="33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="X10" s="33" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="D2:D9">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+      <formula>$X$10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
+      <formula>$X$9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
+      <formula>$X$8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Assigned">
+      <formula>NOT(ISERROR(SEARCH("Assigned",D2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I9">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",I2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",I2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4047,19 +5043,19 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.47265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.80859375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.47265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -4100,19 +5096,19 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.47265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.80859375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.47265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -4151,18 +5147,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:B37"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.83203125" customWidth="1"/>
-    <col min="3" max="3" width="69.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.80859375" customWidth="1"/>
+    <col min="3" max="3" width="69.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>129</v>
       </c>
@@ -4176,7 +5172,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -4190,7 +5186,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -4204,7 +5200,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -4218,7 +5214,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -4232,7 +5228,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -4246,7 +5242,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -4260,7 +5256,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -4274,7 +5270,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -4285,7 +5281,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -4296,7 +5292,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -4307,7 +5303,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -4318,7 +5314,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -4329,7 +5325,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>146</v>
       </c>
@@ -4340,7 +5336,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -4351,7 +5347,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -4362,7 +5358,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -4373,7 +5369,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -4384,7 +5380,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -4395,7 +5391,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -4406,7 +5402,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -4417,7 +5413,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -4428,7 +5424,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -4439,7 +5435,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -4450,7 +5446,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -4461,7 +5457,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>78</v>
       </c>
@@ -4472,7 +5468,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="85" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>161</v>
       </c>
@@ -4483,7 +5479,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>80</v>
       </c>
@@ -4494,7 +5490,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -4505,7 +5501,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -4519,7 +5515,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -4530,7 +5526,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -4541,7 +5537,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -4552,7 +5548,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>92</v>
       </c>
@@ -4563,7 +5559,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>171</v>
       </c>
@@ -4574,7 +5570,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>174</v>
       </c>
@@ -4585,7 +5581,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>177</v>
       </c>
@@ -4596,7 +5592,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>128</v>
       </c>
@@ -4607,7 +5603,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>94</v>
       </c>
@@ -4618,7 +5614,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>183</v>
       </c>
@@ -4629,7 +5625,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>186</v>
       </c>
@@ -4640,7 +5636,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>189</v>
       </c>
@@ -4651,7 +5647,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>192</v>
       </c>
@@ -4664,6 +5660,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added US22 to files
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10909"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\Documents\GitHub\gedcom-parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rozanitis/Documents/Stevens/Semesters/Fall2018/SSW-555/gedcom-parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD3C28E-9F20-4D75-A696-D6CF20EC11B2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5186986-D2BA-8E40-913E-8506F6B78C69}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="462" windowWidth="19878" windowHeight="15240" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19880" windowHeight="15240" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -27,11 +27,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -926,7 +921,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="66"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -934,12 +935,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="68">
@@ -1453,7 +1448,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1524,7 +1519,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3217,15 +3212,15 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.80859375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.47265625" customWidth="1"/>
-    <col min="3" max="3" width="8.47265625" customWidth="1"/>
-    <col min="4" max="5" width="20.47265625" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3242,7 +3237,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>5</v>
       </c>
@@ -3259,7 +3254,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>10</v>
       </c>
@@ -3276,7 +3271,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>15</v>
       </c>
@@ -3293,7 +3288,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
@@ -3310,15 +3305,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
     </row>
   </sheetData>
   <sortState ref="A3:D5">
@@ -3340,20 +3335,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y33"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E33"/>
+    <sheetView topLeftCell="A9" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.80859375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.47265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>27</v>
       </c>
@@ -3370,7 +3365,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3384,7 +3379,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3401,7 +3396,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3418,7 +3413,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3435,7 +3430,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3452,7 +3447,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3469,7 +3464,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3486,7 +3481,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3503,7 +3498,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1</v>
       </c>
@@ -3520,7 +3515,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3537,7 +3532,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>1</v>
       </c>
@@ -3554,7 +3549,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>1</v>
       </c>
@@ -3571,7 +3566,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>1</v>
       </c>
@@ -3588,7 +3583,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2</v>
       </c>
@@ -3605,7 +3600,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>2</v>
       </c>
@@ -3625,7 +3620,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2</v>
       </c>
@@ -3645,7 +3640,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2</v>
       </c>
@@ -3665,7 +3660,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2</v>
       </c>
@@ -3682,7 +3677,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>2</v>
       </c>
@@ -3699,7 +3694,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>2</v>
       </c>
@@ -3716,7 +3711,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>2</v>
       </c>
@@ -3733,7 +3728,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B23" t="s">
         <v>60</v>
       </c>
@@ -3741,7 +3736,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B24" t="s">
         <v>64</v>
       </c>
@@ -3749,7 +3744,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B25" t="s">
         <v>66</v>
       </c>
@@ -3757,7 +3752,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B26" t="s">
         <v>68</v>
       </c>
@@ -3765,7 +3760,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B27" t="s">
         <v>70</v>
       </c>
@@ -3773,7 +3768,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
         <v>76</v>
       </c>
@@ -3781,7 +3776,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B29" t="s">
         <v>78</v>
       </c>
@@ -3789,7 +3784,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B30" t="s">
         <v>82</v>
       </c>
@@ -3798,7 +3793,7 @@
       </c>
       <c r="D30" s="23"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B31" t="s">
         <v>88</v>
       </c>
@@ -3806,7 +3801,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
         <v>90</v>
       </c>
@@ -3814,7 +3809,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B33" t="s">
         <v>92</v>
       </c>
@@ -3933,47 +3928,47 @@
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.80859375" style="2"/>
-    <col min="2" max="2" width="9.47265625" customWidth="1"/>
-    <col min="3" max="3" width="15.80859375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.80859375" customWidth="1"/>
-    <col min="6" max="6" width="12.47265625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>102</v>
       </c>
@@ -3996,7 +3991,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>109</v>
       </c>
@@ -4012,7 +4007,7 @@
       <c r="F15" s="11"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>110</v>
       </c>
@@ -4037,7 +4032,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>111</v>
       </c>
@@ -4062,7 +4057,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>112</v>
       </c>
@@ -4087,7 +4082,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>113</v>
       </c>
@@ -4127,17 +4122,17 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="9.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>102</v>
       </c>
@@ -4160,7 +4155,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="27" t="s">
         <v>109</v>
       </c>
@@ -4175,7 +4170,7 @@
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -4201,7 +4196,7 @@
         <v>14.592592592592593</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -4209,7 +4204,7 @@
         <v>41927</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -4217,7 +4212,7 @@
         <v>41941</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -4237,25 +4232,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5234375" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.234375" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6171875" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -4284,7 +4277,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
         <v>32</v>
       </c>
@@ -4313,7 +4306,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
         <v>34</v>
       </c>
@@ -4345,7 +4338,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="16" t="s">
         <v>36</v>
       </c>
@@ -4377,7 +4370,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="16" t="s">
         <v>38</v>
       </c>
@@ -4409,7 +4402,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="16" t="s">
         <v>40</v>
       </c>
@@ -4438,7 +4431,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>42</v>
       </c>
@@ -4467,7 +4460,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>44</v>
       </c>
@@ -4496,7 +4489,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>84</v>
       </c>
@@ -4525,7 +4518,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>205</v>
       </c>
@@ -4538,115 +4531,115 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="B15" s="34" t="s">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="B15" s="36" t="s">
         <v>199</v>
       </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="B16" s="34" t="s">
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="B16" s="36" t="s">
         <v>196</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B17" s="34" t="s">
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B17" s="36" t="s">
         <v>200</v>
       </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B18" s="34" t="s">
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B18" s="36" t="s">
         <v>197</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B19" s="35" t="s">
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B19" s="37" t="s">
         <v>198</v>
       </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+    </row>
+    <row r="20" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="B20" s="5" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B21" s="34" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B21" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B22" s="34" t="s">
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B22" s="36" t="s">
         <v>202</v>
       </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B24" s="5"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A26" s="37" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A26" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="B26" s="37"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B26" s="35"/>
+    </row>
+    <row r="27" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
@@ -4675,7 +4668,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>177</v>
       </c>
@@ -4704,7 +4697,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>174</v>
       </c>
@@ -4733,7 +4726,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="16" t="s">
         <v>72</v>
       </c>
@@ -4744,7 +4737,7 @@
         <v>10</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E30" s="20">
         <v>15</v>
@@ -4752,11 +4745,17 @@
       <c r="F30" s="20">
         <v>1.5</v>
       </c>
+      <c r="G30" s="20">
+        <v>15</v>
+      </c>
+      <c r="H30" s="20">
+        <v>0.5</v>
+      </c>
       <c r="I30" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -4767,7 +4766,7 @@
         <v>20</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E31" s="20">
         <v>15</v>
@@ -4775,8 +4774,14 @@
       <c r="F31" s="20">
         <v>1.5</v>
       </c>
+      <c r="G31" s="20">
+        <v>5</v>
+      </c>
+      <c r="H31" s="20">
+        <v>0.45</v>
+      </c>
       <c r="I31" s="30" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -4844,23 +4849,23 @@
   <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="28.1875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="28.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.76171875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5234375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.80859375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -4889,7 +4894,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:24" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
         <v>46</v>
       </c>
@@ -4912,7 +4917,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
         <v>48</v>
       </c>
@@ -4935,7 +4940,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="16" t="s">
         <v>50</v>
       </c>
@@ -4958,7 +4963,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="16" t="s">
         <v>54</v>
       </c>
@@ -4981,7 +4986,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="16" t="s">
         <v>56</v>
       </c>
@@ -5004,7 +5009,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>86</v>
       </c>
@@ -5027,7 +5032,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>128</v>
       </c>
@@ -5053,7 +5058,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:24" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>94</v>
       </c>
@@ -5079,8 +5084,8 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.4">
-      <c r="B10" s="36" t="s">
+    <row r="10" spans="1:24" ht="14" x14ac:dyDescent="0.15">
+      <c r="B10" s="33" t="s">
         <v>205</v>
       </c>
       <c r="G10">
@@ -5132,19 +5137,19 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.47265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.80859375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -5185,19 +5190,19 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.47265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.80859375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -5236,18 +5241,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:B31"/>
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.80859375" customWidth="1"/>
-    <col min="3" max="3" width="69.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" customWidth="1"/>
+    <col min="3" max="3" width="69.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>129</v>
       </c>
@@ -5261,7 +5266,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -5275,7 +5280,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -5289,7 +5294,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -5303,7 +5308,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -5317,7 +5322,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -5331,7 +5336,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -5345,7 +5350,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -5359,7 +5364,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -5370,7 +5375,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -5381,7 +5386,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -5392,7 +5397,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -5403,7 +5408,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -5414,7 +5419,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>146</v>
       </c>
@@ -5425,7 +5430,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -5436,7 +5441,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -5447,7 +5452,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -5458,7 +5463,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -5469,7 +5474,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -5480,7 +5485,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -5491,7 +5496,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -5502,7 +5507,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -5513,7 +5518,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -5524,7 +5529,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -5535,7 +5540,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -5546,7 +5551,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>78</v>
       </c>
@@ -5557,7 +5562,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="85" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>161</v>
       </c>
@@ -5568,7 +5573,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>80</v>
       </c>
@@ -5579,7 +5584,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -5590,7 +5595,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -5604,7 +5609,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -5615,7 +5620,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -5626,7 +5631,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -5637,7 +5642,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>92</v>
       </c>
@@ -5648,7 +5653,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>171</v>
       </c>
@@ -5659,7 +5664,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>174</v>
       </c>
@@ -5670,7 +5675,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>177</v>
       </c>
@@ -5681,7 +5686,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>128</v>
       </c>
@@ -5692,7 +5697,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>94</v>
       </c>
@@ -5703,7 +5708,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>183</v>
       </c>
@@ -5714,7 +5719,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>186</v>
       </c>
@@ -5725,7 +5730,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>189</v>
       </c>
@@ -5736,7 +5741,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>192</v>
       </c>

</xml_diff>

<commit_message>
completing US37, added a new GEDCOM for more test data, updated TeamReport
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rozanitis/Documents/Stevens/Semesters/Fall2018/SSW-555/gedcom-parser/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/latinocodes/PycharmProjects/gedcom-parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398F0C5F-C854-8D45-9B03-03F6F1CFE471}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8186813-EFF0-4A4D-9DF8-853C56A80EE7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24440" windowHeight="15240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24440" windowHeight="15240" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="215">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -695,6 +695,9 @@
   </si>
   <si>
     <t>Review results of Sprint 2</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -950,6 +953,7 @@
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -962,7 +966,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -3228,7 +3231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0"/>
+    <sheetView zoomScale="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3327,11 +3330,11 @@
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
     </row>
   </sheetData>
   <sortState ref="A3:D5">
@@ -3365,7 +3368,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="31" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -4561,64 +4564,64 @@
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="34" t="s">
         <v>199</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="34" t="s">
         <v>196</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="34" t="s">
         <v>200</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="34" t="s">
         <v>197</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="35" t="s">
         <v>198</v>
       </c>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
     </row>
     <row r="20" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="B20" s="5" t="s">
@@ -4626,34 +4629,34 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="34" t="s">
         <v>201</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B24" s="5"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="B26" s="32"/>
+      <c r="B26" s="33"/>
     </row>
     <row r="27" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
@@ -4864,7 +4867,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96723CB6-6D85-DA4E-8BFC-88DDD98C4269}">
   <dimension ref="A1:Z24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5067,7 +5072,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E8" s="19">
         <v>20</v>
@@ -5075,8 +5080,14 @@
       <c r="F8" s="19">
         <v>1.5</v>
       </c>
+      <c r="G8" s="20">
+        <v>20</v>
+      </c>
+      <c r="H8" s="20">
+        <v>2</v>
+      </c>
       <c r="I8" s="29" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
@@ -5090,7 +5101,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E9" s="19">
         <v>25</v>
@@ -5098,8 +5109,14 @@
       <c r="F9" s="19">
         <v>1.5</v>
       </c>
+      <c r="G9" s="20">
+        <v>25</v>
+      </c>
+      <c r="H9" s="20">
+        <v>2</v>
+      </c>
       <c r="I9" s="29" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
@@ -5108,11 +5125,11 @@
       </c>
       <c r="G10" s="20">
         <f>SUM(G2:G9)</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="H10" s="20">
         <f>SUM(H2:H9)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
@@ -5129,54 +5146,54 @@
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
     </row>
     <row r="20" spans="2:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="36" t="s">
@@ -5185,21 +5202,21 @@
       <c r="C20" s="36"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B24" s="5"/>
@@ -5234,7 +5251,7 @@
       <formula>NOT(ISERROR(SEARCH("No",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I20:I1048576 I10:I11 D2:D9" xr:uid="{41B507A7-1EDD-5E44-99AB-07AE6335B50A}">
       <formula1>$Z$2:$Z$5</formula1>
     </dataValidation>
@@ -5354,7 +5371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A32" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Team report updated for sprint 2
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\Documents\GitHub\gedcom-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F5C023-1DB1-4935-9848-F61D4C85372C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D39306-B9D9-4FE7-9037-DBC24EC870ED}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="462" windowWidth="24438" windowHeight="15240" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4875,7 +4875,7 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B16" sqref="B16:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -4932,7 +4932,7 @@
         <v>20</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E2" s="19">
         <v>25</v>
@@ -4940,8 +4940,14 @@
       <c r="F2" s="19">
         <v>2</v>
       </c>
+      <c r="G2" s="20">
+        <v>18</v>
+      </c>
+      <c r="H2" s="20">
+        <v>2</v>
+      </c>
       <c r="I2" s="29" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.4">
@@ -5138,11 +5144,11 @@
       </c>
       <c r="G10" s="20">
         <f>SUM(G2:G9)</f>
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="H10" s="20">
         <f>SUM(H2:H9)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Test cases for US10 added
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\Documents\GitHub\gedcom-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D39306-B9D9-4FE7-9037-DBC24EC870ED}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62036BE-CFE3-4BE0-82E3-3D0308C1B879}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="462" windowWidth="24438" windowHeight="15240" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4875,7 +4875,7 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:I16"/>
+      <selection activeCell="B17" sqref="B17:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -5071,7 +5071,7 @@
         <v>2</v>
       </c>
       <c r="G7" s="20">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H7" s="20">
         <v>2</v>
@@ -5144,7 +5144,7 @@
       </c>
       <c r="G10" s="20">
         <f>SUM(G2:G9)</f>
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="H10" s="20">
         <f>SUM(H2:H9)</f>

</xml_diff>

<commit_message>
Team report updated and docstring added
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\Documents\GitHub\gedcom-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62036BE-CFE3-4BE0-82E3-3D0308C1B879}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A04603E-6BDD-4D1A-AAF4-1BCAAD25C20F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="462" windowWidth="24438" windowHeight="15240" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4875,7 +4875,7 @@
   <dimension ref="A1:Z24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:I17"/>
+      <selection activeCell="B18" sqref="B18:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -4987,7 +4987,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E4" s="19">
         <v>30</v>
@@ -4995,8 +4995,14 @@
       <c r="F4" s="19">
         <v>2</v>
       </c>
+      <c r="G4" s="20">
+        <v>28</v>
+      </c>
+      <c r="H4" s="20">
+        <v>1.5</v>
+      </c>
       <c r="I4" s="29" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="Z4" t="s">
         <v>123</v>
@@ -5144,11 +5150,11 @@
       </c>
       <c r="G10" s="20">
         <f>SUM(G2:G9)</f>
-        <v>87</v>
+        <v>115</v>
       </c>
       <c r="H10" s="20">
         <f>SUM(H2:H9)</f>
-        <v>8</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
new stories added to ream report
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\Documents\GitHub\gedcom-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A04603E-6BDD-4D1A-AAF4-1BCAAD25C20F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2E3D30-30F0-4889-8866-A4240E4C8A80}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="462" windowWidth="24438" windowHeight="15240" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="462" windowWidth="24438" windowHeight="15240" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,9 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Stories!$A$1:$E$43</definedName>
+  </definedNames>
   <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="216">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -703,6 +706,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Result</t>
   </si>
 </sst>
 </file>
@@ -896,7 +902,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -973,6 +979,12 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="68">
@@ -3359,10 +3371,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Y33"/>
+  <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -3622,8 +3634,8 @@
       <c r="D15" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="30" t="s">
-        <v>121</v>
+      <c r="E15" s="26" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.4">
@@ -3659,8 +3671,8 @@
       <c r="D17" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="30" t="s">
-        <v>121</v>
+      <c r="E17" s="26" t="s">
+        <v>119</v>
       </c>
       <c r="Y17" t="s">
         <v>123</v>
@@ -3716,8 +3728,8 @@
       <c r="D20" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="30" t="s">
-        <v>121</v>
+      <c r="E20" s="26" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.4">
@@ -3756,95 +3768,119 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
-        <v>60</v>
+        <v>146</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C28" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C29" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B30" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C30" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" s="23"/>
+        <v>77</v>
+      </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B31" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C32" t="s">
-        <v>91</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="D32" s="23"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B35" t="s">
         <v>92</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C35" t="s">
         <v>93</v>
       </c>
     </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B36" t="s">
+        <v>183</v>
+      </c>
+      <c r="C36" t="s">
+        <v>184</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:E33">
+  <sortState ref="A2:E36">
     <sortCondition ref="A2"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3859,7 +3895,7 @@
       <formula>$Y$16</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25:E26">
+  <conditionalFormatting sqref="E26:E27">
     <cfRule type="cellIs" dxfId="35" priority="22" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
@@ -3870,7 +3906,7 @@
       <formula>"Assigned"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
+  <conditionalFormatting sqref="E32:E33">
     <cfRule type="cellIs" dxfId="32" priority="19" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
@@ -3881,7 +3917,7 @@
       <formula>"Assigned"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
+  <conditionalFormatting sqref="E34">
     <cfRule type="cellIs" dxfId="29" priority="16" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
@@ -3892,7 +3928,7 @@
       <formula>"Assigned"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E33">
+  <conditionalFormatting sqref="E35">
     <cfRule type="cellIs" dxfId="26" priority="13" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
@@ -3903,7 +3939,7 @@
       <formula>"Assigned"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
+  <conditionalFormatting sqref="E31">
     <cfRule type="cellIs" dxfId="23" priority="10" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
@@ -3914,7 +3950,7 @@
       <formula>"Assigned"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
+  <conditionalFormatting sqref="E24">
     <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
@@ -3925,7 +3961,7 @@
       <formula>"Assigned"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15:E22">
+  <conditionalFormatting sqref="E15:E23">
     <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
       <formula>$Y$18</formula>
     </cfRule>
@@ -3950,8 +3986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="150" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView topLeftCell="A16" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -4144,8 +4180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:G8"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -4258,7 +4294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
@@ -4874,8 +4910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96723CB6-6D85-DA4E-8BFC-88DDD98C4269}">
   <dimension ref="A1:Z24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:I18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -5394,10 +5430,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D43"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -5405,9 +5442,10 @@
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.80859375" customWidth="1"/>
     <col min="3" max="3" width="69.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>129</v>
       </c>
@@ -5420,8 +5458,11 @@
       <c r="D1" s="22" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+      <c r="E1" s="37" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -5434,8 +5475,12 @@
       <c r="D2" s="23" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+      <c r="E2" s="38" t="str">
+        <f>VLOOKUP(A2,Backlog!B:B,1,FALSE)</f>
+        <v>US01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -5448,8 +5493,12 @@
       <c r="D3" s="23" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+      <c r="E3" s="38" t="str">
+        <f>VLOOKUP(A3,Backlog!B:B,1,FALSE)</f>
+        <v>US02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -5462,8 +5511,12 @@
       <c r="D4" s="23" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+      <c r="E4" s="38" t="str">
+        <f>VLOOKUP(A4,Backlog!B:B,1,FALSE)</f>
+        <v>US03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -5476,8 +5529,12 @@
       <c r="D5" s="23" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+      <c r="E5" s="38" t="str">
+        <f>VLOOKUP(A5,Backlog!B:B,1,FALSE)</f>
+        <v>US04</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -5490,8 +5547,12 @@
       <c r="D6" s="23" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+      <c r="E6" s="38" t="str">
+        <f>VLOOKUP(A6,Backlog!B:B,1,FALSE)</f>
+        <v>US05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -5504,8 +5565,12 @@
       <c r="D7" s="23" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+      <c r="E7" s="38" t="str">
+        <f>VLOOKUP(A7,Backlog!B:B,1,FALSE)</f>
+        <v>US06</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -5518,8 +5583,12 @@
       <c r="D8" s="23" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+      <c r="E8" s="38" t="str">
+        <f>VLOOKUP(A8,Backlog!B:B,1,FALSE)</f>
+        <v>US07</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -5529,8 +5598,15 @@
       <c r="C9" s="9" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+      <c r="D9" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="E9" s="38" t="str">
+        <f>VLOOKUP(A9,Backlog!B:B,1,FALSE)</f>
+        <v>US08</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -5540,8 +5616,15 @@
       <c r="C10" s="9" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+      <c r="D10" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="E10" s="38" t="str">
+        <f>VLOOKUP(A10,Backlog!B:B,1,FALSE)</f>
+        <v>US09</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -5551,8 +5634,15 @@
       <c r="C11" s="9" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+      <c r="D11" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="E11" s="38" t="str">
+        <f>VLOOKUP(A11,Backlog!B:B,1,FALSE)</f>
+        <v>US10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -5562,8 +5652,12 @@
       <c r="C12" s="9" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+      <c r="E12" s="38" t="e">
+        <f>VLOOKUP(A12,Backlog!B:B,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -5573,8 +5667,15 @@
       <c r="C13" s="9" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.4">
+      <c r="D13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E13" s="38" t="str">
+        <f>VLOOKUP(A13,Backlog!B:B,1,FALSE)</f>
+        <v>US12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>146</v>
       </c>
@@ -5584,8 +5685,12 @@
       <c r="C14" s="9" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+      <c r="E14" s="38" t="str">
+        <f>VLOOKUP(A14,Backlog!B:B,1,FALSE)</f>
+        <v>US13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -5595,8 +5700,15 @@
       <c r="C15" s="9" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+      <c r="D15" t="s">
+        <v>134</v>
+      </c>
+      <c r="E15" s="38" t="str">
+        <f>VLOOKUP(A15,Backlog!B:B,1,FALSE)</f>
+        <v>US14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -5606,8 +5718,15 @@
       <c r="C16" s="9" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+      <c r="D16" t="s">
+        <v>134</v>
+      </c>
+      <c r="E16" s="38" t="str">
+        <f>VLOOKUP(A16,Backlog!B:B,1,FALSE)</f>
+        <v>US15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -5617,8 +5736,12 @@
       <c r="C17" s="9" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+      <c r="E17" s="38" t="str">
+        <f>VLOOKUP(A17,Backlog!B:B,1,FALSE)</f>
+        <v>US16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -5628,8 +5751,12 @@
       <c r="C18" s="9" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+      <c r="E18" s="38" t="e">
+        <f>VLOOKUP(A18,Backlog!B:B,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -5639,8 +5766,12 @@
       <c r="C19" s="9" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+      <c r="E19" s="38" t="str">
+        <f>VLOOKUP(A19,Backlog!B:B,1,FALSE)</f>
+        <v>US18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -5650,8 +5781,12 @@
       <c r="C20" s="9" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+      <c r="E20" s="38" t="str">
+        <f>VLOOKUP(A20,Backlog!B:B,1,FALSE)</f>
+        <v>US19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -5661,8 +5796,12 @@
       <c r="C21" s="9" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+      <c r="E21" s="38" t="str">
+        <f>VLOOKUP(A21,Backlog!B:B,1,FALSE)</f>
+        <v>US20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -5672,8 +5811,12 @@
       <c r="C22" s="9" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+      <c r="E22" s="38" t="str">
+        <f>VLOOKUP(A22,Backlog!B:B,1,FALSE)</f>
+        <v>US21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -5683,8 +5826,15 @@
       <c r="C23" s="9" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+      <c r="D23" t="s">
+        <v>134</v>
+      </c>
+      <c r="E23" s="38" t="str">
+        <f>VLOOKUP(A23,Backlog!B:B,1,FALSE)</f>
+        <v>US22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -5694,8 +5844,12 @@
       <c r="C24" s="9" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+      <c r="E24" s="38" t="str">
+        <f>VLOOKUP(A24,Backlog!B:B,1,FALSE)</f>
+        <v>US23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -5705,8 +5859,12 @@
       <c r="C25" s="9" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+      <c r="E25" s="38" t="str">
+        <f>VLOOKUP(A25,Backlog!B:B,1,FALSE)</f>
+        <v>US24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>78</v>
       </c>
@@ -5716,8 +5874,12 @@
       <c r="C26" s="9" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.4">
+      <c r="E26" s="38" t="str">
+        <f>VLOOKUP(A26,Backlog!B:B,1,FALSE)</f>
+        <v>US25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="75" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>161</v>
       </c>
@@ -5727,8 +5889,12 @@
       <c r="C27" s="9" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+      <c r="E27" s="38" t="e">
+        <f>VLOOKUP(A27,Backlog!B:B,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>80</v>
       </c>
@@ -5738,8 +5904,12 @@
       <c r="C28" s="9" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+      <c r="E28" s="38" t="str">
+        <f>VLOOKUP(A28,Backlog!B:B,1,FALSE)</f>
+        <v>US27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -5749,8 +5919,12 @@
       <c r="C29" s="9" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+      <c r="E29" s="38" t="str">
+        <f>VLOOKUP(A29,Backlog!B:B,1,FALSE)</f>
+        <v>US28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -5763,8 +5937,12 @@
       <c r="D30" s="23" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+      <c r="E30" s="38" t="str">
+        <f>VLOOKUP(A30,Backlog!B:B,1,FALSE)</f>
+        <v>US29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -5774,8 +5952,15 @@
       <c r="C31" s="9" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+      <c r="D31" t="s">
+        <v>134</v>
+      </c>
+      <c r="E31" s="38" t="str">
+        <f>VLOOKUP(A31,Backlog!B:B,1,FALSE)</f>
+        <v>US30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -5785,8 +5970,12 @@
       <c r="C32" s="9" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+      <c r="E32" s="38" t="str">
+        <f>VLOOKUP(A32,Backlog!B:B,1,FALSE)</f>
+        <v>US31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -5796,8 +5985,12 @@
       <c r="C33" s="9" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+      <c r="E33" s="38" t="str">
+        <f>VLOOKUP(A33,Backlog!B:B,1,FALSE)</f>
+        <v>US32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>92</v>
       </c>
@@ -5807,8 +6000,12 @@
       <c r="C34" s="9" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+      <c r="E34" s="38" t="str">
+        <f>VLOOKUP(A34,Backlog!B:B,1,FALSE)</f>
+        <v>US33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>171</v>
       </c>
@@ -5818,8 +6015,12 @@
       <c r="C35" s="9" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+      <c r="E35" s="38" t="e">
+        <f>VLOOKUP(A35,Backlog!B:B,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>174</v>
       </c>
@@ -5829,8 +6030,15 @@
       <c r="C36" s="9" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+      <c r="D36" t="s">
+        <v>134</v>
+      </c>
+      <c r="E36" s="38" t="str">
+        <f>VLOOKUP(A36,Backlog!B:B,1,FALSE)</f>
+        <v>US35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>177</v>
       </c>
@@ -5840,8 +6048,15 @@
       <c r="C37" s="9" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+      <c r="D37" t="s">
+        <v>134</v>
+      </c>
+      <c r="E37" s="38" t="str">
+        <f>VLOOKUP(A37,Backlog!B:B,1,FALSE)</f>
+        <v>US36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>128</v>
       </c>
@@ -5851,8 +6066,15 @@
       <c r="C38" s="9" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+      <c r="D38" t="s">
+        <v>134</v>
+      </c>
+      <c r="E38" s="38" t="str">
+        <f>VLOOKUP(A38,Backlog!B:B,1,FALSE)</f>
+        <v>US37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>94</v>
       </c>
@@ -5862,8 +6084,15 @@
       <c r="C39" s="9" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+      <c r="D39" t="s">
+        <v>134</v>
+      </c>
+      <c r="E39" s="38" t="str">
+        <f>VLOOKUP(A39,Backlog!B:B,1,FALSE)</f>
+        <v>US38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>183</v>
       </c>
@@ -5873,8 +6102,15 @@
       <c r="C40" s="9" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+      <c r="D40" t="s">
+        <v>134</v>
+      </c>
+      <c r="E40" s="38" t="str">
+        <f>VLOOKUP(A40,Backlog!B:B,1,FALSE)</f>
+        <v>US39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>186</v>
       </c>
@@ -5884,8 +6120,12 @@
       <c r="C41" s="9" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+      <c r="E41" s="38" t="e">
+        <f>VLOOKUP(A41,Backlog!B:B,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>189</v>
       </c>
@@ -5895,8 +6135,12 @@
       <c r="C42" s="9" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+      <c r="E42" s="38" t="e">
+        <f>VLOOKUP(A42,Backlog!B:B,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>192</v>
       </c>
@@ -5906,8 +6150,19 @@
       <c r="C43" s="9" t="s">
         <v>194</v>
       </c>
+      <c r="E43" s="38" t="e">
+        <f>VLOOKUP(A43,Backlog!B:B,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E43" xr:uid="{736FD6F7-58B9-4FC3-9805-6B2AEF47D95A}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="#N/A"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added check_parents_not_too_old function and tests for US12
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10909"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\Documents\GitHub\gedcom-parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rozanitis/Documents/Stevens/Semesters/Fall2018/SSW-555/gedcom-parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D39306-B9D9-4FE7-9037-DBC24EC870ED}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DE029E-1B35-564E-B78D-DCAEBCE91ADC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="462" windowWidth="24438" windowHeight="15240" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24440" windowHeight="15240" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -27,11 +27,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1476,7 +1471,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1547,7 +1542,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3238,15 +3233,15 @@
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.80859375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.47265625" customWidth="1"/>
-    <col min="3" max="3" width="8.47265625" customWidth="1"/>
-    <col min="4" max="5" width="20.47265625" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3263,7 +3258,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>5</v>
       </c>
@@ -3280,7 +3275,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>10</v>
       </c>
@@ -3297,7 +3292,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>15</v>
       </c>
@@ -3314,7 +3309,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
@@ -3331,7 +3326,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
@@ -3365,16 +3360,16 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.80859375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.47265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="31" t="s">
         <v>27</v>
       </c>
@@ -3391,7 +3386,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3405,7 +3400,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3422,7 +3417,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3439,7 +3434,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3456,7 +3451,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3473,7 +3468,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3490,7 +3485,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3507,7 +3502,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3524,7 +3519,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1</v>
       </c>
@@ -3541,7 +3536,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3558,7 +3553,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>1</v>
       </c>
@@ -3575,7 +3570,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>1</v>
       </c>
@@ -3592,7 +3587,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>1</v>
       </c>
@@ -3609,7 +3604,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2</v>
       </c>
@@ -3626,7 +3621,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>2</v>
       </c>
@@ -3646,7 +3641,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2</v>
       </c>
@@ -3666,7 +3661,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2</v>
       </c>
@@ -3686,7 +3681,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2</v>
       </c>
@@ -3703,7 +3698,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>2</v>
       </c>
@@ -3720,7 +3715,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>2</v>
       </c>
@@ -3737,7 +3732,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>2</v>
       </c>
@@ -3754,7 +3749,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B23" t="s">
         <v>60</v>
       </c>
@@ -3762,7 +3757,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B24" t="s">
         <v>64</v>
       </c>
@@ -3770,7 +3765,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B25" t="s">
         <v>66</v>
       </c>
@@ -3778,7 +3773,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B26" t="s">
         <v>68</v>
       </c>
@@ -3786,7 +3781,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B27" t="s">
         <v>70</v>
       </c>
@@ -3794,7 +3789,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
         <v>76</v>
       </c>
@@ -3802,7 +3797,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B29" t="s">
         <v>78</v>
       </c>
@@ -3810,7 +3805,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B30" t="s">
         <v>82</v>
       </c>
@@ -3819,7 +3814,7 @@
       </c>
       <c r="D30" s="23"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B31" t="s">
         <v>88</v>
       </c>
@@ -3827,7 +3822,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
         <v>90</v>
       </c>
@@ -3835,7 +3830,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B33" t="s">
         <v>92</v>
       </c>
@@ -3954,47 +3949,47 @@
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.80859375" style="2"/>
-    <col min="2" max="2" width="9.47265625" customWidth="1"/>
-    <col min="3" max="3" width="15.80859375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.80859375" customWidth="1"/>
-    <col min="6" max="6" width="12.47265625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>102</v>
       </c>
@@ -4017,7 +4012,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>109</v>
       </c>
@@ -4033,7 +4028,7 @@
       <c r="F15" s="11"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>110</v>
       </c>
@@ -4058,7 +4053,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>111</v>
       </c>
@@ -4083,7 +4078,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>112</v>
       </c>
@@ -4108,7 +4103,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>113</v>
       </c>
@@ -4148,17 +4143,17 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="9.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>102</v>
       </c>
@@ -4181,7 +4176,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="27" t="s">
         <v>109</v>
       </c>
@@ -4196,7 +4191,7 @@
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -4222,7 +4217,7 @@
         <v>14.592592592592593</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -4230,7 +4225,7 @@
         <v>41927</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -4238,7 +4233,7 @@
         <v>41941</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -4260,21 +4255,21 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.47265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" style="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="20" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="21" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -4303,7 +4298,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
         <v>32</v>
       </c>
@@ -4332,7 +4327,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
         <v>34</v>
       </c>
@@ -4364,7 +4359,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="16" t="s">
         <v>36</v>
       </c>
@@ -4396,7 +4391,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="16" t="s">
         <v>38</v>
       </c>
@@ -4428,7 +4423,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="16" t="s">
         <v>40</v>
       </c>
@@ -4457,7 +4452,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>42</v>
       </c>
@@ -4486,7 +4481,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>44</v>
       </c>
@@ -4515,7 +4510,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>84</v>
       </c>
@@ -4544,7 +4539,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>205</v>
       </c>
@@ -4557,20 +4552,20 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B15" s="34" t="s">
         <v>199</v>
       </c>
@@ -4582,7 +4577,7 @@
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B16" s="34" t="s">
         <v>196</v>
       </c>
@@ -4594,7 +4589,7 @@
       <c r="H16" s="34"/>
       <c r="I16" s="34"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B17" s="34" t="s">
         <v>200</v>
       </c>
@@ -4606,7 +4601,7 @@
       <c r="H17" s="34"/>
       <c r="I17" s="34"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B18" s="34" t="s">
         <v>197</v>
       </c>
@@ -4618,7 +4613,7 @@
       <c r="H18" s="34"/>
       <c r="I18" s="34"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B19" s="35" t="s">
         <v>198</v>
       </c>
@@ -4630,12 +4625,12 @@
       <c r="H19" s="35"/>
       <c r="I19" s="35"/>
     </row>
-    <row r="20" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="B20" s="5" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B21" s="34" t="s">
         <v>201</v>
       </c>
@@ -4646,7 +4641,7 @@
       <c r="G21" s="34"/>
       <c r="H21" s="34"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B22" s="34" t="s">
         <v>202</v>
       </c>
@@ -4656,16 +4651,16 @@
       <c r="F22" s="34"/>
       <c r="G22" s="34"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B24" s="5"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="33" t="s">
         <v>127</v>
       </c>
       <c r="B26" s="33"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
@@ -4694,7 +4689,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>177</v>
       </c>
@@ -4723,7 +4718,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>174</v>
       </c>
@@ -4752,7 +4747,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="16" t="s">
         <v>72</v>
       </c>
@@ -4781,7 +4776,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -4874,25 +4869,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96723CB6-6D85-DA4E-8BFC-88DDD98C4269}">
   <dimension ref="A1:Z24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:I16"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.47265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" style="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="20" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="21" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>129</v>
       </c>
@@ -4921,7 +4914,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
         <v>46</v>
       </c>
@@ -4950,7 +4943,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
         <v>48</v>
       </c>
@@ -4976,7 +4969,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="16" t="s">
         <v>50</v>
       </c>
@@ -5002,7 +4995,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="16" t="s">
         <v>54</v>
       </c>
@@ -5013,7 +5006,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E5" s="19">
         <v>20</v>
@@ -5021,6 +5014,12 @@
       <c r="F5" s="19">
         <v>2</v>
       </c>
+      <c r="G5" s="20">
+        <v>15</v>
+      </c>
+      <c r="H5" s="20">
+        <v>2.5</v>
+      </c>
       <c r="I5" s="29" t="s">
         <v>204</v>
       </c>
@@ -5028,7 +5027,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="16" t="s">
         <v>56</v>
       </c>
@@ -5051,7 +5050,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>86</v>
       </c>
@@ -5080,7 +5079,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>128</v>
       </c>
@@ -5109,7 +5108,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>94</v>
       </c>
@@ -5138,33 +5137,33 @@
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>205</v>
       </c>
       <c r="G10" s="20">
         <f>SUM(G2:G9)</f>
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="H10" s="20">
         <f>SUM(H2:H9)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
       <c r="D15" s="34"/>
@@ -5174,7 +5173,7 @@
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B16" s="34"/>
       <c r="C16" s="34"/>
       <c r="D16" s="34"/>
@@ -5184,7 +5183,7 @@
       <c r="H16" s="34"/>
       <c r="I16" s="34"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B17" s="34"/>
       <c r="C17" s="34"/>
       <c r="D17" s="34"/>
@@ -5194,7 +5193,7 @@
       <c r="H17" s="34"/>
       <c r="I17" s="34"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B18" s="34"/>
       <c r="C18" s="34"/>
       <c r="D18" s="34"/>
@@ -5204,7 +5203,7 @@
       <c r="H18" s="34"/>
       <c r="I18" s="34"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B19" s="35"/>
       <c r="C19" s="35"/>
       <c r="D19" s="35"/>
@@ -5214,13 +5213,13 @@
       <c r="H19" s="35"/>
       <c r="I19" s="35"/>
     </row>
-    <row r="20" spans="2:9" ht="13" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="36" t="s">
         <v>126</v>
       </c>
       <c r="C20" s="36"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B21" s="34"/>
       <c r="C21" s="34"/>
       <c r="D21" s="34"/>
@@ -5229,7 +5228,7 @@
       <c r="G21" s="34"/>
       <c r="H21" s="34"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B22" s="34"/>
       <c r="C22" s="34"/>
       <c r="D22" s="34"/>
@@ -5237,7 +5236,7 @@
       <c r="F22" s="34"/>
       <c r="G22" s="34"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B24" s="5"/>
     </row>
   </sheetData>
@@ -5286,19 +5285,19 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.47265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.80859375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -5339,19 +5338,19 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.47265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.80859375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -5390,18 +5389,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.80859375" customWidth="1"/>
-    <col min="3" max="3" width="69.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" customWidth="1"/>
+    <col min="3" max="3" width="69.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>129</v>
       </c>
@@ -5415,7 +5414,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -5429,7 +5428,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -5443,7 +5442,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -5457,7 +5456,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -5471,7 +5470,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -5485,7 +5484,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -5499,7 +5498,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -5513,7 +5512,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -5524,7 +5523,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -5535,7 +5534,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -5546,7 +5545,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -5557,7 +5556,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -5568,7 +5567,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>146</v>
       </c>
@@ -5579,7 +5578,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -5590,7 +5589,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -5601,7 +5600,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -5612,7 +5611,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -5623,7 +5622,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -5634,7 +5633,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -5645,7 +5644,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -5656,7 +5655,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -5667,7 +5666,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -5678,7 +5677,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -5689,7 +5688,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -5700,7 +5699,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>78</v>
       </c>
@@ -5711,7 +5710,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="85" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>161</v>
       </c>
@@ -5722,7 +5721,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>80</v>
       </c>
@@ -5733,7 +5732,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -5744,7 +5743,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -5758,7 +5757,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -5769,7 +5768,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -5780,7 +5779,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -5791,7 +5790,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>92</v>
       </c>
@@ -5802,7 +5801,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>171</v>
       </c>
@@ -5813,7 +5812,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>174</v>
       </c>
@@ -5824,7 +5823,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>177</v>
       </c>
@@ -5835,7 +5834,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>128</v>
       </c>
@@ -5846,7 +5845,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>94</v>
       </c>
@@ -5857,7 +5856,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>183</v>
       </c>
@@ -5868,7 +5867,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>186</v>
       </c>
@@ -5879,7 +5878,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>189</v>
       </c>
@@ -5890,7 +5889,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>192</v>
       </c>

</xml_diff>

<commit_message>
updated TeamReport to reflect completion of US12, US14
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rozanitis/Documents/Stevens/Semesters/Fall2018/SSW-555/gedcom-parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DE029E-1B35-564E-B78D-DCAEBCE91ADC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3728FBD9-C76A-934F-8F0C-EAD59D777DD4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24440" windowHeight="15240" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24440" windowHeight="15240" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -4869,7 +4869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96723CB6-6D85-DA4E-8BFC-88DDD98C4269}">
   <dimension ref="A1:Z24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5021,7 +5021,7 @@
         <v>2.5</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Z5" t="s">
         <v>119</v>
@@ -5038,7 +5038,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E6" s="19">
         <v>15</v>
@@ -5046,8 +5046,14 @@
       <c r="F6" s="19">
         <v>1.5</v>
       </c>
+      <c r="G6" s="20">
+        <v>20</v>
+      </c>
+      <c r="H6" s="20">
+        <v>1.5</v>
+      </c>
       <c r="I6" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
@@ -5143,11 +5149,11 @@
       </c>
       <c r="G10" s="20">
         <f>SUM(G2:G9)</f>
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="H10" s="20">
         <f>SUM(H2:H9)</f>
-        <v>10.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
@@ -5389,8 +5395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
completed sprint 3 stories selection, completed sprint planning.
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11014"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\Documents\GitHub\gedcom-parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/latinocodes/PycharmProjects/gedcom-parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{74320FBB-5F91-44C8-81C2-5D2FBF830D3D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{A84244B5-5935-4751-94BB-7E9D7952CD1A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFC62DA-6F95-8442-B4DE-8EB12411A8FC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="462" windowWidth="24438" windowHeight="15240" tabRatio="500" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24440" windowHeight="15240" tabRatio="500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -28,17 +28,12 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="219">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -712,6 +707,9 @@
   </si>
   <si>
     <t>All dates should be legitimate dates for the months specified (e.g., 2/30/2015 is not legitimate)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Avoid waiting until Tuesday for next sprint planning. </t>
   </si>
 </sst>
 </file>
@@ -722,7 +720,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -883,7 +881,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -939,7 +937,13 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -950,9 +954,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="68">
@@ -1566,7 +1567,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1637,7 +1638,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3329,17 +3330,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}"/>
+    <sheetView zoomScale="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5" customWidth="1"/>
     <col min="3" max="3" width="8.5" customWidth="1"/>
     <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3356,7 +3357,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.95">
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>5</v>
       </c>
@@ -3373,7 +3374,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.95">
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>10</v>
       </c>
@@ -3390,7 +3391,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.95">
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>15</v>
       </c>
@@ -3407,7 +3408,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.95">
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
@@ -3424,15 +3425,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
     </row>
   </sheetData>
   <sortState ref="A3:D5">
@@ -3454,20 +3455,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="150" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView topLeftCell="A11" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="4" customFormat="1">
+    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="25" t="s">
         <v>27</v>
       </c>
@@ -3484,7 +3485,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3498,7 +3499,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3515,7 +3516,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3532,7 +3533,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3549,7 +3550,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3566,7 +3567,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3583,7 +3584,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3600,7 +3601,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3617,7 +3618,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1</v>
       </c>
@@ -3634,7 +3635,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3651,7 +3652,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>1</v>
       </c>
@@ -3668,7 +3669,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>1</v>
       </c>
@@ -3685,7 +3686,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>1</v>
       </c>
@@ -3702,7 +3703,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2</v>
       </c>
@@ -3719,7 +3720,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="12.75">
+    <row r="16" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>2</v>
       </c>
@@ -3739,7 +3740,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2</v>
       </c>
@@ -3759,7 +3760,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2</v>
       </c>
@@ -3779,7 +3780,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2</v>
       </c>
@@ -3796,7 +3797,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>2</v>
       </c>
@@ -3813,7 +3814,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>2</v>
       </c>
@@ -3830,7 +3831,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>2</v>
       </c>
@@ -3847,7 +3848,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>3</v>
       </c>
@@ -3864,23 +3865,41 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>3</v>
+      </c>
       <c r="B24" t="s">
         <v>79</v>
       </c>
       <c r="C24" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="25" spans="1:25">
+      <c r="D24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>3</v>
+      </c>
       <c r="B25" t="s">
         <v>81</v>
       </c>
       <c r="C25" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="26" spans="1:25">
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B26" t="s">
         <v>83</v>
       </c>
@@ -3889,7 +3908,7 @@
       </c>
       <c r="D26" s="21"/>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>3</v>
       </c>
@@ -3906,7 +3925,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
         <v>87</v>
       </c>
@@ -3914,7 +3933,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>3</v>
       </c>
@@ -3931,7 +3950,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B30" t="s">
         <v>91</v>
       </c>
@@ -3940,7 +3959,7 @@
       </c>
       <c r="D30" s="21"/>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>3</v>
       </c>
@@ -3957,7 +3976,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>3</v>
       </c>
@@ -3974,7 +3993,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B33" t="s">
         <v>97</v>
       </c>
@@ -3982,7 +4001,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="12.75">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>3</v>
       </c>
@@ -4048,7 +4067,7 @@
       <formula>"Assigned"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17:E22">
+  <conditionalFormatting sqref="E17:E22 E24">
     <cfRule type="cellIs" dxfId="37" priority="16" operator="equal">
       <formula>$Y$18</formula>
     </cfRule>
@@ -4128,51 +4147,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="150" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
+    <sheetView topLeftCell="A4" zoomScale="150" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.75" style="2"/>
+    <col min="1" max="1" width="10.6640625" style="2"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.75" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>107</v>
       </c>
@@ -4195,7 +4214,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>114</v>
       </c>
@@ -4211,7 +4230,7 @@
       <c r="F15" s="11"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>115</v>
       </c>
@@ -4236,7 +4255,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>116</v>
       </c>
@@ -4261,7 +4280,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>117</v>
       </c>
@@ -4286,7 +4305,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>118</v>
       </c>
@@ -4322,21 +4341,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:G8"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="9.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" s="4" customFormat="1">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>107</v>
       </c>
@@ -4359,7 +4378,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1">
+    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -4374,7 +4393,7 @@
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>115</v>
       </c>
@@ -4400,7 +4419,7 @@
         <v>14.592592592592593</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>116</v>
       </c>
@@ -4426,7 +4445,7 @@
         <v>10.258064516129032</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>117</v>
       </c>
@@ -4434,7 +4453,7 @@
         <v>41941</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>118</v>
       </c>
@@ -4454,25 +4473,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B21" sqref="B21:H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
     <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.125" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.625" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.625" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.125" style="20" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -4501,7 +4520,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
         <v>35</v>
       </c>
@@ -4530,7 +4549,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="15" t="s">
         <v>37</v>
       </c>
@@ -4562,7 +4581,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="15" t="s">
         <v>39</v>
       </c>
@@ -4594,7 +4613,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="15" t="s">
         <v>41</v>
       </c>
@@ -4626,7 +4645,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="15" t="s">
         <v>43</v>
       </c>
@@ -4655,7 +4674,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="15" t="s">
         <v>45</v>
       </c>
@@ -4684,7 +4703,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="15" t="s">
         <v>47</v>
       </c>
@@ -4713,7 +4732,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="15" t="s">
         <v>53</v>
       </c>
@@ -4742,7 +4761,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>127</v>
       </c>
@@ -4755,115 +4774,115 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
-      <c r="B15" s="28" t="s">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="B15" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-    </row>
-    <row r="16" spans="1:26">
-      <c r="B16" s="28" t="s">
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="B16" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="B17" s="28" t="s">
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B17" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="B18" s="28" t="s">
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B18" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="B19" s="29" t="s">
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B19" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-    </row>
-    <row r="20" spans="1:9" ht="24.6">
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+    </row>
+    <row r="20" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="B20" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
-      <c r="B21" s="28" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B21" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="B22" s="28" t="s">
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B22" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B24" s="5"/>
     </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="31" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A26" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="B26" s="31"/>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="B26" s="29"/>
+    </row>
+    <row r="27" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
@@ -4892,7 +4911,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -4921,7 +4940,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -4950,7 +4969,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="15" t="s">
         <v>51</v>
       </c>
@@ -4979,7 +4998,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -5072,25 +5091,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96723CB6-6D85-DA4E-8BFC-88DDD98C4269}">
   <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{BA7E6921-9E23-5D53-A4E4-A351F9C68F3B}">
-      <selection activeCell="B17" sqref="B17:I17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
     <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.125" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.625" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.625" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.125" style="20" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>140</v>
       </c>
@@ -5119,7 +5138,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
         <v>59</v>
       </c>
@@ -5148,7 +5167,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="15" t="s">
         <v>61</v>
       </c>
@@ -5180,7 +5199,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="15" t="s">
         <v>64</v>
       </c>
@@ -5212,7 +5231,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="15" t="s">
         <v>67</v>
       </c>
@@ -5244,7 +5263,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="15" t="s">
         <v>69</v>
       </c>
@@ -5273,7 +5292,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="15" t="s">
         <v>71</v>
       </c>
@@ -5302,7 +5321,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="15" t="s">
         <v>73</v>
       </c>
@@ -5331,7 +5350,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="15" t="s">
         <v>75</v>
       </c>
@@ -5360,7 +5379,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>127</v>
       </c>
@@ -5373,68 +5392,68 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" ht="12.75">
+    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="12.4" customHeight="1">
-      <c r="B15" s="28" t="s">
+    <row r="15" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-    </row>
-    <row r="16" spans="1:26" ht="12.4" customHeight="1">
-      <c r="B16" s="28" t="s">
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+    </row>
+    <row r="16" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-    </row>
-    <row r="17" spans="2:9" ht="12.4" customHeight="1">
-      <c r="B17" s="28" t="s">
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+    </row>
+    <row r="17" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-    </row>
-    <row r="18" spans="2:9" ht="12.4" customHeight="1">
-      <c r="B18" s="28" t="s">
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+    </row>
+    <row r="18" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-    </row>
-    <row r="19" spans="2:9" ht="12.4" customHeight="1">
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+    </row>
+    <row r="19" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="26" t="s">
         <v>151</v>
       </c>
@@ -5446,47 +5465,46 @@
       <c r="H19" s="26"/>
       <c r="I19" s="26"/>
     </row>
-    <row r="20" spans="2:9" ht="12.4" customHeight="1">
-      <c r="B20" s="29" t="s">
+    <row r="20" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-    </row>
-    <row r="21" spans="2:9" ht="12.95" customHeight="1">
-      <c r="B21" s="30" t="s">
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+    </row>
+    <row r="21" spans="2:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="C21" s="30"/>
-    </row>
-    <row r="22" spans="2:9" ht="12.4" customHeight="1">
-      <c r="B22" s="28" t="s">
+      <c r="C21" s="32"/>
+    </row>
+    <row r="22" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-    </row>
-    <row r="23" spans="2:9" ht="12.4" customHeight="1">
-      <c r="B23" s="28" t="s">
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+    </row>
+    <row r="23" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-    </row>
-    <row r="24" spans="2:9" ht="12.75"/>
-    <row r="25" spans="2:9">
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B25" s="5"/>
     </row>
   </sheetData>
@@ -5531,27 +5549,27 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:Z24"/>
+  <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0" xr3:uid="{9B253EF2-77E0-53E3-AE26-4D66ECD923F3}">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
     <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.125" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.625" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.625" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.5" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.125" style="20" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>140</v>
       </c>
@@ -5580,7 +5598,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="12.75">
+    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
         <v>85</v>
       </c>
@@ -5603,7 +5621,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="12.75">
+    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="15" t="s">
         <v>89</v>
       </c>
@@ -5629,7 +5647,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="12.75">
+    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -5657,7 +5675,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="12.75">
+    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -5683,7 +5701,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="12.75">
+    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="15" t="s">
         <v>77</v>
       </c>
@@ -5706,7 +5724,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="12.75">
+    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="15" t="s">
         <v>99</v>
       </c>
@@ -5729,25 +5747,53 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="I8" s="24"/>
-    </row>
-    <row r="9" spans="1:26">
-      <c r="A9" s="15"/>
-      <c r="B9"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="I9" s="24"/>
-    </row>
-    <row r="10" spans="1:26">
+    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="18">
+        <v>25</v>
+      </c>
+      <c r="F8" s="18">
+        <v>2</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="A9" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="18">
+        <v>30</v>
+      </c>
+      <c r="F9" s="18">
+        <v>3</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>127</v>
       </c>
@@ -5760,108 +5806,144 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-    </row>
-    <row r="16" spans="1:26">
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-    </row>
-    <row r="17" spans="2:9">
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-    </row>
-    <row r="18" spans="2:9">
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-    </row>
-    <row r="19" spans="2:9">
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-    </row>
-    <row r="20" spans="2:9" ht="12.95" customHeight="1">
-      <c r="B20" s="30" t="s">
+    <row r="15" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+    </row>
+    <row r="16" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+    </row>
+    <row r="17" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+    </row>
+    <row r="18" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+    </row>
+    <row r="19" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+    </row>
+    <row r="20" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+    </row>
+    <row r="21" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+    </row>
+    <row r="22" spans="2:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="C20" s="30"/>
-    </row>
-    <row r="21" spans="2:9">
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-    </row>
-    <row r="22" spans="2:9">
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-    </row>
-    <row r="24" spans="2:9">
-      <c r="B24" s="5"/>
+      <c r="C22" s="32"/>
+    </row>
+    <row r="23" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="30" t="s">
+        <v>218</v>
+      </c>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B26" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B22:G22"/>
+  <mergeCells count="9">
     <mergeCell ref="B15:I15"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B24:G24"/>
     <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:I23"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="I1 I10:I11 I20:I1048576 D2:D9">
+  <conditionalFormatting sqref="I1 I10:I11 I22 D2:D9 I24:I1048576">
     <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>$Z$5</formula>
     </cfRule>
@@ -5880,8 +5962,8 @@
       <formula>NOT(ISERROR(SEARCH("No",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I20:I1048576 I10:I11 D2:D9" xr:uid="{A80F38BE-1FDE-425D-8913-2158C100C802}">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D9 I10:I11 I22 I24:I1048576" xr:uid="{A80F38BE-1FDE-425D-8913-2158C100C802}">
       <formula1>$Z$2:$Z$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -5894,21 +5976,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0" xr3:uid="{85D5C41F-068E-5C55-9968-509E7C2A5619}"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -5947,18 +6029,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0" xr3:uid="{44B22561-5205-5C8A-B808-2C70100D228F}">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.75" customWidth="1"/>
-    <col min="3" max="3" width="69.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="69.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>140</v>
       </c>
@@ -5972,7 +6054,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -5986,7 +6068,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -6000,7 +6082,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -6014,7 +6096,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30">
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -6028,7 +6110,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -6042,7 +6124,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -6056,7 +6138,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30">
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -6070,7 +6152,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30">
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -6081,7 +6163,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30">
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -6092,7 +6174,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30">
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>64</v>
       </c>
@@ -6103,7 +6185,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15">
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>167</v>
       </c>
@@ -6114,7 +6196,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30">
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -6125,7 +6207,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="45">
+    <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>171</v>
       </c>
@@ -6136,7 +6218,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15">
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -6147,7 +6229,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15">
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -6158,7 +6240,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15">
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -6169,7 +6251,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15">
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>177</v>
       </c>
@@ -6180,7 +6262,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15">
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -6191,7 +6273,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15">
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>81</v>
       </c>
@@ -6202,7 +6284,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15">
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -6213,7 +6295,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15">
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>85</v>
       </c>
@@ -6227,7 +6309,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15">
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -6238,7 +6320,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30">
+    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>99</v>
       </c>
@@ -6249,7 +6331,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30">
+    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>87</v>
       </c>
@@ -6260,7 +6342,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30">
+    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>89</v>
       </c>
@@ -6274,7 +6356,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="75">
+    <row r="27" spans="1:4" ht="85" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>189</v>
       </c>
@@ -6285,7 +6367,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15">
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -6296,7 +6378,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15">
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>91</v>
       </c>
@@ -6307,7 +6389,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15">
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -6321,7 +6403,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15">
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -6332,7 +6414,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15">
+    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>93</v>
       </c>
@@ -6346,7 +6428,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15">
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>95</v>
       </c>
@@ -6360,7 +6442,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30">
+    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>97</v>
       </c>
@@ -6371,7 +6453,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30">
+    <row r="35" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>199</v>
       </c>
@@ -6382,7 +6464,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15">
+    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -6393,7 +6475,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15">
+    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -6404,7 +6486,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30">
+    <row r="38" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>73</v>
       </c>
@@ -6415,7 +6497,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15">
+    <row r="39" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -6426,7 +6508,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30">
+    <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>206</v>
       </c>
@@ -6437,7 +6519,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15">
+    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>209</v>
       </c>
@@ -6448,7 +6530,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15">
+    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>212</v>
       </c>
@@ -6459,7 +6541,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30">
+    <row r="43" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>215</v>
       </c>

</xml_diff>

<commit_message>
Team Report updated with updated backlog
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\Documents\GitHub\gedcom-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E1E482-7462-4CA7-A29F-E7A840C7AD2E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B106A8CE-5E77-4DCA-89E7-0ED7EE44F8BB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="462" windowWidth="24438" windowHeight="15240" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="462" windowWidth="24438" windowHeight="15240" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="222">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1043,7 +1043,67 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="66" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
   </cellStyles>
-  <dxfs count="50">
+  <dxfs count="56">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3470,10 +3530,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Y34"/>
+  <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -3917,37 +3977,54 @@
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A26">
+        <v>3</v>
+      </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C26" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" s="21"/>
+        <v>86</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
-      </c>
-      <c r="D27" s="21" t="s">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="D27" t="s">
+        <v>20</v>
       </c>
       <c r="E27" s="23" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A28">
+        <v>3</v>
+      </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C28" t="s">
-        <v>88</v>
+        <v>90</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.4">
@@ -3955,136 +4032,173 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E29" s="23" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A30">
+        <v>3</v>
+      </c>
       <c r="B30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B31" t="s">
+        <v>169</v>
+      </c>
+      <c r="C31" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="21"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B33" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B34" t="s">
         <v>91</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C34" t="s">
         <v>92</v>
       </c>
-      <c r="D30" s="21"/>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A31">
-        <v>3</v>
-      </c>
-      <c r="B31" t="s">
-        <v>93</v>
-      </c>
-      <c r="C31" t="s">
-        <v>94</v>
-      </c>
-      <c r="D31" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E31" s="23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A32">
-        <v>3</v>
-      </c>
-      <c r="B32" t="s">
-        <v>95</v>
-      </c>
-      <c r="C32" t="s">
-        <v>96</v>
-      </c>
-      <c r="D32" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E32" s="23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B33" t="s">
+      <c r="D34" s="21"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B35" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B36" t="s">
         <v>97</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C36" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A34">
-        <v>3</v>
-      </c>
-      <c r="B34" t="s">
-        <v>99</v>
-      </c>
-      <c r="C34" t="s">
-        <v>100</v>
-      </c>
-      <c r="D34" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34" s="23" t="s">
-        <v>63</v>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B37" t="s">
+        <v>197</v>
+      </c>
+      <c r="C37" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B38" t="s">
+        <v>204</v>
+      </c>
+      <c r="C38" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:E33">
+  <sortState ref="A2:E38">
     <sortCondition ref="A2"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="E2:E16">
-    <cfRule type="cellIs" dxfId="49" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="46" operator="equal">
       <formula>$Y$18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="47" operator="equal">
       <formula>$Y$17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="48" operator="equal">
       <formula>$Y$16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25:E26">
-    <cfRule type="cellIs" dxfId="46" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="43" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="44" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="45" operator="equal">
       <formula>"Assigned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="cellIs" dxfId="43" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="34" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="35" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="36" operator="equal">
       <formula>"Assigned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="40" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="28" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="29" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="30" operator="equal">
       <formula>"Assigned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17:E22 E24">
+    <cfRule type="cellIs" dxfId="43" priority="22" operator="equal">
+      <formula>$Y$18</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="23" operator="equal">
+      <formula>$Y$17</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="24" operator="equal">
+      <formula>$Y$16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="cellIs" dxfId="40" priority="19" operator="equal">
+      <formula>$Y$18</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="20" operator="equal">
+      <formula>$Y$17</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="21" operator="equal">
+      <formula>$Y$16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29">
     <cfRule type="cellIs" dxfId="37" priority="16" operator="equal">
       <formula>$Y$18</formula>
     </cfRule>
@@ -4095,7 +4209,7 @@
       <formula>$Y$16</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
+  <conditionalFormatting sqref="E31">
     <cfRule type="cellIs" dxfId="34" priority="13" operator="equal">
       <formula>$Y$18</formula>
     </cfRule>
@@ -4106,7 +4220,7 @@
       <formula>$Y$16</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
+  <conditionalFormatting sqref="E32">
     <cfRule type="cellIs" dxfId="31" priority="10" operator="equal">
       <formula>$Y$18</formula>
     </cfRule>
@@ -4117,7 +4231,7 @@
       <formula>$Y$16</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
+  <conditionalFormatting sqref="E34">
     <cfRule type="cellIs" dxfId="28" priority="7" operator="equal">
       <formula>$Y$18</formula>
     </cfRule>
@@ -4128,25 +4242,25 @@
       <formula>$Y$16</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
+  <conditionalFormatting sqref="E30">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>$Y$18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>$Y$17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>$Y$16</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E34">
-    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
+  <conditionalFormatting sqref="E28">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>$Y$18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>$Y$17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>$Y$16</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5057,40 +5171,40 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I20:I26 I1 I10:I11 D2:D9 I32:I1048576 D28:D31">
-    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="8" operator="equal">
       <formula>$Z$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="9" operator="equal">
       <formula>$Z$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="10" operator="equal">
       <formula>$Z$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27">
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="5" operator="equal">
       <formula>$Z$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="6" operator="equal">
       <formula>$Z$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
       <formula>$Z$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I9">
-    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="19" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="18" priority="4" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28:I31">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",I28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I28)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5108,7 +5222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96723CB6-6D85-DA4E-8BFC-88DDD98C4269}">
   <dimension ref="A1:Z27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -5519,21 +5633,21 @@
     <mergeCell ref="B21:H21"/>
   </mergeCells>
   <conditionalFormatting sqref="I1 I10:I11 I23:I1048576 D2:D9">
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
       <formula>$Z$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
       <formula>$Z$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
       <formula>$Z$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I9">
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5930,21 +6044,21 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I1 I10:I11 I22 D2:D9 I24:I1048576">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>$Z$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>$Z$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>$Z$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I9">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6015,8 +6129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
app.py updated to match output
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\Documents\GitHub\gedcom-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B106A8CE-5E77-4DCA-89E7-0ED7EE44F8BB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C89A244-3639-489D-8778-1148142399E3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="462" windowWidth="24438" windowHeight="15240" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="462" windowWidth="24438" windowHeight="15240" tabRatio="500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="223">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -724,6 +724,9 @@
   </si>
   <si>
     <t>1) Avoid waiting until Tuesday for next sprint planning and sprint retrospective.</t>
+  </si>
+  <si>
+    <t>complete</t>
   </si>
 </sst>
 </file>
@@ -1056,16 +1059,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1186,6 +1179,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1216,21 +1229,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3532,7 +3535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScale="150" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -4243,24 +4246,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
       <formula>$Y$18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
       <formula>$Y$17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
       <formula>$Y$16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
       <formula>$Y$18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
       <formula>$Y$17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
       <formula>$Y$16</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5171,40 +5174,40 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I20:I26 I1 I10:I11 D2:D9 I32:I1048576 D28:D31">
-    <cfRule type="cellIs" dxfId="25" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
       <formula>$Z$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
       <formula>$Z$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
       <formula>$Z$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27">
-    <cfRule type="cellIs" dxfId="22" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>$Z$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>$Z$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>$Z$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I9">
-    <cfRule type="containsText" dxfId="19" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="4" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28:I31">
-    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",I28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I28)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5633,21 +5636,21 @@
     <mergeCell ref="B21:H21"/>
   </mergeCells>
   <conditionalFormatting sqref="I1 I10:I11 I23:I1048576 D2:D9">
-    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>$Z$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>$Z$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>$Z$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I9">
-    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5665,8 +5668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -5772,7 +5775,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>63</v>
+        <v>222</v>
       </c>
       <c r="E4" s="18">
         <v>25</v>
@@ -5780,10 +5783,14 @@
       <c r="F4" s="18">
         <v>2</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
+      <c r="G4" s="18">
+        <v>14</v>
+      </c>
+      <c r="H4" s="18">
+        <v>1</v>
+      </c>
       <c r="I4" s="23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="Z4" t="s">
         <v>66</v>
@@ -5913,11 +5920,11 @@
       </c>
       <c r="G10" s="19">
         <f>SUM(G2:G9)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H10" s="19">
         <f>SUM(H2:H9)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.4">
@@ -6044,25 +6051,25 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I1 I10:I11 I22 D2:D9 I24:I1048576">
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>$Z$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>$Z$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>$Z$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I9">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D9 I10:I11 I22 I24:I1048576" xr:uid="{A80F38BE-1FDE-425D-8913-2158C100C802}">
       <formula1>$Z$2:$Z$5</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
updated tab for sprint 3 and sprint 4
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10909"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\Documents\GitHub\gedcom-parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rozanitis/Documents/Stevens/Semesters/Fall2018/SSW-555/gedcom-parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284C4E2D-411A-414D-859A-DE3FD42CC81B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCF69D1-E65D-3747-9FE8-9793920EA02D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="462" windowWidth="24438" windowHeight="15240" tabRatio="500" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24440" windowHeight="15240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -28,17 +28,12 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="223">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1046,7 +1041,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="66" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
   </cellStyles>
-  <dxfs count="61">
+  <dxfs count="106">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1069,6 +1074,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1079,6 +1104,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -1109,6 +1144,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1159,6 +1214,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1209,6 +1274,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1229,6 +1304,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1329,6 +1414,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1584,6 +1689,346 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1697,7 +2142,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1768,7 +2213,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3463,17 +3908,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.47265625" customWidth="1"/>
-    <col min="3" max="3" width="8.47265625" customWidth="1"/>
-    <col min="4" max="5" width="20.47265625" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3490,7 +3935,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>5</v>
       </c>
@@ -3507,7 +3952,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>10</v>
       </c>
@@ -3524,7 +3969,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>15</v>
       </c>
@@ -3541,7 +3986,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>20</v>
       </c>
@@ -3558,7 +4003,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
@@ -3588,20 +4033,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y37"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:C31"/>
-    </sheetView>
+    <sheetView zoomScale="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.47265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
@@ -3618,7 +4061,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3632,7 +4075,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3649,7 +4092,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3666,7 +4109,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3683,7 +4126,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3700,7 +4143,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3717,7 +4160,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3734,7 +4177,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3751,7 +4194,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1</v>
       </c>
@@ -3768,7 +4211,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3785,7 +4228,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>1</v>
       </c>
@@ -3802,7 +4245,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>1</v>
       </c>
@@ -3819,7 +4262,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>1</v>
       </c>
@@ -3836,7 +4279,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2</v>
       </c>
@@ -3853,7 +4296,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>2</v>
       </c>
@@ -3873,7 +4316,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2</v>
       </c>
@@ -3893,7 +4336,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2</v>
       </c>
@@ -3913,7 +4356,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2</v>
       </c>
@@ -3930,7 +4373,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>2</v>
       </c>
@@ -3947,7 +4390,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>2</v>
       </c>
@@ -3964,7 +4407,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>2</v>
       </c>
@@ -3981,7 +4424,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>3</v>
       </c>
@@ -3998,7 +4441,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>3</v>
       </c>
@@ -4015,7 +4458,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>3</v>
       </c>
@@ -4032,7 +4475,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>3</v>
       </c>
@@ -4046,10 +4489,10 @@
         <v>10</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>3</v>
       </c>
@@ -4066,7 +4509,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>3</v>
       </c>
@@ -4083,7 +4526,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>3</v>
       </c>
@@ -4100,7 +4543,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>3</v>
       </c>
@@ -4117,15 +4560,24 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A31">
+        <v>4</v>
+      </c>
       <c r="B31" t="s">
         <v>169</v>
       </c>
       <c r="C31" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="D31" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
         <v>83</v>
       </c>
@@ -4134,32 +4586,58 @@
       </c>
       <c r="D32" s="20"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A33">
+        <v>4</v>
+      </c>
       <c r="B33" t="s">
         <v>87</v>
       </c>
       <c r="C33" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D33" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A34">
+        <v>4</v>
+      </c>
       <c r="B34" t="s">
         <v>91</v>
       </c>
       <c r="C34" t="s">
         <v>92</v>
       </c>
-      <c r="D34" s="20"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D34" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A35">
+        <v>4</v>
+      </c>
       <c r="B35" t="s">
         <v>97</v>
       </c>
       <c r="C35" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D35" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>4</v>
       </c>
@@ -4169,8 +4647,14 @@
       <c r="C36" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>4</v>
       </c>
@@ -4179,6 +4663,12 @@
       </c>
       <c r="C37" t="s">
         <v>205</v>
+      </c>
+      <c r="D37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -4186,136 +4676,15 @@
     <sortCondition ref="A2"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="E2:E16">
-    <cfRule type="cellIs" dxfId="60" priority="46" operator="equal">
-      <formula>$Y$18</formula>
+  <conditionalFormatting sqref="E2:E50">
+    <cfRule type="cellIs" dxfId="5" priority="48" operator="equal">
+      <formula>$Y$16</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="47" operator="equal">
       <formula>$Y$17</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="48" operator="equal">
-      <formula>$Y$16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25:E26">
-    <cfRule type="cellIs" dxfId="57" priority="43" operator="equal">
-      <formula>"Complete"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="44" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="45" operator="equal">
-      <formula>"Assigned"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E33">
-    <cfRule type="cellIs" dxfId="54" priority="34" operator="equal">
-      <formula>"Complete"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="35" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="36" operator="equal">
-      <formula>"Assigned"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="51" priority="28" operator="equal">
-      <formula>"Complete"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="29" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="30" operator="equal">
-      <formula>"Assigned"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E17:E22 E24">
-    <cfRule type="cellIs" dxfId="48" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="46" operator="equal">
       <formula>$Y$18</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="23" operator="equal">
-      <formula>$Y$17</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="24" operator="equal">
-      <formula>$Y$16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
-    <cfRule type="cellIs" dxfId="45" priority="19" operator="equal">
-      <formula>$Y$18</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="20" operator="equal">
-      <formula>$Y$17</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="21" operator="equal">
-      <formula>$Y$16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="42" priority="16" operator="equal">
-      <formula>$Y$18</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="17" operator="equal">
-      <formula>$Y$17</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="18" operator="equal">
-      <formula>$Y$16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" dxfId="39" priority="13" operator="equal">
-      <formula>$Y$18</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="14" operator="equal">
-      <formula>$Y$17</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="15" operator="equal">
-      <formula>$Y$16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="36" priority="10" operator="equal">
-      <formula>$Y$18</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="11" operator="equal">
-      <formula>$Y$17</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="12" operator="equal">
-      <formula>$Y$16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E34">
-    <cfRule type="cellIs" dxfId="33" priority="7" operator="equal">
-      <formula>$Y$18</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="8" operator="equal">
-      <formula>$Y$17</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="9" operator="equal">
-      <formula>$Y$16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
-      <formula>$Y$18</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="5" operator="equal">
-      <formula>$Y$17</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="6" operator="equal">
-      <formula>$Y$16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E28">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
-      <formula>$Y$18</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
-      <formula>$Y$17</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
-      <formula>$Y$16</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -4332,51 +4701,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="150" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
-    </sheetView>
+    <sheetView zoomScale="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="2"/>
-    <col min="2" max="2" width="9.47265625" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
     <col min="5" max="5" width="6.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.47265625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>107</v>
       </c>
@@ -4399,7 +4766,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>114</v>
       </c>
@@ -4415,7 +4782,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>115</v>
       </c>
@@ -4440,7 +4807,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>116</v>
       </c>
@@ -4465,7 +4832,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>117</v>
       </c>
@@ -4490,7 +4857,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>118</v>
       </c>
@@ -4526,21 +4893,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:G8"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView zoomScale="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="9.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>107</v>
       </c>
@@ -4563,7 +4928,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -4578,7 +4943,7 @@
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>115</v>
       </c>
@@ -4604,7 +4969,7 @@
         <v>14.592592592592593</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>116</v>
       </c>
@@ -4630,7 +4995,7 @@
         <v>10.258064516129032</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>117</v>
       </c>
@@ -4645,18 +5010,18 @@
       </c>
       <c r="E7">
         <f>Sprint3!G10</f>
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="F7">
         <f>(Sprint3!H10*60)</f>
-        <v>420</v>
+        <v>510</v>
       </c>
       <c r="G7" s="7">
         <f>E7/(F7/60)</f>
-        <v>14.428571428571429</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+        <v>12.941176470588236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>118</v>
       </c>
@@ -4676,25 +5041,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:H22"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.47265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="19" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -4723,7 +5086,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
@@ -4752,7 +5115,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
         <v>37</v>
       </c>
@@ -4784,7 +5147,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
         <v>39</v>
       </c>
@@ -4816,7 +5179,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
         <v>41</v>
       </c>
@@ -4848,7 +5211,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
@@ -4877,7 +5240,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
         <v>45</v>
       </c>
@@ -4906,7 +5269,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="14" t="s">
         <v>47</v>
       </c>
@@ -4935,7 +5298,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>53</v>
       </c>
@@ -4964,7 +5327,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>127</v>
       </c>
@@ -4977,20 +5340,20 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B15" s="31" t="s">
         <v>130</v>
       </c>
@@ -5002,7 +5365,7 @@
       <c r="H15" s="31"/>
       <c r="I15" s="31"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B16" s="31" t="s">
         <v>131</v>
       </c>
@@ -5014,7 +5377,7 @@
       <c r="H16" s="31"/>
       <c r="I16" s="31"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B17" s="31" t="s">
         <v>132</v>
       </c>
@@ -5026,7 +5389,7 @@
       <c r="H17" s="31"/>
       <c r="I17" s="31"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B18" s="31" t="s">
         <v>133</v>
       </c>
@@ -5038,7 +5401,7 @@
       <c r="H18" s="31"/>
       <c r="I18" s="31"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B19" s="32" t="s">
         <v>134</v>
       </c>
@@ -5050,12 +5413,12 @@
       <c r="H19" s="32"/>
       <c r="I19" s="32"/>
     </row>
-    <row r="20" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="B20" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B21" s="31" t="s">
         <v>136</v>
       </c>
@@ -5066,7 +5429,7 @@
       <c r="G21" s="31"/>
       <c r="H21" s="31"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B22" s="31" t="s">
         <v>137</v>
       </c>
@@ -5076,16 +5439,16 @@
       <c r="F22" s="31"/>
       <c r="G22" s="31"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B24" s="5"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="30" t="s">
         <v>138</v>
       </c>
       <c r="B26" s="30"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
@@ -5114,7 +5477,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -5143,7 +5506,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -5172,7 +5535,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="14" t="s">
         <v>51</v>
       </c>
@@ -5201,7 +5564,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -5243,40 +5606,40 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I20:I26 I1 I10:I11 D2:D9 I32:I1048576 D28:D31">
-    <cfRule type="cellIs" dxfId="24" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="8" operator="equal">
       <formula>$Z$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="9" operator="equal">
       <formula>$Z$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="10" operator="equal">
       <formula>$Z$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27">
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="5" operator="equal">
       <formula>$Z$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="6" operator="equal">
       <formula>$Z$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="7" operator="equal">
       <formula>$Z$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I9">
-    <cfRule type="containsText" dxfId="18" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="99" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="98" priority="4" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28:I31">
-    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="97" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",I28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="96" priority="2" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I28)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5294,25 +5657,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96723CB6-6D85-DA4E-8BFC-88DDD98C4269}">
   <dimension ref="A1:Z27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.47265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="19" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>140</v>
       </c>
@@ -5341,7 +5702,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
         <v>59</v>
       </c>
@@ -5370,7 +5731,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
         <v>61</v>
       </c>
@@ -5402,7 +5763,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
         <v>64</v>
       </c>
@@ -5434,7 +5795,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
         <v>67</v>
       </c>
@@ -5466,7 +5827,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="14" t="s">
         <v>69</v>
       </c>
@@ -5495,7 +5856,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
         <v>71</v>
       </c>
@@ -5524,7 +5885,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="14" t="s">
         <v>73</v>
       </c>
@@ -5553,7 +5914,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>75</v>
       </c>
@@ -5582,7 +5943,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>127</v>
       </c>
@@ -5595,20 +5956,20 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="31" t="s">
         <v>217</v>
       </c>
@@ -5620,7 +5981,7 @@
       <c r="H15" s="31"/>
       <c r="I15" s="31"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B16" s="31" t="s">
         <v>218</v>
       </c>
@@ -5632,7 +5993,7 @@
       <c r="H16" s="31"/>
       <c r="I16" s="31"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B17" s="31" t="s">
         <v>219</v>
       </c>
@@ -5644,7 +6005,7 @@
       <c r="H17" s="31"/>
       <c r="I17" s="25"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B18" s="31" t="s">
         <v>220</v>
       </c>
@@ -5656,13 +6017,13 @@
       <c r="H18" s="32"/>
       <c r="I18" s="32"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B20" s="33" t="s">
         <v>135</v>
       </c>
       <c r="C20" s="33"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B21" s="31" t="s">
         <v>221</v>
       </c>
@@ -5673,7 +6034,7 @@
       <c r="G21" s="31"/>
       <c r="H21" s="31"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B22" s="27"/>
       <c r="C22" s="27"/>
       <c r="D22" s="27"/>
@@ -5683,7 +6044,7 @@
       <c r="H22" s="27"/>
       <c r="I22" s="27"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B25" s="31"/>
       <c r="C25" s="31"/>
       <c r="D25" s="31"/>
@@ -5691,7 +6052,7 @@
       <c r="F25" s="31"/>
       <c r="G25" s="31"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B27" s="5"/>
     </row>
   </sheetData>
@@ -5705,21 +6066,21 @@
     <mergeCell ref="B21:H21"/>
   </mergeCells>
   <conditionalFormatting sqref="I1 I10:I11 I23:I1048576 D2:D9">
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="8" operator="equal">
       <formula>$Z$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="9" operator="equal">
       <formula>$Z$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="10" operator="equal">
       <formula>$Z$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I9">
-    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="92" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="91" priority="4" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5737,25 +6098,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.47265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="19" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>140</v>
       </c>
@@ -5784,7 +6143,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
         <v>85</v>
       </c>
@@ -5795,7 +6154,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="E2" s="17">
         <v>15</v>
@@ -5803,11 +6162,17 @@
       <c r="F2" s="17">
         <v>1.5</v>
       </c>
+      <c r="G2" s="18">
+        <v>9</v>
+      </c>
+      <c r="H2" s="18">
+        <v>1.5</v>
+      </c>
       <c r="I2" s="22" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
         <v>89</v>
       </c>
@@ -5833,7 +6198,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -5865,7 +6230,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -5897,7 +6262,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="14" t="s">
         <v>77</v>
       </c>
@@ -5920,7 +6285,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
         <v>99</v>
       </c>
@@ -5943,7 +6308,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -5972,7 +6337,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>213</v>
       </c>
@@ -6001,33 +6366,33 @@
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>127</v>
       </c>
       <c r="G10" s="18">
         <f>SUM(G2:G9)</f>
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="H10" s="18">
         <f>SUM(H2:H9)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="31"/>
       <c r="C15" s="31"/>
       <c r="D15" s="31"/>
@@ -6037,7 +6402,7 @@
       <c r="H15" s="31"/>
       <c r="I15" s="31"/>
     </row>
-    <row r="16" spans="1:26" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="31"/>
       <c r="C16" s="31"/>
       <c r="D16" s="31"/>
@@ -6047,7 +6412,7 @@
       <c r="H16" s="31"/>
       <c r="I16" s="31"/>
     </row>
-    <row r="17" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="31"/>
       <c r="C17" s="31"/>
       <c r="D17" s="31"/>
@@ -6057,7 +6422,7 @@
       <c r="H17" s="31"/>
       <c r="I17" s="31"/>
     </row>
-    <row r="18" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="31"/>
       <c r="C18" s="31"/>
       <c r="D18" s="31"/>
@@ -6067,7 +6432,7 @@
       <c r="H18" s="31"/>
       <c r="I18" s="31"/>
     </row>
-    <row r="19" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
@@ -6077,7 +6442,7 @@
       <c r="H19" s="26"/>
       <c r="I19" s="26"/>
     </row>
-    <row r="20" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="32"/>
       <c r="C20" s="32"/>
       <c r="D20" s="32"/>
@@ -6087,7 +6452,7 @@
       <c r="H20" s="32"/>
       <c r="I20" s="32"/>
     </row>
-    <row r="21" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
       <c r="D21" s="32"/>
@@ -6097,13 +6462,13 @@
       <c r="H21" s="32"/>
       <c r="I21" s="32"/>
     </row>
-    <row r="22" spans="2:9" ht="13" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="33" t="s">
         <v>135</v>
       </c>
       <c r="C22" s="33"/>
     </row>
-    <row r="23" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="31"/>
       <c r="C23" s="31"/>
       <c r="D23" s="31"/>
@@ -6113,7 +6478,7 @@
       <c r="H23" s="31"/>
       <c r="I23" s="31"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B24" s="31"/>
       <c r="C24" s="31"/>
       <c r="D24" s="31"/>
@@ -6121,7 +6486,7 @@
       <c r="F24" s="31"/>
       <c r="G24" s="31"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B26" s="5"/>
     </row>
   </sheetData>
@@ -6138,21 +6503,21 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I1 I10:I11 I22 D2:D9 I24:I1048576">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="3" operator="equal">
       <formula>$Z$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="4" operator="equal">
       <formula>$Z$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="5" operator="equal">
       <formula>$Z$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I9">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="87" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="86" priority="2" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6170,25 +6535,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.47265625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="18" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="19" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>140</v>
       </c>
@@ -6217,32 +6582,48 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="A2" s="14"/>
-      <c r="B2"/>
+    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="A2" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
       <c r="C2" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="E2" s="17">
+        <v>10</v>
+      </c>
+      <c r="F2" s="17">
+        <v>1.5</v>
+      </c>
       <c r="I2" s="22" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="A3" s="14"/>
-      <c r="B3"/>
+    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" t="s">
+        <v>92</v>
+      </c>
       <c r="C3" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
+      <c r="E3" s="17">
+        <v>20</v>
+      </c>
+      <c r="F3" s="17">
+        <v>2</v>
+      </c>
       <c r="I3" s="22" t="s">
         <v>151</v>
       </c>
@@ -6250,7 +6631,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>169</v>
       </c>
@@ -6278,7 +6659,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>97</v>
       </c>
@@ -6304,7 +6685,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="C6" s="17" t="s">
         <v>20</v>
       </c>
@@ -6317,7 +6698,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="C7" s="17" t="s">
         <v>20</v>
       </c>
@@ -6330,7 +6711,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>197</v>
       </c>
@@ -6353,7 +6734,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>204</v>
       </c>
@@ -6376,7 +6757,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>127</v>
       </c>
@@ -6389,20 +6770,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="31"/>
       <c r="C15" s="31"/>
       <c r="D15" s="31"/>
@@ -6412,7 +6793,7 @@
       <c r="H15" s="31"/>
       <c r="I15" s="31"/>
     </row>
-    <row r="16" spans="1:26" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="31"/>
       <c r="C16" s="31"/>
       <c r="D16" s="31"/>
@@ -6422,7 +6803,7 @@
       <c r="H16" s="31"/>
       <c r="I16" s="31"/>
     </row>
-    <row r="17" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="31"/>
       <c r="C17" s="31"/>
       <c r="D17" s="31"/>
@@ -6432,7 +6813,7 @@
       <c r="H17" s="31"/>
       <c r="I17" s="31"/>
     </row>
-    <row r="18" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="31"/>
       <c r="C18" s="31"/>
       <c r="D18" s="31"/>
@@ -6442,7 +6823,7 @@
       <c r="H18" s="31"/>
       <c r="I18" s="31"/>
     </row>
-    <row r="19" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="28"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
@@ -6452,7 +6833,7 @@
       <c r="H19" s="28"/>
       <c r="I19" s="28"/>
     </row>
-    <row r="20" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="32"/>
       <c r="C20" s="32"/>
       <c r="D20" s="32"/>
@@ -6462,7 +6843,7 @@
       <c r="H20" s="32"/>
       <c r="I20" s="32"/>
     </row>
-    <row r="21" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
       <c r="D21" s="32"/>
@@ -6472,13 +6853,13 @@
       <c r="H21" s="32"/>
       <c r="I21" s="32"/>
     </row>
-    <row r="22" spans="2:9" ht="13" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="33" t="s">
         <v>135</v>
       </c>
       <c r="C22" s="33"/>
     </row>
-    <row r="23" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="31"/>
       <c r="C23" s="31"/>
       <c r="D23" s="31"/>
@@ -6488,7 +6869,7 @@
       <c r="H23" s="31"/>
       <c r="I23" s="31"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B24" s="31"/>
       <c r="C24" s="31"/>
       <c r="D24" s="31"/>
@@ -6496,7 +6877,7 @@
       <c r="F24" s="31"/>
       <c r="G24" s="31"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B26" s="5"/>
     </row>
   </sheetData>
@@ -6513,21 +6894,21 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I1 I10:I11 I22 I24:I1048576 D2:D9">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="3" operator="equal">
       <formula>$Z$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="4" operator="equal">
       <formula>$Z$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="5" operator="equal">
       <formula>$Z$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I9">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="82" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="81" priority="2" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6544,18 +6925,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.6640625" customWidth="1"/>
-    <col min="3" max="3" width="69.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="69.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>140</v>
       </c>
@@ -6569,7 +6948,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -6583,7 +6962,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -6597,7 +6976,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -6611,7 +6990,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -6625,7 +7004,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -6639,7 +7018,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -6653,7 +7032,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -6667,7 +7046,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -6678,7 +7057,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -6689,7 +7068,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>64</v>
       </c>
@@ -6700,7 +7079,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>165</v>
       </c>
@@ -6711,7 +7090,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -6722,7 +7101,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>169</v>
       </c>
@@ -6733,7 +7112,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -6744,7 +7123,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -6755,7 +7134,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -6766,7 +7145,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>175</v>
       </c>
@@ -6777,7 +7156,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -6788,7 +7167,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>81</v>
       </c>
@@ -6799,7 +7178,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -6810,7 +7189,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>85</v>
       </c>
@@ -6824,7 +7203,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -6835,7 +7214,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>99</v>
       </c>
@@ -6846,7 +7225,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>87</v>
       </c>
@@ -6857,7 +7236,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>89</v>
       </c>
@@ -6871,7 +7250,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="85" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>187</v>
       </c>
@@ -6882,7 +7261,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -6893,7 +7272,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>91</v>
       </c>
@@ -6904,7 +7283,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -6918,7 +7297,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -6929,7 +7308,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>93</v>
       </c>
@@ -6943,7 +7322,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>95</v>
       </c>
@@ -6957,7 +7336,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>97</v>
       </c>
@@ -6968,7 +7347,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>197</v>
       </c>
@@ -6979,7 +7358,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -6990,7 +7369,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -7001,7 +7380,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>73</v>
       </c>
@@ -7012,7 +7391,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -7023,7 +7402,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>204</v>
       </c>
@@ -7034,7 +7413,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>207</v>
       </c>
@@ -7045,7 +7424,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>210</v>
       </c>
@@ -7056,7 +7435,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>213</v>
       </c>

</xml_diff>

<commit_message>
added more things to continue to do
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rozanitis/Documents/Stevens/Semesters/Fall2018/SSW-555/gedcom-parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4D8F76-638C-404C-8C91-05DE70A9EB9A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E1628F-A70C-AC48-A33E-40D8598F25A2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="24440" windowHeight="15240" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="230">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -740,6 +740,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>6. Continue to discuss any issues with the group to come up with a solution rather than spending more time to solve it on your own.</t>
   </si>
 </sst>
 </file>
@@ -976,6 +979,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -991,16 +995,15 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="68">
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
@@ -3258,11 +3261,11 @@
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
     </row>
   </sheetData>
   <sortState ref="A3:D5">
@@ -4630,64 +4633,64 @@
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="30" t="s">
         <v>139</v>
       </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
     </row>
     <row r="20" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="B20" s="5" t="s">
@@ -4695,34 +4698,34 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B24" s="5"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="B26" s="28"/>
+      <c r="B26" s="29"/>
     </row>
     <row r="27" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
@@ -5246,69 +5249,69 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
       <c r="I17" s="25"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="C20" s="31"/>
+      <c r="C20" s="32"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B22" s="26"/>
@@ -5321,12 +5324,12 @@
       <c r="I22" s="26"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B27" s="5"/>
@@ -5682,166 +5685,170 @@
       <c r="B13" s="5"/>
     </row>
     <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
-      <c r="A14" s="35"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="5" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="30" t="s">
         <v>221</v>
       </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
     </row>
     <row r="16" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="35" t="s">
         <v>223</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-    </row>
-    <row r="17" spans="2:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="32" t="s">
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+    </row>
+    <row r="17" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-    </row>
-    <row r="18" spans="2:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="32" t="s">
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+    </row>
+    <row r="18" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-    </row>
-    <row r="19" spans="2:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="32" t="s">
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+    </row>
+    <row r="19" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-    </row>
-    <row r="20" spans="2:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-    </row>
-    <row r="21" spans="2:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-    </row>
-    <row r="22" spans="2:10" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="31" t="s">
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+    </row>
+    <row r="20" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+    </row>
+    <row r="21" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+    </row>
+    <row r="22" spans="2:12" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="C22" s="31"/>
-    </row>
-    <row r="23" spans="2:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="32" t="s">
+      <c r="C22" s="32"/>
+    </row>
+    <row r="23" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="35" t="s">
         <v>225</v>
       </c>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B24" s="32" t="s">
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B24" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B15:J15"/>
+    <mergeCell ref="B21:J21"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="B18:J18"/>
+    <mergeCell ref="B17:J17"/>
+    <mergeCell ref="B16:J16"/>
+    <mergeCell ref="B20:L20"/>
     <mergeCell ref="B26:J26"/>
     <mergeCell ref="B25:J25"/>
     <mergeCell ref="B24:J24"/>
     <mergeCell ref="B23:J23"/>
     <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B15:J15"/>
-    <mergeCell ref="B21:J21"/>
-    <mergeCell ref="B20:J20"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="B18:J18"/>
-    <mergeCell ref="B17:J17"/>
-    <mergeCell ref="B16:J16"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I1 I10:I11 I22 D2:D9 I27:I1048576">
@@ -6144,44 +6151,44 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
     </row>
     <row r="16" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
     </row>
     <row r="17" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
     </row>
     <row r="18" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
     </row>
     <row r="19" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="25"/>
@@ -6194,48 +6201,48 @@
       <c r="I19" s="25"/>
     </row>
     <row r="20" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
     </row>
     <row r="21" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
     </row>
     <row r="22" spans="2:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="C22" s="31"/>
+      <c r="C22" s="32"/>
     </row>
     <row r="23" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B26" s="5"/>

</xml_diff>

<commit_message>
test cases updated for US33
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rozanitis/Documents/Stevens/Semesters/Fall2018/SSW-555/gedcom-parser/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\Documents\GitHub\gedcom-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E1628F-A70C-AC48-A33E-40D8598F25A2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3434E185-5FC6-4A92-A09B-730B1D206089}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24440" windowHeight="15240" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="462" windowWidth="24438" windowHeight="15240" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,17 +23,22 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="179020" concurrentCalc="0"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="231">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -743,6 +748,9 @@
   </si>
   <si>
     <t>6. Continue to discuss any issues with the group to come up with a solution rather than spending more time to solve it on your own.</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -995,13 +1003,13 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1396,7 +1404,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1467,7 +1475,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1594,6 +1602,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3164,15 +3175,15 @@
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="6.47265625" customWidth="1"/>
+    <col min="3" max="3" width="8.47265625" customWidth="1"/>
+    <col min="4" max="5" width="20.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3189,7 +3200,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
       <c r="A3" s="12" t="s">
         <v>5</v>
       </c>
@@ -3206,7 +3217,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
       <c r="A4" s="12" t="s">
         <v>10</v>
       </c>
@@ -3223,7 +3234,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
       <c r="A5" s="12" t="s">
         <v>15</v>
       </c>
@@ -3240,7 +3251,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
       <c r="A6" s="12" t="s">
         <v>20</v>
       </c>
@@ -3257,7 +3268,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
@@ -3289,16 +3300,16 @@
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.47265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
@@ -3315,7 +3326,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3329,7 +3340,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3346,7 +3357,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3363,7 +3374,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3380,7 +3391,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3397,7 +3408,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3414,7 +3425,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3431,7 +3442,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3448,7 +3459,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>1</v>
       </c>
@@ -3465,7 +3476,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3482,7 +3493,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>1</v>
       </c>
@@ -3499,7 +3510,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>1</v>
       </c>
@@ -3516,7 +3527,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>1</v>
       </c>
@@ -3533,7 +3544,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>2</v>
       </c>
@@ -3550,7 +3561,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>2</v>
       </c>
@@ -3570,7 +3581,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>2</v>
       </c>
@@ -3590,7 +3601,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>2</v>
       </c>
@@ -3610,7 +3621,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="14" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>2</v>
       </c>
@@ -3627,7 +3638,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>2</v>
       </c>
@@ -3644,7 +3655,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>2</v>
       </c>
@@ -3661,7 +3672,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>2</v>
       </c>
@@ -3678,7 +3689,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>3</v>
       </c>
@@ -3695,7 +3706,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>3</v>
       </c>
@@ -3712,7 +3723,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>3</v>
       </c>
@@ -3729,7 +3740,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>3</v>
       </c>
@@ -3746,7 +3757,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>3</v>
       </c>
@@ -3763,7 +3774,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>3</v>
       </c>
@@ -3780,7 +3791,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>3</v>
       </c>
@@ -3797,7 +3808,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>3</v>
       </c>
@@ -3814,7 +3825,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>4</v>
       </c>
@@ -3831,7 +3842,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>4</v>
       </c>
@@ -3848,7 +3859,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>4</v>
       </c>
@@ -3865,7 +3876,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>4</v>
       </c>
@@ -3882,7 +3893,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>4</v>
       </c>
@@ -3899,7 +3910,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>4</v>
       </c>
@@ -3916,7 +3927,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>4</v>
       </c>
@@ -3933,7 +3944,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>4</v>
       </c>
@@ -3982,47 +3993,47 @@
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="2"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="9.47265625" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
     <col min="5" max="5" width="6.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.47265625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>116</v>
       </c>
@@ -4045,7 +4056,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>123</v>
       </c>
@@ -4061,7 +4072,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>124</v>
       </c>
@@ -4086,7 +4097,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>125</v>
       </c>
@@ -4111,7 +4122,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>126</v>
       </c>
@@ -4136,7 +4147,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>127</v>
       </c>
@@ -4172,19 +4183,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:G8"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="9.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>116</v>
       </c>
@@ -4207,7 +4220,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -4222,7 +4235,7 @@
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>124</v>
       </c>
@@ -4248,7 +4261,7 @@
         <v>14.592592592592593</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>125</v>
       </c>
@@ -4274,7 +4287,7 @@
         <v>10.258064516129032</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>126</v>
       </c>
@@ -4300,12 +4313,30 @@
         <v>11.533333333333333</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>127</v>
       </c>
       <c r="B8" s="2">
         <v>41955</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <f>Sprint4!G10</f>
+        <v>56</v>
+      </c>
+      <c r="F8">
+        <f>(Sprint4!H10*60)</f>
+        <v>240</v>
+      </c>
+      <c r="G8" s="7">
+        <f>E8/(F8/60)</f>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -4322,21 +4353,21 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.47265625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.47265625" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="19" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -4365,7 +4396,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
@@ -4394,7 +4425,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A3" s="14" t="s">
         <v>37</v>
       </c>
@@ -4426,7 +4457,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A4" s="14" t="s">
         <v>39</v>
       </c>
@@ -4458,7 +4489,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A5" s="14" t="s">
         <v>41</v>
       </c>
@@ -4490,7 +4521,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
@@ -4519,7 +4550,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A7" s="14" t="s">
         <v>45</v>
       </c>
@@ -4548,7 +4579,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A8" s="14" t="s">
         <v>47</v>
       </c>
@@ -4577,7 +4608,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A9" s="14" t="s">
         <v>53</v>
       </c>
@@ -4606,7 +4637,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B10" s="5" t="s">
         <v>136</v>
       </c>
@@ -4619,20 +4650,20 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B12" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B14" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B15" s="30" t="s">
         <v>139</v>
       </c>
@@ -4644,7 +4675,7 @@
       <c r="H15" s="30"/>
       <c r="I15" s="30"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B16" s="30" t="s">
         <v>140</v>
       </c>
@@ -4656,7 +4687,7 @@
       <c r="H16" s="30"/>
       <c r="I16" s="30"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B17" s="30" t="s">
         <v>141</v>
       </c>
@@ -4668,7 +4699,7 @@
       <c r="H17" s="30"/>
       <c r="I17" s="30"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B18" s="30" t="s">
         <v>142</v>
       </c>
@@ -4680,7 +4711,7 @@
       <c r="H18" s="30"/>
       <c r="I18" s="30"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B19" s="31" t="s">
         <v>143</v>
       </c>
@@ -4692,12 +4723,12 @@
       <c r="H19" s="31"/>
       <c r="I19" s="31"/>
     </row>
-    <row r="20" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B20" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B21" s="30" t="s">
         <v>145</v>
       </c>
@@ -4708,7 +4739,7 @@
       <c r="G21" s="30"/>
       <c r="H21" s="30"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B22" s="30" t="s">
         <v>146</v>
       </c>
@@ -4718,16 +4749,16 @@
       <c r="F22" s="30"/>
       <c r="G22" s="30"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B24" s="5"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="29" t="s">
         <v>147</v>
       </c>
       <c r="B26" s="29"/>
     </row>
-    <row r="27" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
@@ -4756,7 +4787,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -4785,7 +4816,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -4814,7 +4845,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" s="14" t="s">
         <v>51</v>
       </c>
@@ -4843,7 +4874,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -4938,21 +4969,21 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.47265625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.47265625" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="19" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>149</v>
       </c>
@@ -4981,7 +5012,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A2" s="14" t="s">
         <v>59</v>
       </c>
@@ -5010,7 +5041,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A3" s="14" t="s">
         <v>61</v>
       </c>
@@ -5042,7 +5073,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A4" s="14" t="s">
         <v>64</v>
       </c>
@@ -5074,7 +5105,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A5" s="14" t="s">
         <v>67</v>
       </c>
@@ -5106,7 +5137,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A6" s="14" t="s">
         <v>69</v>
       </c>
@@ -5135,7 +5166,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A7" s="14" t="s">
         <v>71</v>
       </c>
@@ -5164,7 +5195,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A8" s="14" t="s">
         <v>73</v>
       </c>
@@ -5193,7 +5224,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A9" s="14" t="s">
         <v>75</v>
       </c>
@@ -5222,7 +5253,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B10" s="5" t="s">
         <v>136</v>
       </c>
@@ -5235,20 +5266,20 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B12" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B14" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="30" t="s">
         <v>159</v>
       </c>
@@ -5260,7 +5291,7 @@
       <c r="H15" s="30"/>
       <c r="I15" s="30"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B16" s="30" t="s">
         <v>160</v>
       </c>
@@ -5272,7 +5303,7 @@
       <c r="H16" s="30"/>
       <c r="I16" s="30"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B17" s="30" t="s">
         <v>161</v>
       </c>
@@ -5284,7 +5315,7 @@
       <c r="H17" s="30"/>
       <c r="I17" s="25"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B18" s="30" t="s">
         <v>162</v>
       </c>
@@ -5296,13 +5327,13 @@
       <c r="H18" s="31"/>
       <c r="I18" s="31"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B20" s="32" t="s">
         <v>144</v>
       </c>
       <c r="C20" s="32"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B21" s="30" t="s">
         <v>163</v>
       </c>
@@ -5313,7 +5344,7 @@
       <c r="G21" s="30"/>
       <c r="H21" s="30"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
       <c r="D22" s="26"/>
@@ -5323,7 +5354,7 @@
       <c r="H22" s="26"/>
       <c r="I22" s="26"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B25" s="30"/>
       <c r="C25" s="30"/>
       <c r="D25" s="30"/>
@@ -5331,7 +5362,7 @@
       <c r="F25" s="30"/>
       <c r="G25" s="30"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B27" s="5"/>
     </row>
   </sheetData>
@@ -5377,23 +5408,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.47265625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.47265625" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="19" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>149</v>
       </c>
@@ -5422,7 +5453,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A2" s="14" t="s">
         <v>84</v>
       </c>
@@ -5451,7 +5482,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A3" s="14" t="s">
         <v>88</v>
       </c>
@@ -5483,7 +5514,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -5515,7 +5546,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -5547,7 +5578,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A6" s="14" t="s">
         <v>77</v>
       </c>
@@ -5576,7 +5607,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
@@ -5605,7 +5636,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -5634,7 +5665,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A9" s="14" t="s">
         <v>82</v>
       </c>
@@ -5663,7 +5694,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B10" s="5" t="s">
         <v>136</v>
       </c>
@@ -5676,21 +5707,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B12" s="5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A14" s="27"/>
       <c r="B14" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:26" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="30" t="s">
         <v>221</v>
       </c>
@@ -5703,140 +5734,145 @@
       <c r="I15" s="30"/>
       <c r="J15" s="30"/>
     </row>
-    <row r="16" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="35" t="s">
+    <row r="16" spans="1:26" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="34" t="s">
         <v>223</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-    </row>
-    <row r="17" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="35" t="s">
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+    </row>
+    <row r="17" spans="2:12" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-    </row>
-    <row r="18" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="35" t="s">
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+    </row>
+    <row r="18" spans="2:12" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="34" t="s">
         <v>224</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-    </row>
-    <row r="19" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="35" t="s">
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+    </row>
+    <row r="19" spans="2:12" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-    </row>
-    <row r="20" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="34" t="s">
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+    </row>
+    <row r="20" spans="2:12" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="33" t="s">
         <v>229</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
-    </row>
-    <row r="21" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-    </row>
-    <row r="22" spans="2:12" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
+    </row>
+    <row r="21" spans="2:12" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+    </row>
+    <row r="22" spans="2:12" ht="13" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B22" s="32" t="s">
         <v>144</v>
       </c>
       <c r="C22" s="32"/>
     </row>
-    <row r="23" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="35" t="s">
+    <row r="23" spans="2:12" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="35"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B24" s="35" t="s">
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B24" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B26:J26"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="B24:J24"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B15:J15"/>
     <mergeCell ref="B21:J21"/>
     <mergeCell ref="B19:J19"/>
@@ -5844,11 +5880,6 @@
     <mergeCell ref="B17:J17"/>
     <mergeCell ref="B16:J16"/>
     <mergeCell ref="B20:L20"/>
-    <mergeCell ref="B26:J26"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="B24:J24"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I1 I10:I11 I22 D2:D9 I27:I1048576">
@@ -5884,23 +5915,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" style="18" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.47265625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.47265625" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="19" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>149</v>
       </c>
@@ -5929,7 +5962,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A2" s="14" t="s">
         <v>100</v>
       </c>
@@ -5952,7 +5985,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>102</v>
       </c>
@@ -5978,7 +6011,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -5989,7 +6022,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="E4" s="17">
         <v>30</v>
@@ -5997,16 +6030,20 @@
       <c r="F4" s="17">
         <v>2</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
+      <c r="G4" s="17">
+        <v>28</v>
+      </c>
+      <c r="H4" s="17">
+        <v>2</v>
+      </c>
       <c r="I4" s="22" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="Z4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -6017,7 +6054,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="E5" s="17">
         <v>25</v>
@@ -6025,14 +6062,20 @@
       <c r="F5" s="17">
         <v>2</v>
       </c>
+      <c r="G5" s="18">
+        <v>28</v>
+      </c>
+      <c r="H5" s="18">
+        <v>2</v>
+      </c>
       <c r="I5" s="22" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="Z5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -6055,7 +6098,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -6078,7 +6121,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -6101,7 +6144,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A9" s="14" t="s">
         <v>108</v>
       </c>
@@ -6124,33 +6167,33 @@
         <v>228</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B10" s="5" t="s">
         <v>136</v>
       </c>
       <c r="G10" s="18">
         <f>SUM(G2:G9)</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="H10" s="18">
         <f>SUM(H2:H9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B12" s="5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B14" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:26" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="30"/>
       <c r="C15" s="30"/>
       <c r="D15" s="30"/>
@@ -6160,7 +6203,7 @@
       <c r="H15" s="30"/>
       <c r="I15" s="30"/>
     </row>
-    <row r="16" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:26" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="30"/>
       <c r="C16" s="30"/>
       <c r="D16" s="30"/>
@@ -6170,7 +6213,7 @@
       <c r="H16" s="30"/>
       <c r="I16" s="30"/>
     </row>
-    <row r="17" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="30"/>
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
@@ -6180,7 +6223,7 @@
       <c r="H17" s="30"/>
       <c r="I17" s="30"/>
     </row>
-    <row r="18" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="30"/>
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
@@ -6190,7 +6233,7 @@
       <c r="H18" s="30"/>
       <c r="I18" s="30"/>
     </row>
-    <row r="19" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="25"/>
       <c r="C19" s="25"/>
       <c r="D19" s="25"/>
@@ -6200,7 +6243,7 @@
       <c r="H19" s="25"/>
       <c r="I19" s="25"/>
     </row>
-    <row r="20" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="31"/>
       <c r="C20" s="31"/>
       <c r="D20" s="31"/>
@@ -6210,7 +6253,7 @@
       <c r="H20" s="31"/>
       <c r="I20" s="31"/>
     </row>
-    <row r="21" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B21" s="31"/>
       <c r="C21" s="31"/>
       <c r="D21" s="31"/>
@@ -6220,13 +6263,13 @@
       <c r="H21" s="31"/>
       <c r="I21" s="31"/>
     </row>
-    <row r="22" spans="2:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:9" ht="13" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B22" s="32" t="s">
         <v>144</v>
       </c>
       <c r="C22" s="32"/>
     </row>
-    <row r="23" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B23" s="30"/>
       <c r="C23" s="30"/>
       <c r="D23" s="30"/>
@@ -6236,7 +6279,7 @@
       <c r="H23" s="30"/>
       <c r="I23" s="30"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B24" s="30"/>
       <c r="C24" s="30"/>
       <c r="D24" s="30"/>
@@ -6244,7 +6287,7 @@
       <c r="F24" s="30"/>
       <c r="G24" s="30"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B26" s="5"/>
     </row>
   </sheetData>
@@ -6296,14 +6339,14 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.6640625" customWidth="1"/>
-    <col min="3" max="3" width="69.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="69.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>149</v>
       </c>
@@ -6317,7 +6360,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -6331,7 +6374,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -6345,7 +6388,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -6359,7 +6402,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -6373,7 +6416,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -6387,7 +6430,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -6401,7 +6444,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -6415,7 +6458,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -6426,7 +6469,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -6437,7 +6480,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>64</v>
       </c>
@@ -6448,7 +6491,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>96</v>
       </c>
@@ -6459,7 +6502,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -6470,7 +6513,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -6481,7 +6524,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -6492,7 +6535,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -6503,7 +6546,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -6514,7 +6557,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>184</v>
       </c>
@@ -6525,7 +6568,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -6536,7 +6579,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>98</v>
       </c>
@@ -6547,7 +6590,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>189</v>
       </c>
@@ -6558,7 +6601,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -6572,7 +6615,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -6583,7 +6626,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>86</v>
       </c>
@@ -6594,7 +6637,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>100</v>
       </c>
@@ -6605,7 +6648,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -6619,7 +6662,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="85" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>198</v>
       </c>
@@ -6630,7 +6673,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -6641,7 +6684,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>102</v>
       </c>
@@ -6652,7 +6695,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -6666,7 +6709,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -6677,7 +6720,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>90</v>
       </c>
@@ -6691,7 +6734,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>92</v>
       </c>
@@ -6705,7 +6748,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -6716,7 +6759,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>106</v>
       </c>
@@ -6727,7 +6770,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -6738,7 +6781,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -6749,7 +6792,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>73</v>
       </c>
@@ -6760,7 +6803,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -6771,7 +6814,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>108</v>
       </c>
@@ -6782,7 +6825,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>214</v>
       </c>
@@ -6793,7 +6836,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>217</v>
       </c>
@@ -6804,7 +6847,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>82</v>
       </c>

</xml_diff>

<commit_message>
completing US34 and US39
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11014"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\Documents\GitHub\gedcom-parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/latinocodes/PycharmProjects/gedcom-parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3434E185-5FC6-4A92-A09B-730B1D206089}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96496FD8-5AD9-A246-94B3-40F95BAAA77D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="462" windowWidth="24438" windowHeight="15240" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24440" windowHeight="15240" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -28,17 +28,12 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="232">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -751,6 +746,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Review results of Sprint 4</t>
   </si>
 </sst>
 </file>
@@ -1003,13 +1001,13 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1404,7 +1402,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1475,7 +1473,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3175,15 +3173,15 @@
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.47265625" customWidth="1"/>
-    <col min="3" max="3" width="8.47265625" customWidth="1"/>
-    <col min="4" max="5" width="20.47265625" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3200,7 +3198,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>5</v>
       </c>
@@ -3217,7 +3215,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>10</v>
       </c>
@@ -3234,7 +3232,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>15</v>
       </c>
@@ -3251,7 +3249,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>20</v>
       </c>
@@ -3268,7 +3266,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
@@ -3300,16 +3298,16 @@
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.47265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
@@ -3326,7 +3324,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3340,7 +3338,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3357,7 +3355,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3374,7 +3372,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3391,7 +3389,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3408,7 +3406,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3425,7 +3423,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3442,7 +3440,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3459,7 +3457,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1</v>
       </c>
@@ -3476,7 +3474,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3493,7 +3491,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>1</v>
       </c>
@@ -3510,7 +3508,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>1</v>
       </c>
@@ -3527,7 +3525,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>1</v>
       </c>
@@ -3544,7 +3542,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2</v>
       </c>
@@ -3561,7 +3559,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>2</v>
       </c>
@@ -3581,7 +3579,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2</v>
       </c>
@@ -3601,7 +3599,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2</v>
       </c>
@@ -3621,7 +3619,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2</v>
       </c>
@@ -3638,7 +3636,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>2</v>
       </c>
@@ -3655,7 +3653,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>2</v>
       </c>
@@ -3672,7 +3670,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>2</v>
       </c>
@@ -3689,7 +3687,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>3</v>
       </c>
@@ -3706,7 +3704,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>3</v>
       </c>
@@ -3723,7 +3721,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>3</v>
       </c>
@@ -3740,7 +3738,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>3</v>
       </c>
@@ -3757,7 +3755,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>3</v>
       </c>
@@ -3774,7 +3772,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>3</v>
       </c>
@@ -3791,7 +3789,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>3</v>
       </c>
@@ -3808,7 +3806,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>3</v>
       </c>
@@ -3825,7 +3823,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>4</v>
       </c>
@@ -3842,7 +3840,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>4</v>
       </c>
@@ -3859,7 +3857,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>4</v>
       </c>
@@ -3876,7 +3874,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>4</v>
       </c>
@@ -3893,7 +3891,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>4</v>
       </c>
@@ -3910,7 +3908,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>4</v>
       </c>
@@ -3927,7 +3925,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>4</v>
       </c>
@@ -3944,7 +3942,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>4</v>
       </c>
@@ -3993,47 +3991,47 @@
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="2"/>
-    <col min="2" max="2" width="9.47265625" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
     <col min="5" max="5" width="6.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.47265625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>116</v>
       </c>
@@ -4056,7 +4054,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>123</v>
       </c>
@@ -4072,7 +4070,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>124</v>
       </c>
@@ -4097,7 +4095,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>125</v>
       </c>
@@ -4122,7 +4120,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>126</v>
       </c>
@@ -4147,7 +4145,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>127</v>
       </c>
@@ -4183,21 +4181,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="9.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>116</v>
       </c>
@@ -4220,7 +4218,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -4235,7 +4233,7 @@
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>124</v>
       </c>
@@ -4261,7 +4259,7 @@
         <v>14.592592592592593</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>125</v>
       </c>
@@ -4287,7 +4285,7 @@
         <v>10.258064516129032</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>126</v>
       </c>
@@ -4313,7 +4311,7 @@
         <v>11.533333333333333</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>127</v>
       </c>
@@ -4328,15 +4326,15 @@
       </c>
       <c r="E8">
         <f>Sprint4!G10</f>
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="F8">
         <f>(Sprint4!H10*60)</f>
-        <v>240</v>
+        <v>390</v>
       </c>
       <c r="G8" s="7">
         <f>E8/(F8/60)</f>
-        <v>14</v>
+        <v>15.538461538461538</v>
       </c>
     </row>
   </sheetData>
@@ -4353,21 +4351,21 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.47265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="19" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -4396,7 +4394,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
@@ -4425,7 +4423,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
         <v>37</v>
       </c>
@@ -4457,7 +4455,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
         <v>39</v>
       </c>
@@ -4489,7 +4487,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
         <v>41</v>
       </c>
@@ -4521,7 +4519,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
@@ -4550,7 +4548,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
         <v>45</v>
       </c>
@@ -4579,7 +4577,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="14" t="s">
         <v>47</v>
       </c>
@@ -4608,7 +4606,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>53</v>
       </c>
@@ -4637,7 +4635,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>136</v>
       </c>
@@ -4650,20 +4648,20 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B15" s="30" t="s">
         <v>139</v>
       </c>
@@ -4675,7 +4673,7 @@
       <c r="H15" s="30"/>
       <c r="I15" s="30"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B16" s="30" t="s">
         <v>140</v>
       </c>
@@ -4687,7 +4685,7 @@
       <c r="H16" s="30"/>
       <c r="I16" s="30"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B17" s="30" t="s">
         <v>141</v>
       </c>
@@ -4699,7 +4697,7 @@
       <c r="H17" s="30"/>
       <c r="I17" s="30"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B18" s="30" t="s">
         <v>142</v>
       </c>
@@ -4711,7 +4709,7 @@
       <c r="H18" s="30"/>
       <c r="I18" s="30"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B19" s="31" t="s">
         <v>143</v>
       </c>
@@ -4723,12 +4721,12 @@
       <c r="H19" s="31"/>
       <c r="I19" s="31"/>
     </row>
-    <row r="20" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="B20" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B21" s="30" t="s">
         <v>145</v>
       </c>
@@ -4739,7 +4737,7 @@
       <c r="G21" s="30"/>
       <c r="H21" s="30"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B22" s="30" t="s">
         <v>146</v>
       </c>
@@ -4749,16 +4747,16 @@
       <c r="F22" s="30"/>
       <c r="G22" s="30"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B24" s="5"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="29" t="s">
         <v>147</v>
       </c>
       <c r="B26" s="29"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
@@ -4787,7 +4785,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -4816,7 +4814,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -4845,7 +4843,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="14" t="s">
         <v>51</v>
       </c>
@@ -4874,7 +4872,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -4969,21 +4967,21 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.47265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="19" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>149</v>
       </c>
@@ -5012,7 +5010,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
         <v>59</v>
       </c>
@@ -5041,7 +5039,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
         <v>61</v>
       </c>
@@ -5073,7 +5071,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
         <v>64</v>
       </c>
@@ -5105,7 +5103,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
         <v>67</v>
       </c>
@@ -5137,7 +5135,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="14" t="s">
         <v>69</v>
       </c>
@@ -5166,7 +5164,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
         <v>71</v>
       </c>
@@ -5195,7 +5193,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="14" t="s">
         <v>73</v>
       </c>
@@ -5224,7 +5222,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>75</v>
       </c>
@@ -5253,7 +5251,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>136</v>
       </c>
@@ -5266,20 +5264,20 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="30" t="s">
         <v>159</v>
       </c>
@@ -5291,7 +5289,7 @@
       <c r="H15" s="30"/>
       <c r="I15" s="30"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B16" s="30" t="s">
         <v>160</v>
       </c>
@@ -5303,7 +5301,7 @@
       <c r="H16" s="30"/>
       <c r="I16" s="30"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B17" s="30" t="s">
         <v>161</v>
       </c>
@@ -5315,7 +5313,7 @@
       <c r="H17" s="30"/>
       <c r="I17" s="25"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B18" s="30" t="s">
         <v>162</v>
       </c>
@@ -5327,13 +5325,13 @@
       <c r="H18" s="31"/>
       <c r="I18" s="31"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B20" s="32" t="s">
         <v>144</v>
       </c>
       <c r="C20" s="32"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B21" s="30" t="s">
         <v>163</v>
       </c>
@@ -5344,7 +5342,7 @@
       <c r="G21" s="30"/>
       <c r="H21" s="30"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
       <c r="D22" s="26"/>
@@ -5354,7 +5352,7 @@
       <c r="H22" s="26"/>
       <c r="I22" s="26"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B25" s="30"/>
       <c r="C25" s="30"/>
       <c r="D25" s="30"/>
@@ -5362,7 +5360,7 @@
       <c r="F25" s="30"/>
       <c r="G25" s="30"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B27" s="5"/>
     </row>
   </sheetData>
@@ -5410,21 +5408,21 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.47265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="19" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>149</v>
       </c>
@@ -5453,7 +5451,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
         <v>84</v>
       </c>
@@ -5482,7 +5480,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
         <v>88</v>
       </c>
@@ -5514,7 +5512,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -5546,7 +5544,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -5578,7 +5576,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="14" t="s">
         <v>77</v>
       </c>
@@ -5607,7 +5605,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
@@ -5636,7 +5634,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -5665,7 +5663,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>82</v>
       </c>
@@ -5694,7 +5692,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>136</v>
       </c>
@@ -5707,21 +5705,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="27"/>
       <c r="B14" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="30" t="s">
         <v>221</v>
       </c>
@@ -5734,145 +5732,140 @@
       <c r="I15" s="30"/>
       <c r="J15" s="30"/>
     </row>
-    <row r="16" spans="1:26" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="34" t="s">
+    <row r="16" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="35" t="s">
         <v>223</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-    </row>
-    <row r="17" spans="2:12" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="34" t="s">
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+    </row>
+    <row r="17" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-    </row>
-    <row r="18" spans="2:12" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="34" t="s">
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+    </row>
+    <row r="18" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-    </row>
-    <row r="19" spans="2:12" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="34" t="s">
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+    </row>
+    <row r="19" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-    </row>
-    <row r="20" spans="2:12" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="33" t="s">
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+    </row>
+    <row r="20" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="34" t="s">
         <v>229</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-    </row>
-    <row r="21" spans="2:12" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-    </row>
-    <row r="22" spans="2:12" ht="13" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+    </row>
+    <row r="21" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+    </row>
+    <row r="22" spans="2:12" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="32" t="s">
         <v>144</v>
       </c>
       <c r="C22" s="32"/>
     </row>
-    <row r="23" spans="2:12" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="34" t="s">
+    <row r="23" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="35" t="s">
         <v>225</v>
       </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B24" s="34" t="s">
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B24" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="35"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B26:J26"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="B24:J24"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B15:J15"/>
     <mergeCell ref="B21:J21"/>
     <mergeCell ref="B19:J19"/>
@@ -5880,6 +5873,11 @@
     <mergeCell ref="B17:J17"/>
     <mergeCell ref="B16:J16"/>
     <mergeCell ref="B20:L20"/>
+    <mergeCell ref="B26:J26"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="B24:J24"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I1 I10:I11 I22 D2:D9 I27:I1048576">
@@ -5915,25 +5913,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.47265625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="18" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="19" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>149</v>
       </c>
@@ -5962,7 +5960,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
         <v>100</v>
       </c>
@@ -5985,7 +5983,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>102</v>
       </c>
@@ -6011,7 +6009,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -6043,7 +6041,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -6075,7 +6073,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -6098,7 +6096,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -6121,7 +6119,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -6132,7 +6130,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="E8" s="17">
         <v>25</v>
@@ -6140,11 +6138,17 @@
       <c r="F8" s="17">
         <v>1.5</v>
       </c>
+      <c r="G8" s="18">
+        <v>25</v>
+      </c>
+      <c r="H8" s="18">
+        <v>1.5</v>
+      </c>
       <c r="I8" s="23" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>108</v>
       </c>
@@ -6155,7 +6159,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="E9" s="17">
         <v>20</v>
@@ -6163,37 +6167,43 @@
       <c r="F9" s="17">
         <v>1</v>
       </c>
+      <c r="G9" s="18">
+        <v>20</v>
+      </c>
+      <c r="H9" s="18">
+        <v>1</v>
+      </c>
       <c r="I9" s="23" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>136</v>
       </c>
       <c r="G10" s="18">
         <f>SUM(G2:G9)</f>
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="H10" s="18">
         <f>SUM(H2:H9)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="30"/>
       <c r="C15" s="30"/>
       <c r="D15" s="30"/>
@@ -6203,7 +6213,7 @@
       <c r="H15" s="30"/>
       <c r="I15" s="30"/>
     </row>
-    <row r="16" spans="1:26" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="30"/>
       <c r="C16" s="30"/>
       <c r="D16" s="30"/>
@@ -6213,7 +6223,7 @@
       <c r="H16" s="30"/>
       <c r="I16" s="30"/>
     </row>
-    <row r="17" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="30"/>
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
@@ -6223,7 +6233,7 @@
       <c r="H17" s="30"/>
       <c r="I17" s="30"/>
     </row>
-    <row r="18" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="30"/>
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
@@ -6233,7 +6243,7 @@
       <c r="H18" s="30"/>
       <c r="I18" s="30"/>
     </row>
-    <row r="19" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="25"/>
       <c r="C19" s="25"/>
       <c r="D19" s="25"/>
@@ -6243,7 +6253,7 @@
       <c r="H19" s="25"/>
       <c r="I19" s="25"/>
     </row>
-    <row r="20" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="31"/>
       <c r="C20" s="31"/>
       <c r="D20" s="31"/>
@@ -6253,7 +6263,7 @@
       <c r="H20" s="31"/>
       <c r="I20" s="31"/>
     </row>
-    <row r="21" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="31"/>
       <c r="C21" s="31"/>
       <c r="D21" s="31"/>
@@ -6263,13 +6273,13 @@
       <c r="H21" s="31"/>
       <c r="I21" s="31"/>
     </row>
-    <row r="22" spans="2:9" ht="13" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="32" t="s">
         <v>144</v>
       </c>
       <c r="C22" s="32"/>
     </row>
-    <row r="23" spans="2:9" ht="12.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="30"/>
       <c r="C23" s="30"/>
       <c r="D23" s="30"/>
@@ -6279,7 +6289,7 @@
       <c r="H23" s="30"/>
       <c r="I23" s="30"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B24" s="30"/>
       <c r="C24" s="30"/>
       <c r="D24" s="30"/>
@@ -6287,7 +6297,7 @@
       <c r="F24" s="30"/>
       <c r="G24" s="30"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B26" s="5"/>
     </row>
   </sheetData>
@@ -6328,6 +6338,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -6335,18 +6346,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A29" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.6640625" customWidth="1"/>
-    <col min="3" max="3" width="69.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="69.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>149</v>
       </c>
@@ -6360,7 +6371,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -6374,7 +6385,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -6388,7 +6399,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -6402,7 +6413,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -6416,7 +6427,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -6430,7 +6441,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -6444,7 +6455,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -6458,7 +6469,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -6469,7 +6480,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -6480,7 +6491,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>64</v>
       </c>
@@ -6491,7 +6502,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>96</v>
       </c>
@@ -6502,7 +6513,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -6513,7 +6524,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -6524,7 +6535,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -6535,7 +6546,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -6546,7 +6557,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -6557,7 +6568,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>184</v>
       </c>
@@ -6568,7 +6579,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -6579,7 +6590,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>98</v>
       </c>
@@ -6590,7 +6601,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>189</v>
       </c>
@@ -6601,7 +6612,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -6615,7 +6626,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -6626,7 +6637,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>86</v>
       </c>
@@ -6637,7 +6648,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>100</v>
       </c>
@@ -6648,7 +6659,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -6662,7 +6673,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="85" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>198</v>
       </c>
@@ -6673,7 +6684,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -6684,7 +6695,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>102</v>
       </c>
@@ -6695,7 +6706,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -6709,7 +6720,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -6720,7 +6731,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>90</v>
       </c>
@@ -6734,7 +6745,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>92</v>
       </c>
@@ -6748,7 +6759,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -6759,7 +6770,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>106</v>
       </c>
@@ -6770,7 +6781,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -6781,7 +6792,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -6792,7 +6803,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>73</v>
       </c>
@@ -6803,7 +6814,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -6814,7 +6825,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>108</v>
       </c>
@@ -6825,7 +6836,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>214</v>
       </c>
@@ -6836,7 +6847,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>217</v>
       </c>
@@ -6847,7 +6858,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>82</v>
       </c>

</xml_diff>

<commit_message>
added US24 unique_families_by_spouses and test cases
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/latinocodes/PycharmProjects/gedcom-parser/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rozanitis/Documents/Stevens/Semesters/Fall2018/SSW-555/gedcom-parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96496FD8-5AD9-A246-94B3-40F95BAAA77D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC71BAE-6AFA-0745-96A6-C39A5D7E907D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="24440" windowHeight="15240" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1001,13 +1001,13 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -4326,15 +4326,15 @@
       </c>
       <c r="E8">
         <f>Sprint4!G10</f>
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="F8">
         <f>(Sprint4!H10*60)</f>
-        <v>390</v>
+        <v>510</v>
       </c>
       <c r="G8" s="7">
         <f>E8/(F8/60)</f>
-        <v>15.538461538461538</v>
+        <v>13.882352941176471</v>
       </c>
     </row>
   </sheetData>
@@ -5733,82 +5733,82 @@
       <c r="J15" s="30"/>
     </row>
     <row r="16" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="34" t="s">
         <v>223</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
     </row>
     <row r="17" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
     </row>
     <row r="18" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="34" t="s">
         <v>224</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
     </row>
     <row r="19" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="33" t="s">
         <v>229</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
     </row>
     <row r="21" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
     </row>
     <row r="22" spans="2:12" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="32" t="s">
@@ -5817,55 +5817,60 @@
       <c r="C22" s="32"/>
     </row>
     <row r="23" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="35"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B24" s="35" t="s">
+      <c r="B24" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B26:J26"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="B24:J24"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B15:J15"/>
     <mergeCell ref="B21:J21"/>
     <mergeCell ref="B19:J19"/>
@@ -5873,11 +5878,6 @@
     <mergeCell ref="B17:J17"/>
     <mergeCell ref="B16:J16"/>
     <mergeCell ref="B20:L20"/>
-    <mergeCell ref="B26:J26"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="B24:J24"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I1 I10:I11 I22 D2:D9 I27:I1048576">
@@ -5913,9 +5913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5971,7 +5969,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="E2" s="17">
         <v>10</v>
@@ -5979,8 +5977,14 @@
       <c r="F2" s="17">
         <v>1.5</v>
       </c>
+      <c r="G2" s="18">
+        <v>17</v>
+      </c>
+      <c r="H2" s="18">
+        <v>2</v>
+      </c>
       <c r="I2" s="22" t="s">
-        <v>228</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
@@ -6183,11 +6187,11 @@
       </c>
       <c r="G10" s="18">
         <f>SUM(G2:G9)</f>
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="H10" s="18">
         <f>SUM(H2:H9)</f>
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
@@ -6346,9 +6350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>

<commit_message>
updated to indicate US28 complete
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rozanitis/Documents/Stevens/Semesters/Fall2018/SSW-555/gedcom-parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC71BAE-6AFA-0745-96A6-C39A5D7E907D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA261576-E7FD-FC41-BAB0-C8243E3D306F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="24440" windowHeight="15240" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="231">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -743,9 +743,6 @@
   </si>
   <si>
     <t>6. Continue to discuss any issues with the group to come up with a solution rather than spending more time to solve it on your own.</t>
-  </si>
-  <si>
-    <t>yes</t>
   </si>
   <si>
     <t>Review results of Sprint 4</t>
@@ -832,7 +829,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -856,6 +853,19 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -929,7 +939,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1001,15 +1011,16 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="68">
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
@@ -3837,7 +3848,7 @@
         <v>15</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.15">
@@ -3888,7 +3899,7 @@
         <v>10</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
@@ -3905,7 +3916,7 @@
         <v>10</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
@@ -3922,7 +3933,7 @@
         <v>15</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
@@ -3939,7 +3950,7 @@
         <v>5</v>
       </c>
       <c r="E37" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
@@ -3956,7 +3967,7 @@
         <v>5</v>
       </c>
       <c r="E38" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -4326,15 +4337,15 @@
       </c>
       <c r="E8">
         <f>Sprint4!G10</f>
-        <v>118</v>
+        <v>151</v>
       </c>
       <c r="F8">
         <f>(Sprint4!H10*60)</f>
-        <v>510</v>
+        <v>690</v>
       </c>
       <c r="G8" s="7">
         <f>E8/(F8/60)</f>
-        <v>13.882352941176471</v>
+        <v>13.130434782608695</v>
       </c>
     </row>
   </sheetData>
@@ -5733,82 +5744,82 @@
       <c r="J15" s="30"/>
     </row>
     <row r="16" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="35" t="s">
         <v>223</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
     </row>
     <row r="20" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="34" t="s">
         <v>229</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
     </row>
     <row r="21" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
     </row>
     <row r="22" spans="2:12" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="32" t="s">
@@ -5817,60 +5828,55 @@
       <c r="C22" s="32"/>
     </row>
     <row r="23" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="35" t="s">
         <v>225</v>
       </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="35"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B26:J26"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="B24:J24"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B15:J15"/>
     <mergeCell ref="B21:J21"/>
     <mergeCell ref="B19:J19"/>
@@ -5878,6 +5884,11 @@
     <mergeCell ref="B17:J17"/>
     <mergeCell ref="B16:J16"/>
     <mergeCell ref="B20:L20"/>
+    <mergeCell ref="B26:J26"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="B24:J24"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I1 I10:I11 I22 D2:D9 I27:I1048576">
@@ -5930,7 +5941,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="36" t="s">
         <v>149</v>
       </c>
       <c r="B1" s="5" t="s">
@@ -5998,7 +6009,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="E3" s="17">
         <v>20</v>
@@ -6006,8 +6017,14 @@
       <c r="F3" s="17">
         <v>2</v>
       </c>
+      <c r="G3" s="18">
+        <v>33</v>
+      </c>
+      <c r="H3" s="18">
+        <v>3</v>
+      </c>
       <c r="I3" s="22" t="s">
-        <v>228</v>
+        <v>133</v>
       </c>
       <c r="Z3" t="s">
         <v>63</v>
@@ -6039,7 +6056,7 @@
         <v>2</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>230</v>
+        <v>133</v>
       </c>
       <c r="Z4" t="s">
         <v>66</v>
@@ -6071,7 +6088,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>230</v>
+        <v>133</v>
       </c>
       <c r="Z5" t="s">
         <v>34</v>
@@ -6187,16 +6204,16 @@
       </c>
       <c r="G10" s="18">
         <f>SUM(G2:G9)</f>
-        <v>118</v>
+        <v>151</v>
       </c>
       <c r="H10" s="18">
         <f>SUM(H2:H9)</f>
-        <v>8.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
user stories sorted by numbers
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rozanitis/Documents/Stevens/Semesters/Fall2018/SSW-555/gedcom-parser/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\Documents\GitHub\gedcom-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{FA261576-E7FD-FC41-BAB0-C8243E3D306F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{A5E64E9C-1507-40A6-8281-A0E473A4C914}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32539DE-7F74-444E-8760-8A5CE919F93E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24440" windowHeight="15240" tabRatio="500" firstSheet="7" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="462" windowWidth="24438" windowHeight="15240" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -758,7 +758,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -817,7 +817,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -827,6 +827,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -941,7 +947,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1014,15 +1020,16 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="68">
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
@@ -3184,17 +3191,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}"/>
+    <sheetView zoomScale="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.6171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.47265625" customWidth="1"/>
+    <col min="3" max="3" width="8.47265625" customWidth="1"/>
+    <col min="4" max="5" width="20.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3211,7 +3218,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17.100000000000001">
+    <row r="3" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
       <c r="A3" s="12" t="s">
         <v>5</v>
       </c>
@@ -3228,7 +3235,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17.100000000000001">
+    <row r="4" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
       <c r="A4" s="12" t="s">
         <v>10</v>
       </c>
@@ -3245,7 +3252,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17.100000000000001">
+    <row r="5" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
       <c r="A5" s="12" t="s">
         <v>15</v>
       </c>
@@ -3262,7 +3269,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17.100000000000001">
+    <row r="6" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
       <c r="A6" s="12" t="s">
         <v>20</v>
       </c>
@@ -3279,7 +3286,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
@@ -3309,20 +3316,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.47265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="4" customFormat="1">
+    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
@@ -3339,80 +3346,83 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>20</v>
       </c>
       <c r="E2" s="22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="14.1">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="14.1">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>37</v>
+      <c r="B4" s="37" t="s">
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="14.1">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="14.1">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>10</v>
@@ -3421,32 +3431,32 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="14.1">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="14.1">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>15</v>
@@ -3455,32 +3465,32 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="14.1">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="14.1">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>20</v>
@@ -3489,100 +3499,100 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="14.1">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="D11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="20" t="s">
+      <c r="E13" s="22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>5</v>
-      </c>
       <c r="E14" s="22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="14.1">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E15" s="22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="14.1">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>20</v>
@@ -3594,174 +3604,171 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="14.1">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
         <v>34</v>
       </c>
       <c r="Y17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="14.1">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" ht="14.1">
-      <c r="A19">
-        <v>2</v>
-      </c>
-      <c r="B19" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" t="s">
-        <v>70</v>
-      </c>
-      <c r="D19" s="14" t="s">
+      <c r="E20" s="22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25">
-      <c r="A20">
-        <v>2</v>
-      </c>
-      <c r="B20" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25">
-      <c r="A21">
-        <v>2</v>
-      </c>
-      <c r="B21" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>5</v>
-      </c>
       <c r="E21" s="22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>5</v>
+        <v>87</v>
+      </c>
+      <c r="D22" t="s">
+        <v>20</v>
       </c>
       <c r="E22" s="22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
-      </c>
-      <c r="D23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25">
+        <v>101</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
-      </c>
-      <c r="D24" t="s">
-        <v>5</v>
+        <v>89</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>10</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A25">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
-      </c>
-      <c r="D25" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="C26" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="D26" s="20" t="s">
         <v>10</v>
@@ -3770,41 +3777,41 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>87</v>
-      </c>
-      <c r="D27" t="s">
-        <v>20</v>
+        <v>54</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>5</v>
       </c>
       <c r="E27" s="22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E28" s="22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>3</v>
       </c>
@@ -3821,7 +3828,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>3</v>
       </c>
@@ -3838,117 +3845,117 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="D31" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E31" s="22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25">
+      <c r="E31" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>4</v>
       </c>
-      <c r="B32" t="s">
-        <v>96</v>
+      <c r="B32" s="37" t="s">
+        <v>106</v>
       </c>
       <c r="C32" t="s">
-        <v>97</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>20</v>
+        <v>107</v>
+      </c>
+      <c r="D32" t="s">
+        <v>5</v>
       </c>
       <c r="E32" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="C33" t="s">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E33" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>15</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>101</v>
+        <v>58</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>5</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A35">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="C35" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E35" s="22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="C36" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E36" s="20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>5</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C37" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D37" t="s">
         <v>5</v>
@@ -3957,26 +3964,26 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38">
-        <v>4</v>
-      </c>
-      <c r="B38" t="s">
-        <v>108</v>
+        <v>3</v>
+      </c>
+      <c r="B38" s="37" t="s">
+        <v>82</v>
       </c>
       <c r="C38" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="D38" t="s">
         <v>5</v>
       </c>
-      <c r="E38" t="s">
-        <v>34</v>
+      <c r="E38" s="22" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:E38">
-    <sortCondition ref="A2"/>
+    <sortCondition ref="B38"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="E2:E51">
@@ -4004,49 +4011,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}"/>
+    <sheetView zoomScale="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="2"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.625" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.6171875" style="2"/>
+    <col min="2" max="2" width="9.47265625" customWidth="1"/>
+    <col min="3" max="3" width="15.6171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.37890625" customWidth="1"/>
+    <col min="5" max="5" width="6.6171875" customWidth="1"/>
+    <col min="6" max="6" width="12.47265625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>116</v>
       </c>
@@ -4069,7 +4076,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>123</v>
       </c>
@@ -4085,7 +4092,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>124</v>
       </c>
@@ -4110,7 +4117,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>125</v>
       </c>
@@ -4135,7 +4142,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>126</v>
       </c>
@@ -4160,7 +4167,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>127</v>
       </c>
@@ -4196,21 +4203,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:G8"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
+    <sheetView topLeftCell="A6" zoomScale="150" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="9.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.37890625" style="2" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.37890625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6171875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" s="4" customFormat="1">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>116</v>
       </c>
@@ -4233,7 +4240,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1">
+    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -4248,7 +4255,7 @@
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>124</v>
       </c>
@@ -4274,7 +4281,7 @@
         <v>14.592592592592593</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>125</v>
       </c>
@@ -4300,7 +4307,7 @@
         <v>10.258064516129032</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>126</v>
       </c>
@@ -4326,7 +4333,7 @@
         <v>11.533333333333333</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>127</v>
       </c>
@@ -4364,23 +4371,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
-    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.125" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.625" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.125" style="19" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.37890625" customWidth="1"/>
+    <col min="2" max="2" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.47265625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6171875" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.37890625" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6171875" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.47265625" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.6171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.1">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -4409,7 +4416,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="14.1">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
@@ -4438,7 +4445,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.1">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A3" s="14" t="s">
         <v>37</v>
       </c>
@@ -4470,7 +4477,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.1">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A4" s="14" t="s">
         <v>39</v>
       </c>
@@ -4502,7 +4509,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.1">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A5" s="14" t="s">
         <v>41</v>
       </c>
@@ -4534,7 +4541,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.1">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
@@ -4563,7 +4570,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.1">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A7" s="14" t="s">
         <v>45</v>
       </c>
@@ -4592,7 +4599,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.1">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A8" s="14" t="s">
         <v>47</v>
       </c>
@@ -4621,7 +4628,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.1">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A9" s="14" t="s">
         <v>53</v>
       </c>
@@ -4650,7 +4657,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.1">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B10" s="5" t="s">
         <v>136</v>
       </c>
@@ -4663,20 +4670,20 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.1">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B12" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" ht="14.1">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B14" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B15" s="31" t="s">
         <v>139</v>
       </c>
@@ -4688,7 +4695,7 @@
       <c r="H15" s="31"/>
       <c r="I15" s="31"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B16" s="31" t="s">
         <v>140</v>
       </c>
@@ -4700,7 +4707,7 @@
       <c r="H16" s="31"/>
       <c r="I16" s="31"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B17" s="31" t="s">
         <v>141</v>
       </c>
@@ -4712,7 +4719,7 @@
       <c r="H17" s="31"/>
       <c r="I17" s="31"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B18" s="31" t="s">
         <v>142</v>
       </c>
@@ -4724,7 +4731,7 @@
       <c r="H18" s="31"/>
       <c r="I18" s="31"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B19" s="32" t="s">
         <v>143</v>
       </c>
@@ -4736,12 +4743,12 @@
       <c r="H19" s="32"/>
       <c r="I19" s="32"/>
     </row>
-    <row r="20" spans="1:9" ht="27.95">
+    <row r="20" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B20" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B21" s="31" t="s">
         <v>145</v>
       </c>
@@ -4752,7 +4759,7 @@
       <c r="G21" s="31"/>
       <c r="H21" s="31"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B22" s="31" t="s">
         <v>146</v>
       </c>
@@ -4762,16 +4769,16 @@
       <c r="F22" s="31"/>
       <c r="G22" s="31"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B24" s="5"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="30" t="s">
         <v>147</v>
       </c>
       <c r="B26" s="30"/>
     </row>
-    <row r="27" spans="1:9" ht="14.1">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
@@ -4800,7 +4807,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -4829,7 +4836,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -4858,7 +4865,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="14.1">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" s="14" t="s">
         <v>51</v>
       </c>
@@ -4887,7 +4894,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -4980,23 +4987,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96723CB6-6D85-DA4E-8BFC-88DDD98C4269}">
   <dimension ref="A1:Z27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0" xr3:uid="{BA7E6921-9E23-5D53-A4E4-A351F9C68F3B}"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
-    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.125" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.625" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.125" style="19" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.37890625" customWidth="1"/>
+    <col min="2" max="2" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.47265625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6171875" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.37890625" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6171875" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.47265625" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.6171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.1">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>149</v>
       </c>
@@ -5025,7 +5032,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="14.1">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A2" s="14" t="s">
         <v>59</v>
       </c>
@@ -5054,7 +5061,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.1">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A3" s="14" t="s">
         <v>61</v>
       </c>
@@ -5086,7 +5093,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.1">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A4" s="14" t="s">
         <v>64</v>
       </c>
@@ -5118,7 +5125,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.1">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A5" s="14" t="s">
         <v>67</v>
       </c>
@@ -5150,7 +5157,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.1">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A6" s="14" t="s">
         <v>69</v>
       </c>
@@ -5179,7 +5186,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.1">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A7" s="14" t="s">
         <v>71</v>
       </c>
@@ -5208,7 +5215,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.1">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A8" s="14" t="s">
         <v>73</v>
       </c>
@@ -5237,7 +5244,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.1">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A9" s="14" t="s">
         <v>75</v>
       </c>
@@ -5266,7 +5273,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.1">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B10" s="5" t="s">
         <v>136</v>
       </c>
@@ -5279,20 +5286,20 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.1">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B12" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" ht="14.1">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B14" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="24.95" customHeight="1">
+    <row r="15" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="31" t="s">
         <v>159</v>
       </c>
@@ -5304,7 +5311,7 @@
       <c r="H15" s="31"/>
       <c r="I15" s="31"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B16" s="31" t="s">
         <v>160</v>
       </c>
@@ -5316,7 +5323,7 @@
       <c r="H16" s="31"/>
       <c r="I16" s="31"/>
     </row>
-    <row r="17" spans="2:9">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B17" s="31" t="s">
         <v>161</v>
       </c>
@@ -5328,7 +5335,7 @@
       <c r="H17" s="31"/>
       <c r="I17" s="26"/>
     </row>
-    <row r="18" spans="2:9">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B18" s="31" t="s">
         <v>162</v>
       </c>
@@ -5340,13 +5347,13 @@
       <c r="H18" s="32"/>
       <c r="I18" s="32"/>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B20" s="33" t="s">
         <v>144</v>
       </c>
       <c r="C20" s="33"/>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B21" s="31" t="s">
         <v>163</v>
       </c>
@@ -5357,7 +5364,7 @@
       <c r="G21" s="31"/>
       <c r="H21" s="31"/>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B22" s="27"/>
       <c r="C22" s="27"/>
       <c r="D22" s="27"/>
@@ -5367,7 +5374,7 @@
       <c r="H22" s="27"/>
       <c r="I22" s="27"/>
     </row>
-    <row r="25" spans="2:9">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B25" s="31"/>
       <c r="C25" s="31"/>
       <c r="D25" s="31"/>
@@ -5375,7 +5382,7 @@
       <c r="F25" s="31"/>
       <c r="G25" s="31"/>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B27" s="5"/>
     </row>
   </sheetData>
@@ -5421,23 +5428,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0" xr3:uid="{9B253EF2-77E0-53E3-AE26-4D66ECD923F3}"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
-    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.125" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.625" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.125" style="19" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.37890625" customWidth="1"/>
+    <col min="2" max="2" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.47265625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6171875" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.37890625" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6171875" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.47265625" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.6171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.1">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>149</v>
       </c>
@@ -5466,7 +5473,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="14.1">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A2" s="14" t="s">
         <v>84</v>
       </c>
@@ -5495,7 +5502,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.1">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A3" s="14" t="s">
         <v>88</v>
       </c>
@@ -5527,7 +5534,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.1">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -5559,7 +5566,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.1">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -5591,7 +5598,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.1">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A6" s="14" t="s">
         <v>77</v>
       </c>
@@ -5620,7 +5627,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.1">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
@@ -5649,7 +5656,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.1">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -5678,7 +5685,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.1">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A9" s="14" t="s">
         <v>82</v>
       </c>
@@ -5707,7 +5714,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.1">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B10" s="5" t="s">
         <v>136</v>
       </c>
@@ -5720,21 +5727,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.1">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B12" s="5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" ht="14.1">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A14" s="25"/>
       <c r="B14" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="12.6" customHeight="1">
+    <row r="15" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="31" t="s">
         <v>165</v>
       </c>
@@ -5747,145 +5754,140 @@
       <c r="I15" s="31"/>
       <c r="J15" s="31"/>
     </row>
-    <row r="16" spans="1:26" ht="12.6" customHeight="1">
-      <c r="B16" s="35" t="s">
+    <row r="16" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-    </row>
-    <row r="17" spans="2:12" ht="12.6" customHeight="1">
-      <c r="B17" s="35" t="s">
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+    </row>
+    <row r="17" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="36" t="s">
         <v>167</v>
       </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-    </row>
-    <row r="18" spans="2:12" ht="12.6" customHeight="1">
-      <c r="B18" s="35" t="s">
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+    </row>
+    <row r="18" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-    </row>
-    <row r="19" spans="2:12" ht="12.6" customHeight="1">
-      <c r="B19" s="35" t="s">
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+    </row>
+    <row r="19" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-    </row>
-    <row r="20" spans="2:12" ht="12.6" customHeight="1">
-      <c r="B20" s="34" t="s">
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+    </row>
+    <row r="20" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
-    </row>
-    <row r="21" spans="2:12" ht="12.6" customHeight="1">
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-    </row>
-    <row r="22" spans="2:12" ht="12.95" customHeight="1">
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
+    </row>
+    <row r="21" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+    </row>
+    <row r="22" spans="2:12" ht="13" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B22" s="33" t="s">
         <v>144</v>
       </c>
       <c r="C22" s="33"/>
     </row>
-    <row r="23" spans="2:12" ht="12.6" customHeight="1">
-      <c r="B23" s="35" t="s">
+    <row r="23" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="35"/>
-    </row>
-    <row r="24" spans="2:12">
-      <c r="B24" s="35" t="s">
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B24" s="36" t="s">
         <v>172</v>
       </c>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-    </row>
-    <row r="25" spans="2:12">
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
-    </row>
-    <row r="26" spans="2:12">
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="35"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B26:J26"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="B24:J24"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B15:J15"/>
     <mergeCell ref="B21:J21"/>
     <mergeCell ref="B19:J19"/>
@@ -5893,6 +5895,11 @@
     <mergeCell ref="B17:J17"/>
     <mergeCell ref="B16:J16"/>
     <mergeCell ref="B20:L20"/>
+    <mergeCell ref="B26:J26"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="B24:J24"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I1 I10:I11 I22 D2:D9 I27:I1048576">
@@ -5928,25 +5935,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0" xr3:uid="{85D5C41F-068E-5C55-9968-509E7C2A5619}">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
-    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" style="18" customWidth="1"/>
-    <col min="4" max="4" width="8.125" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.625" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.125" style="19" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.37890625" customWidth="1"/>
+    <col min="2" max="2" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.47265625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6171875" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.37890625" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6171875" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.47265625" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.6171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.1">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A1" s="28" t="s">
         <v>149</v>
       </c>
@@ -5975,7 +5982,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="14.1">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A2" s="14" t="s">
         <v>100</v>
       </c>
@@ -6004,7 +6011,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.1">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>102</v>
       </c>
@@ -6036,7 +6043,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.1">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -6068,7 +6075,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.1">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -6100,7 +6107,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.1">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -6129,7 +6136,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.1">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -6158,7 +6165,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.1">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -6187,7 +6194,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.1">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A9" s="14" t="s">
         <v>108</v>
       </c>
@@ -6216,7 +6223,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.1">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B10" s="5" t="s">
         <v>136</v>
       </c>
@@ -6229,20 +6236,20 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.1">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B12" s="5" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" ht="14.1">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B14" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="12.6" customHeight="1">
+    <row r="15" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="31"/>
       <c r="C15" s="31"/>
       <c r="D15" s="31"/>
@@ -6252,7 +6259,7 @@
       <c r="H15" s="31"/>
       <c r="I15" s="31"/>
     </row>
-    <row r="16" spans="1:26" ht="12.6" customHeight="1">
+    <row r="16" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="31"/>
       <c r="C16" s="31"/>
       <c r="D16" s="31"/>
@@ -6262,7 +6269,7 @@
       <c r="H16" s="31"/>
       <c r="I16" s="31"/>
     </row>
-    <row r="17" spans="2:9" ht="12.6" customHeight="1">
+    <row r="17" spans="2:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="31"/>
       <c r="C17" s="31"/>
       <c r="D17" s="31"/>
@@ -6272,7 +6279,7 @@
       <c r="H17" s="31"/>
       <c r="I17" s="31"/>
     </row>
-    <row r="18" spans="2:9" ht="12.6" customHeight="1">
+    <row r="18" spans="2:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="31"/>
       <c r="C18" s="31"/>
       <c r="D18" s="31"/>
@@ -6282,7 +6289,7 @@
       <c r="H18" s="31"/>
       <c r="I18" s="31"/>
     </row>
-    <row r="19" spans="2:9" ht="12.6" customHeight="1">
+    <row r="19" spans="2:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
@@ -6292,7 +6299,7 @@
       <c r="H19" s="26"/>
       <c r="I19" s="26"/>
     </row>
-    <row r="20" spans="2:9" ht="12.6" customHeight="1">
+    <row r="20" spans="2:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="32"/>
       <c r="C20" s="32"/>
       <c r="D20" s="32"/>
@@ -6302,7 +6309,7 @@
       <c r="H20" s="32"/>
       <c r="I20" s="32"/>
     </row>
-    <row r="21" spans="2:9" ht="12.6" customHeight="1">
+    <row r="21" spans="2:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
       <c r="D21" s="32"/>
@@ -6312,13 +6319,13 @@
       <c r="H21" s="32"/>
       <c r="I21" s="32"/>
     </row>
-    <row r="22" spans="2:9" ht="12.95" customHeight="1">
+    <row r="22" spans="2:9" ht="13" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B22" s="33" t="s">
         <v>144</v>
       </c>
       <c r="C22" s="33"/>
     </row>
-    <row r="23" spans="2:9" ht="12.6" customHeight="1">
+    <row r="23" spans="2:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B23" s="31"/>
       <c r="C23" s="31"/>
       <c r="D23" s="31"/>
@@ -6328,7 +6335,7 @@
       <c r="H23" s="31"/>
       <c r="I23" s="31"/>
     </row>
-    <row r="24" spans="2:9">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B24" s="31"/>
       <c r="C24" s="31"/>
       <c r="D24" s="31"/>
@@ -6336,7 +6343,7 @@
       <c r="F24" s="31"/>
       <c r="G24" s="31"/>
     </row>
-    <row r="26" spans="2:9">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B26" s="5"/>
     </row>
   </sheetData>
@@ -6385,16 +6392,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0" xr3:uid="{44B22561-5205-5C8A-B808-2C70100D228F}"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.625" customWidth="1"/>
-    <col min="3" max="3" width="69.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6171875" customWidth="1"/>
+    <col min="3" max="3" width="69.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="14.1">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>149</v>
       </c>
@@ -6408,7 +6417,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="33.950000000000003">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -6422,7 +6431,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.100000000000001">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -6436,7 +6445,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.100000000000001">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -6450,7 +6459,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="33.950000000000003">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -6464,7 +6473,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17.100000000000001">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -6478,7 +6487,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17.100000000000001">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -6492,7 +6501,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="33.950000000000003">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -6506,7 +6515,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="33.950000000000003">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -6517,7 +6526,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="33.950000000000003">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -6528,7 +6537,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="33.950000000000003">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>64</v>
       </c>
@@ -6539,7 +6548,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17.100000000000001">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>96</v>
       </c>
@@ -6550,7 +6559,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="33.950000000000003">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -6561,7 +6570,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="51">
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -6572,7 +6581,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="17.100000000000001">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -6583,7 +6592,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17.100000000000001">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -6594,7 +6603,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17.100000000000001">
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -6605,7 +6614,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17.100000000000001">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>193</v>
       </c>
@@ -6616,7 +6625,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17.100000000000001">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -6627,7 +6636,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17.100000000000001">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>98</v>
       </c>
@@ -6638,7 +6647,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.100000000000001">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>198</v>
       </c>
@@ -6649,7 +6658,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.100000000000001">
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -6663,7 +6672,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17.100000000000001">
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -6674,7 +6683,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="33.950000000000003">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>86</v>
       </c>
@@ -6685,7 +6694,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="33.950000000000003">
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>100</v>
       </c>
@@ -6696,7 +6705,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="33.950000000000003">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -6710,7 +6719,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="84.95">
+    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>207</v>
       </c>
@@ -6721,7 +6730,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="17.100000000000001">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -6732,7 +6741,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="17.100000000000001">
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>102</v>
       </c>
@@ -6743,7 +6752,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17.100000000000001">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -6757,7 +6766,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17.100000000000001">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -6768,7 +6777,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="33.950000000000003">
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>90</v>
       </c>
@@ -6782,7 +6791,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="17.100000000000001">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>92</v>
       </c>
@@ -6796,7 +6805,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="33.950000000000003">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -6807,7 +6816,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="33.950000000000003">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>106</v>
       </c>
@@ -6818,7 +6827,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17.100000000000001">
+    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -6829,7 +6838,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17.100000000000001">
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -6840,7 +6849,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="33.950000000000003">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>73</v>
       </c>
@@ -6851,7 +6860,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="33.950000000000003">
+    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -6862,7 +6871,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="33.950000000000003">
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>108</v>
       </c>
@@ -6873,7 +6882,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="17.100000000000001">
+    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>223</v>
       </c>
@@ -6884,7 +6893,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="17.100000000000001">
+    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>226</v>
       </c>
@@ -6895,7 +6904,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="33.950000000000003">
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>82</v>
       </c>

</xml_diff>

<commit_message>
user stories with no output highlighted
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\Documents\GitHub\gedcom-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32539DE-7F74-444E-8760-8A5CE919F93E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EDE224-F141-4B8F-A211-08C22E79CCF3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="462" windowWidth="24438" windowHeight="15240" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="179020" concurrentCalc="0"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,6 +31,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -817,7 +818,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -833,6 +834,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -947,7 +954,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1005,6 +1012,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1020,16 +1028,16 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="68">
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
@@ -3290,14 +3298,14 @@
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
     </row>
   </sheetData>
-  <sortState ref="A3:D5">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D5">
     <sortCondition ref="C3:C5"/>
   </sortState>
   <mergeCells count="1">
@@ -3316,8 +3324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -3384,7 +3392,7 @@
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="29" t="s">
         <v>39</v>
       </c>
       <c r="C4" t="s">
@@ -3537,7 +3545,7 @@
       <c r="A13">
         <v>2</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="29" t="s">
         <v>67</v>
       </c>
       <c r="C13" t="s">
@@ -3866,7 +3874,7 @@
       <c r="A32">
         <v>4</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="38" t="s">
         <v>106</v>
       </c>
       <c r="C32" t="s">
@@ -3968,7 +3976,7 @@
       <c r="A38">
         <v>3</v>
       </c>
-      <c r="B38" s="37" t="s">
+      <c r="B38" s="38" t="s">
         <v>82</v>
       </c>
       <c r="C38" t="s">
@@ -3982,7 +3990,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:E38">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E38">
     <sortCondition ref="B38"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4684,64 +4692,64 @@
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
     </row>
     <row r="20" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B20" s="5" t="s">
@@ -4749,34 +4757,34 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B24" s="5"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="B26" s="30"/>
+      <c r="B26" s="31"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
@@ -5300,69 +5308,69 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
       <c r="I17" s="26"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="C20" s="33"/>
+      <c r="C20" s="34"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B22" s="27"/>
@@ -5375,12 +5383,12 @@
       <c r="I22" s="27"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B27" s="5"/>
@@ -5742,17 +5750,17 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
     </row>
     <row r="16" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="36" t="s">
@@ -5833,10 +5841,10 @@
       <c r="J21" s="35"/>
     </row>
     <row r="22" spans="2:12" ht="13" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="C22" s="33"/>
+      <c r="C22" s="34"/>
     </row>
     <row r="23" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B23" s="36" t="s">
@@ -5876,18 +5884,23 @@
       <c r="J25" s="35"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B26:J26"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="B24:J24"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B15:J15"/>
     <mergeCell ref="B21:J21"/>
     <mergeCell ref="B19:J19"/>
@@ -5895,11 +5908,6 @@
     <mergeCell ref="B17:J17"/>
     <mergeCell ref="B16:J16"/>
     <mergeCell ref="B20:L20"/>
-    <mergeCell ref="B26:J26"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="B24:J24"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I1 I10:I11 I22 D2:D9 I27:I1048576">
@@ -6250,44 +6258,44 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
     </row>
     <row r="16" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
     </row>
     <row r="17" spans="2:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
     </row>
     <row r="18" spans="2:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
     </row>
     <row r="19" spans="2:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="26"/>
@@ -6300,48 +6308,48 @@
       <c r="I19" s="26"/>
     </row>
     <row r="20" spans="2:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
     </row>
     <row r="21" spans="2:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
     </row>
     <row r="22" spans="2:9" ht="13" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="C22" s="33"/>
+      <c r="C22" s="34"/>
     </row>
     <row r="23" spans="2:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B26" s="5"/>
@@ -6392,8 +6400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
minor changes to app.py
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\Documents\GitHub\gedcom-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EDE224-F141-4B8F-A211-08C22E79CCF3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E62530-FAA3-4FB3-A6ED-31112F15C6F2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="462" windowWidth="24438" windowHeight="15240" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1013,6 +1013,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1028,16 +1029,15 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="68">
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
@@ -3298,11 +3298,11 @@
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D5">
@@ -3324,8 +3324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -3392,7 +3392,7 @@
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="30" t="s">
         <v>39</v>
       </c>
       <c r="C4" t="s">
@@ -3874,7 +3874,7 @@
       <c r="A32">
         <v>4</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="30" t="s">
         <v>106</v>
       </c>
       <c r="C32" t="s">
@@ -3976,7 +3976,7 @@
       <c r="A38">
         <v>3</v>
       </c>
-      <c r="B38" s="38" t="s">
+      <c r="B38" s="30" t="s">
         <v>82</v>
       </c>
       <c r="C38" t="s">
@@ -4692,64 +4692,64 @@
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
     </row>
     <row r="20" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B20" s="5" t="s">
@@ -4757,34 +4757,34 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B24" s="5"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="B26" s="31"/>
+      <c r="B26" s="32"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
@@ -5308,69 +5308,69 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="33" t="s">
         <v>159</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
       <c r="I17" s="26"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="35" t="s">
         <v>144</v>
       </c>
-      <c r="C20" s="34"/>
+      <c r="C20" s="35"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B22" s="27"/>
@@ -5383,12 +5383,12 @@
       <c r="I22" s="27"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B27" s="5"/>
@@ -5750,157 +5750,152 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="33" t="s">
         <v>165</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
     </row>
     <row r="16" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
     </row>
     <row r="17" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
     </row>
     <row r="18" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
     </row>
     <row r="19" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
     </row>
     <row r="20" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="35"/>
-      <c r="L20" s="35"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
     </row>
     <row r="21" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
     </row>
     <row r="22" spans="2:12" ht="13" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="35" t="s">
         <v>144</v>
       </c>
-      <c r="C22" s="34"/>
+      <c r="C22" s="35"/>
     </row>
     <row r="23" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B26:J26"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="B24:J24"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B15:J15"/>
     <mergeCell ref="B21:J21"/>
     <mergeCell ref="B19:J19"/>
@@ -5908,6 +5903,11 @@
     <mergeCell ref="B17:J17"/>
     <mergeCell ref="B16:J16"/>
     <mergeCell ref="B20:L20"/>
+    <mergeCell ref="B26:J26"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="B24:J24"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I1 I10:I11 I22 D2:D9 I27:I1048576">
@@ -6258,44 +6258,44 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
     </row>
     <row r="16" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
     </row>
     <row r="17" spans="2:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
     </row>
     <row r="18" spans="2:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
     </row>
     <row r="19" spans="2:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="26"/>
@@ -6308,48 +6308,48 @@
       <c r="I19" s="26"/>
     </row>
     <row r="20" spans="2:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
     </row>
     <row r="21" spans="2:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
     </row>
     <row r="22" spans="2:9" ht="13" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="35" t="s">
         <v>144</v>
       </c>
-      <c r="C22" s="34"/>
+      <c r="C22" s="35"/>
     </row>
     <row r="23" spans="2:9" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B26" s="5"/>

</xml_diff>

<commit_message>
updated My_Family.ged file to force demonstration of US12
</commit_message>
<xml_diff>
--- a/TeamReport.xlsx
+++ b/TeamReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11014"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\Documents\GitHub\gedcom-parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rozanitis/Documents/Stevens/Semesters/Fall2018/SSW-555/gedcom-parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE82B9B6-7429-4D82-90B6-89FAD6269EAD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A167E127-351E-3B49-9356-D77003D6B91D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="462" windowWidth="24438" windowHeight="15240" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24440" windowHeight="15240" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -28,18 +28,12 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="236">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -751,13 +745,22 @@
     <t>All dates should be legitimate dates for the months specified (e.g., 2/30/2015 is not legitimate)</t>
   </si>
   <si>
-    <t>1. Coordination between all the team memebers were great.</t>
-  </si>
-  <si>
-    <t>2. Use of whatsapp has been good platform to share daily thought for standups.</t>
-  </si>
-  <si>
     <t>1. Change code or merge branch without informing other team mates</t>
+  </si>
+  <si>
+    <t>1. Coordination between all the team memebers were great</t>
+  </si>
+  <si>
+    <t>2. WhatsApp has been good platform to share daily thought for standups</t>
+  </si>
+  <si>
+    <t>3. Creating separate branches for each user story so no one is merging to master branch directly</t>
+  </si>
+  <si>
+    <t>4. Adding TravisCI to the GitHub repository before the project starts</t>
+  </si>
+  <si>
+    <t>5. Completing user stories 3-4 days before the sprint deadline to ensure all user stories will be completed on-time</t>
   </si>
 </sst>
 </file>
@@ -1038,13 +1041,13 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1439,7 +1442,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1510,7 +1513,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3210,15 +3213,15 @@
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.6171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.47265625" customWidth="1"/>
-    <col min="3" max="3" width="8.47265625" customWidth="1"/>
-    <col min="4" max="5" width="20.47265625" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3235,7 +3238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>5</v>
       </c>
@@ -3252,7 +3255,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>10</v>
       </c>
@@ -3269,7 +3272,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>15</v>
       </c>
@@ -3286,7 +3289,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.9" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>20</v>
       </c>
@@ -3303,7 +3306,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
@@ -3314,7 +3317,7 @@
       <c r="G9" s="31"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D5">
+  <sortState ref="A3:D5">
     <sortCondition ref="C3:C5"/>
   </sortState>
   <mergeCells count="1">
@@ -3337,16 +3340,16 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.47265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
@@ -3363,7 +3366,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3380,7 +3383,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3397,7 +3400,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3414,7 +3417,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3431,7 +3434,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3448,7 +3451,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3465,7 +3468,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3482,7 +3485,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>2</v>
       </c>
@@ -3499,7 +3502,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>2</v>
       </c>
@@ -3516,7 +3519,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>2</v>
       </c>
@@ -3533,7 +3536,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>4</v>
       </c>
@@ -3550,7 +3553,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2</v>
       </c>
@@ -3567,7 +3570,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>4</v>
       </c>
@@ -3584,7 +3587,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2</v>
       </c>
@@ -3601,7 +3604,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>1</v>
       </c>
@@ -3621,7 +3624,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>3</v>
       </c>
@@ -3641,7 +3644,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>3</v>
       </c>
@@ -3661,7 +3664,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>4</v>
       </c>
@@ -3678,7 +3681,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>3</v>
       </c>
@@ -3695,7 +3698,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>1</v>
       </c>
@@ -3712,7 +3715,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>3</v>
       </c>
@@ -3729,7 +3732,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>4</v>
       </c>
@@ -3746,7 +3749,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>3</v>
       </c>
@@ -3763,7 +3766,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>0</v>
       </c>
@@ -3777,7 +3780,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>4</v>
       </c>
@@ -3794,7 +3797,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>1</v>
       </c>
@@ -3811,7 +3814,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>2</v>
       </c>
@@ -3828,7 +3831,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>3</v>
       </c>
@@ -3845,7 +3848,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>3</v>
       </c>
@@ -3862,7 +3865,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>4</v>
       </c>
@@ -3879,7 +3882,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>4</v>
       </c>
@@ -3896,7 +3899,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>1</v>
       </c>
@@ -3913,7 +3916,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>1</v>
       </c>
@@ -3930,7 +3933,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>2</v>
       </c>
@@ -3947,7 +3950,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>2</v>
       </c>
@@ -3964,7 +3967,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>4</v>
       </c>
@@ -3981,7 +3984,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>3</v>
       </c>
@@ -3999,7 +4002,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E38">
+  <sortState ref="A2:E38">
     <sortCondition ref="B38"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4030,47 +4033,47 @@
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.6171875" style="2"/>
-    <col min="2" max="2" width="9.47265625" customWidth="1"/>
-    <col min="3" max="3" width="15.6171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.37890625" customWidth="1"/>
-    <col min="5" max="5" width="6.6171875" customWidth="1"/>
-    <col min="6" max="6" width="12.47265625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="2"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>116</v>
       </c>
@@ -4093,7 +4096,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>123</v>
       </c>
@@ -4109,7 +4112,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>124</v>
       </c>
@@ -4134,7 +4137,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>125</v>
       </c>
@@ -4159,7 +4162,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>126</v>
       </c>
@@ -4184,7 +4187,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>127</v>
       </c>
@@ -4224,17 +4227,17 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="9.37890625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.37890625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6171875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>116</v>
       </c>
@@ -4257,7 +4260,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -4272,7 +4275,7 @@
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>124</v>
       </c>
@@ -4298,7 +4301,7 @@
         <v>14.592592592592593</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>125</v>
       </c>
@@ -4324,7 +4327,7 @@
         <v>10.258064516129032</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>126</v>
       </c>
@@ -4350,7 +4353,7 @@
         <v>11.533333333333333</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>127</v>
       </c>
@@ -4390,21 +4393,21 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.37890625" customWidth="1"/>
-    <col min="2" max="2" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.47265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6171875" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.37890625" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6171875" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.6171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -4433,7 +4436,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
@@ -4462,7 +4465,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
         <v>37</v>
       </c>
@@ -4494,7 +4497,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
         <v>39</v>
       </c>
@@ -4526,7 +4529,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
         <v>41</v>
       </c>
@@ -4558,7 +4561,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
@@ -4587,7 +4590,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
         <v>45</v>
       </c>
@@ -4616,7 +4619,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="14" t="s">
         <v>47</v>
       </c>
@@ -4645,7 +4648,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>53</v>
       </c>
@@ -4674,7 +4677,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>136</v>
       </c>
@@ -4687,20 +4690,20 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B15" s="33" t="s">
         <v>139</v>
       </c>
@@ -4712,7 +4715,7 @@
       <c r="H15" s="33"/>
       <c r="I15" s="33"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B16" s="33" t="s">
         <v>140</v>
       </c>
@@ -4724,7 +4727,7 @@
       <c r="H16" s="33"/>
       <c r="I16" s="33"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B17" s="33" t="s">
         <v>141</v>
       </c>
@@ -4736,7 +4739,7 @@
       <c r="H17" s="33"/>
       <c r="I17" s="33"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B18" s="33" t="s">
         <v>142</v>
       </c>
@@ -4748,7 +4751,7 @@
       <c r="H18" s="33"/>
       <c r="I18" s="33"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B19" s="34" t="s">
         <v>143</v>
       </c>
@@ -4760,12 +4763,12 @@
       <c r="H19" s="34"/>
       <c r="I19" s="34"/>
     </row>
-    <row r="20" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="B20" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B21" s="33" t="s">
         <v>145</v>
       </c>
@@ -4776,7 +4779,7 @@
       <c r="G21" s="33"/>
       <c r="H21" s="33"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B22" s="33" t="s">
         <v>146</v>
       </c>
@@ -4786,16 +4789,16 @@
       <c r="F22" s="33"/>
       <c r="G22" s="33"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B24" s="5"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="32" t="s">
         <v>147</v>
       </c>
       <c r="B26" s="32"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
@@ -4824,7 +4827,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -4853,7 +4856,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -4882,7 +4885,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="14" t="s">
         <v>51</v>
       </c>
@@ -4911,7 +4914,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -5006,21 +5009,21 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.37890625" customWidth="1"/>
-    <col min="2" max="2" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.47265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6171875" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.37890625" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6171875" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.6171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>149</v>
       </c>
@@ -5049,7 +5052,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
         <v>59</v>
       </c>
@@ -5078,7 +5081,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
         <v>61</v>
       </c>
@@ -5110,7 +5113,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
         <v>64</v>
       </c>
@@ -5142,7 +5145,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
         <v>67</v>
       </c>
@@ -5174,7 +5177,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="14" t="s">
         <v>69</v>
       </c>
@@ -5203,7 +5206,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
         <v>71</v>
       </c>
@@ -5232,7 +5235,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="14" t="s">
         <v>73</v>
       </c>
@@ -5261,7 +5264,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>75</v>
       </c>
@@ -5290,7 +5293,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>136</v>
       </c>
@@ -5303,20 +5306,20 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="33" t="s">
         <v>159</v>
       </c>
@@ -5328,7 +5331,7 @@
       <c r="H15" s="33"/>
       <c r="I15" s="33"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B16" s="33" t="s">
         <v>160</v>
       </c>
@@ -5340,7 +5343,7 @@
       <c r="H16" s="33"/>
       <c r="I16" s="33"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B17" s="33" t="s">
         <v>161</v>
       </c>
@@ -5352,7 +5355,7 @@
       <c r="H17" s="33"/>
       <c r="I17" s="26"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B18" s="33" t="s">
         <v>162</v>
       </c>
@@ -5364,13 +5367,13 @@
       <c r="H18" s="34"/>
       <c r="I18" s="34"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B20" s="35" t="s">
         <v>144</v>
       </c>
       <c r="C20" s="35"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B21" s="33" t="s">
         <v>163</v>
       </c>
@@ -5381,7 +5384,7 @@
       <c r="G21" s="33"/>
       <c r="H21" s="33"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B22" s="27"/>
       <c r="C22" s="27"/>
       <c r="D22" s="27"/>
@@ -5391,7 +5394,7 @@
       <c r="H22" s="27"/>
       <c r="I22" s="27"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B25" s="33"/>
       <c r="C25" s="33"/>
       <c r="D25" s="33"/>
@@ -5399,7 +5402,7 @@
       <c r="F25" s="33"/>
       <c r="G25" s="33"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B27" s="5"/>
     </row>
   </sheetData>
@@ -5445,25 +5448,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:J24"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.37890625" customWidth="1"/>
-    <col min="2" max="2" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.47265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6171875" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.37890625" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6171875" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.6171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>149</v>
       </c>
@@ -5492,7 +5493,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
         <v>84</v>
       </c>
@@ -5521,7 +5522,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
         <v>88</v>
       </c>
@@ -5553,7 +5554,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -5585,7 +5586,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -5617,7 +5618,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="14" t="s">
         <v>77</v>
       </c>
@@ -5646,7 +5647,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
@@ -5675,7 +5676,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -5704,7 +5705,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>82</v>
       </c>
@@ -5733,7 +5734,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>136</v>
       </c>
@@ -5746,21 +5747,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="25"/>
       <c r="B14" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="33" t="s">
         <v>165</v>
       </c>
@@ -5773,145 +5774,140 @@
       <c r="I15" s="33"/>
       <c r="J15" s="33"/>
     </row>
-    <row r="16" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="37" t="s">
+    <row r="16" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-    </row>
-    <row r="17" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="37" t="s">
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+    </row>
+    <row r="17" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-    </row>
-    <row r="18" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="37" t="s">
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+    </row>
+    <row r="18" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-    </row>
-    <row r="19" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="37" t="s">
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+    </row>
+    <row r="19" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-    </row>
-    <row r="20" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="36" t="s">
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+    </row>
+    <row r="20" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-    </row>
-    <row r="21" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
-    </row>
-    <row r="22" spans="2:12" ht="13" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+    </row>
+    <row r="21" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+    </row>
+    <row r="22" spans="2:12" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="35" t="s">
         <v>144</v>
       </c>
       <c r="C22" s="35"/>
     </row>
-    <row r="23" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="37" t="s">
+    <row r="23" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B24" s="37" t="s">
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B24" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="38"/>
-      <c r="J26" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B26:J26"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="B24:J24"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B15:J15"/>
     <mergeCell ref="B21:J21"/>
     <mergeCell ref="B19:J19"/>
@@ -5919,6 +5915,11 @@
     <mergeCell ref="B17:J17"/>
     <mergeCell ref="B16:J16"/>
     <mergeCell ref="B20:L20"/>
+    <mergeCell ref="B26:J26"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="B24:J24"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I1 I10:I11 I22 D2:D9 I27:I1048576">
@@ -5954,25 +5955,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.37890625" customWidth="1"/>
-    <col min="2" max="2" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.47265625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6171875" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.37890625" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6171875" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.6171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="18" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="28" t="s">
         <v>149</v>
       </c>
@@ -6001,7 +6000,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
         <v>100</v>
       </c>
@@ -6030,7 +6029,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>102</v>
       </c>
@@ -6062,7 +6061,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -6094,7 +6093,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -6126,7 +6125,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -6155,7 +6154,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -6184,7 +6183,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -6213,7 +6212,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>108</v>
       </c>
@@ -6242,7 +6241,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
         <v>136</v>
       </c>
@@ -6255,22 +6254,22 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="33" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C15" s="33"/>
       <c r="D15" s="33"/>
@@ -6281,66 +6280,72 @@
       <c r="I15" s="33"/>
       <c r="J15" s="33"/>
     </row>
-    <row r="16" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="37" t="s">
-        <v>231</v>
-      </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-    </row>
-    <row r="17" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-    </row>
-    <row r="18" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-    </row>
-    <row r="19" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-    </row>
-    <row r="20" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-    </row>
-    <row r="21" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+    </row>
+    <row r="17" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="38" t="s">
+        <v>233</v>
+      </c>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+    </row>
+    <row r="18" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="38" t="s">
+        <v>234</v>
+      </c>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+    </row>
+    <row r="19" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+    </row>
+    <row r="20" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+    </row>
+    <row r="21" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="34"/>
       <c r="C21" s="34"/>
       <c r="D21" s="34"/>
@@ -6350,37 +6355,37 @@
       <c r="H21" s="34"/>
       <c r="I21" s="34"/>
     </row>
-    <row r="22" spans="2:12" ht="13" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:12" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="35" t="s">
         <v>144</v>
       </c>
       <c r="C22" s="35"/>
     </row>
-    <row r="23" spans="2:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="37" t="s">
-        <v>232</v>
-      </c>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B26" s="5"/>
     </row>
   </sheetData>
@@ -6430,18 +6435,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6171875" customWidth="1"/>
-    <col min="3" max="3" width="69.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="69.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>149</v>
       </c>
@@ -6455,7 +6460,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -6469,7 +6474,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -6483,7 +6488,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -6497,7 +6502,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -6511,7 +6516,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -6525,7 +6530,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -6539,7 +6544,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -6553,7 +6558,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -6564,7 +6569,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -6575,7 +6580,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>64</v>
       </c>
@@ -6586,7 +6591,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>96</v>
       </c>
@@ -6597,7 +6602,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -6608,7 +6613,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -6619,7 +6624,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -6630,7 +6635,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -6641,7 +6646,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -6652,7 +6657,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>193</v>
       </c>
@@ -6663,7 +6668,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -6674,7 +6679,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>98</v>
       </c>
@@ -6685,7 +6690,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>198</v>
       </c>
@@ -6696,7 +6701,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -6710,7 +6715,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -6721,7 +6726,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>86</v>
       </c>
@@ -6732,7 +6737,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>100</v>
       </c>
@@ -6743,7 +6748,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -6757,7 +6762,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="85" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>207</v>
       </c>
@@ -6768,7 +6773,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -6779,7 +6784,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>102</v>
       </c>
@@ -6790,7 +6795,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -6804,7 +6809,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -6815,7 +6820,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>90</v>
       </c>
@@ -6829,7 +6834,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>92</v>
       </c>
@@ -6843,7 +6848,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -6854,7 +6859,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>106</v>
       </c>
@@ -6865,7 +6870,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -6876,7 +6881,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -6887,7 +6892,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>73</v>
       </c>
@@ -6898,7 +6903,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -6909,7 +6914,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>108</v>
       </c>
@@ -6920,7 +6925,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>223</v>
       </c>
@@ -6931,7 +6936,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>226</v>
       </c>
@@ -6942,7 +6947,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>82</v>
       </c>

</xml_diff>